<commit_message>
adding problem 4 data to ttsp spreadsheet
</commit_message>
<xml_diff>
--- a/doc/ttsp2013/data/problem_4/problem_4_preconditioning.xlsx
+++ b/doc/ttsp2013/data/problem_4/problem_4_preconditioning.xlsx
@@ -4,12 +4,12 @@
   <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="24816"/>
   <workbookPr showInkAnnotation="0" autoCompressPictures="0"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="28800" windowHeight="17480" tabRatio="500"/>
+    <workbookView xWindow="52860" yWindow="4740" windowWidth="51200" windowHeight="28280" tabRatio="500"/>
   </bookViews>
   <sheets>
     <sheet name="Results" sheetId="1" r:id="rId1"/>
     <sheet name="Jacobi" sheetId="5" r:id="rId2"/>
-    <sheet name="SPAINV" sheetId="6" r:id="rId3"/>
+    <sheet name="Case 1 Pstudy" sheetId="6" r:id="rId3"/>
   </sheets>
   <calcPr calcId="140000" concurrentCalc="0"/>
   <extLst>
@@ -21,7 +21,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="66" uniqueCount="33">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="96" uniqueCount="69">
   <si>
     <t>MCSA Preconditioning Analysis</t>
   </si>
@@ -92,9 +92,6 @@
     <t>ARNOLDI-BELOS-GMRES-MGE</t>
   </si>
   <si>
-    <t>ARNOLDI-MCLS-MCSA-JACOBI</t>
-  </si>
-  <si>
     <t>Histories per Iteration</t>
   </si>
   <si>
@@ -120,13 +117,124 @@
   </si>
   <si>
     <t>Total MCSA Iterations</t>
+  </si>
+  <si>
+    <t>Parameter Studies for Sparse Approximate Inverse Preconditioning</t>
+  </si>
+  <si>
+    <t>Threshold</t>
+  </si>
+  <si>
+    <t>Levels</t>
+  </si>
+  <si>
+    <t>DOFs = 717,876</t>
+  </si>
+  <si>
+    <t>1 Iters</t>
+  </si>
+  <si>
+    <t>1 time</t>
+  </si>
+  <si>
+    <t>2 Iters</t>
+  </si>
+  <si>
+    <t>2 time</t>
+  </si>
+  <si>
+    <t>3 Iters</t>
+  </si>
+  <si>
+    <t>3 time</t>
+  </si>
+  <si>
+    <t>4 Iters</t>
+  </si>
+  <si>
+    <t>4 time</t>
+  </si>
+  <si>
+    <t>5 Iters</t>
+  </si>
+  <si>
+    <t>5 time</t>
+  </si>
+  <si>
+    <t>6 Iters</t>
+  </si>
+  <si>
+    <t>6 time</t>
+  </si>
+  <si>
+    <t>7 Iters</t>
+  </si>
+  <si>
+    <t>7 time</t>
+  </si>
+  <si>
+    <t>8 Iters</t>
+  </si>
+  <si>
+    <t>8 time</t>
+  </si>
+  <si>
+    <t>9 Iters</t>
+  </si>
+  <si>
+    <t>9 time</t>
+  </si>
+  <si>
+    <t>10 Iters</t>
+  </si>
+  <si>
+    <t>10 time</t>
+  </si>
+  <si>
+    <t>11 Iters</t>
+  </si>
+  <si>
+    <t>11 time</t>
+  </si>
+  <si>
+    <t>12 Iters</t>
+  </si>
+  <si>
+    <t>12 time</t>
+  </si>
+  <si>
+    <t>13 Iters</t>
+  </si>
+  <si>
+    <t>13 time</t>
+  </si>
+  <si>
+    <t>Total Iters</t>
+  </si>
+  <si>
+    <t>Total Time</t>
+  </si>
+  <si>
+    <t>Solve Time</t>
+  </si>
+  <si>
+    <t>Prec Time</t>
+  </si>
+  <si>
+    <t># Matvecs</t>
+  </si>
+  <si>
+    <t>Richardson FP</t>
+  </si>
+  <si>
+    <t>Total MCSA Iters</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <fonts count="7" x14ac:knownFonts="1">
+  <fonts count="8" x14ac:knownFonts="1">
     <font>
       <sz val="12"/>
       <color theme="1"/>
@@ -181,6 +289,13 @@
       <family val="2"/>
       <scheme val="minor"/>
     </font>
+    <font>
+      <sz val="12"/>
+      <color rgb="FFFF0000"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
   </fonts>
   <fills count="2">
     <fill>
@@ -199,7 +314,7 @@
       <diagonal/>
     </border>
   </borders>
-  <cellStyleXfs count="33">
+  <cellStyleXfs count="159">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="5" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
@@ -233,8 +348,134 @@
     <xf numFmtId="0" fontId="5" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="5" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="7">
+  <cellXfs count="13">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1"/>
@@ -246,8 +487,14 @@
     <xf numFmtId="0" fontId="6" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="3" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
+    <xf numFmtId="2" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="3" fontId="7" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
+    <xf numFmtId="2" fontId="7" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
   </cellXfs>
-  <cellStyles count="33">
+  <cellStyles count="159">
     <cellStyle name="Followed Hyperlink" xfId="2" builtinId="9" hidden="1"/>
     <cellStyle name="Followed Hyperlink" xfId="4" builtinId="9" hidden="1"/>
     <cellStyle name="Followed Hyperlink" xfId="6" builtinId="9" hidden="1"/>
@@ -264,6 +511,69 @@
     <cellStyle name="Followed Hyperlink" xfId="28" builtinId="9" hidden="1"/>
     <cellStyle name="Followed Hyperlink" xfId="30" builtinId="9" hidden="1"/>
     <cellStyle name="Followed Hyperlink" xfId="32" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="34" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="36" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="38" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="40" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="42" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="44" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="46" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="48" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="50" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="52" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="54" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="56" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="58" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="60" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="62" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="64" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="66" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="68" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="70" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="72" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="74" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="76" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="78" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="80" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="82" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="84" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="86" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="88" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="90" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="92" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="94" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="96" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="98" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="100" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="102" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="104" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="106" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="108" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="110" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="112" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="114" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="116" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="118" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="120" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="122" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="124" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="126" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="128" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="130" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="132" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="134" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="136" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="138" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="140" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="142" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="144" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="146" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="148" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="150" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="152" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="154" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="156" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="158" builtinId="9" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="1" builtinId="8" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="3" builtinId="8" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="5" builtinId="8" hidden="1"/>
@@ -280,6 +590,69 @@
     <cellStyle name="Hyperlink" xfId="27" builtinId="8" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="29" builtinId="8" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="31" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="33" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="35" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="37" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="39" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="41" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="43" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="45" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="47" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="49" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="51" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="53" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="55" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="57" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="59" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="61" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="63" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="65" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="67" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="69" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="71" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="73" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="75" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="77" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="79" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="81" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="83" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="85" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="87" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="89" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="91" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="93" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="95" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="97" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="99" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="101" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="103" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="105" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="107" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="109" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="111" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="113" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="115" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="117" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="119" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="121" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="123" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="125" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="127" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="129" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="131" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="133" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="135" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="137" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="139" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="141" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="143" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="145" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="147" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="149" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="151" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="153" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="155" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="157" builtinId="8" hidden="1"/>
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="0"/>
@@ -609,10 +982,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:L58"/>
+  <dimension ref="A1:L49"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="I7" sqref="I7"/>
+      <selection activeCell="P13" sqref="P13"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0"/>
@@ -623,7 +996,7 @@
     <col min="4" max="4" width="11.5" bestFit="1" customWidth="1"/>
     <col min="5" max="5" width="13.33203125" bestFit="1" customWidth="1"/>
     <col min="6" max="6" width="12.83203125" bestFit="1" customWidth="1"/>
-    <col min="7" max="7" width="12.5" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="9.6640625" bestFit="1" customWidth="1"/>
     <col min="8" max="8" width="19.5" bestFit="1" customWidth="1"/>
     <col min="9" max="9" width="10.33203125" bestFit="1" customWidth="1"/>
     <col min="12" max="12" width="13.6640625" bestFit="1" customWidth="1"/>
@@ -676,10 +1049,10 @@
         <v>10</v>
       </c>
       <c r="K6" s="1" t="s">
+        <v>24</v>
+      </c>
+      <c r="L6" s="1" t="s">
         <v>25</v>
-      </c>
-      <c r="L6" s="1" t="s">
-        <v>26</v>
       </c>
     </row>
     <row r="7" spans="1:12">
@@ -700,7 +1073,7 @@
         <v>23</v>
       </c>
       <c r="F7">
-        <v>3</v>
+        <v>1</v>
       </c>
       <c r="G7">
         <v>1</v>
@@ -709,19 +1082,19 @@
         <v>1</v>
       </c>
       <c r="I7" s="4">
-        <f>B7*C7*D7*D7*E7*H7*(F7+1)/2</f>
-        <v>478584</v>
+        <f>B7*C7*D7*D7*E7*(H7+2)*(F7+1)/2</f>
+        <v>717876</v>
       </c>
       <c r="J7">
-        <v>16</v>
+        <f>K7*16</f>
+        <v>32</v>
       </c>
       <c r="K7">
-        <f>J7/16</f>
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="L7" s="4">
         <f>I7/J7</f>
-        <v>29911.5</v>
+        <v>22433.625</v>
       </c>
     </row>
     <row r="8" spans="1:12">
@@ -742,7 +1115,7 @@
         <v>23</v>
       </c>
       <c r="F8">
-        <v>3</v>
+        <v>1</v>
       </c>
       <c r="G8">
         <v>1</v>
@@ -751,19 +1124,19 @@
         <v>5</v>
       </c>
       <c r="I8" s="4">
-        <f>B8*C8*D8*D8*E8*H8*(F8+1)/2</f>
-        <v>2392920</v>
+        <f t="shared" ref="I8:I12" si="0">B8*C8*D8*D8*E8*(H8+2)*(F8+1)/2</f>
+        <v>1675044</v>
       </c>
       <c r="J8">
-        <v>96</v>
+        <f t="shared" ref="J8:J12" si="1">K8*16</f>
+        <v>64</v>
       </c>
       <c r="K8">
-        <f t="shared" ref="K8:K12" si="0">J8/16</f>
-        <v>6</v>
+        <v>4</v>
       </c>
       <c r="L8" s="4">
-        <f t="shared" ref="L8:L12" si="1">I8/J8</f>
-        <v>24926.25</v>
+        <f t="shared" ref="L8:L12" si="2">I8/J8</f>
+        <v>26172.5625</v>
       </c>
     </row>
     <row r="9" spans="1:12">
@@ -771,7 +1144,7 @@
         <v>3</v>
       </c>
       <c r="B9">
-        <f t="shared" ref="B9:B12" si="2">17*17</f>
+        <f t="shared" ref="B9:B12" si="3">17*17</f>
         <v>289</v>
       </c>
       <c r="C9">
@@ -784,7 +1157,7 @@
         <v>23</v>
       </c>
       <c r="F9">
-        <v>3</v>
+        <v>1</v>
       </c>
       <c r="G9">
         <v>1</v>
@@ -793,19 +1166,19 @@
         <v>10</v>
       </c>
       <c r="I9" s="4">
-        <f t="shared" ref="I9:I12" si="3">B9*C9*D9*D9*E9*H9*(F9+1)/2</f>
-        <v>4785840</v>
+        <f t="shared" si="0"/>
+        <v>2871504</v>
       </c>
       <c r="J9">
-        <v>192</v>
+        <f t="shared" si="1"/>
+        <v>128</v>
       </c>
       <c r="K9">
-        <f t="shared" si="0"/>
-        <v>12</v>
+        <v>8</v>
       </c>
       <c r="L9" s="4">
-        <f t="shared" si="1"/>
-        <v>24926.25</v>
+        <f t="shared" si="2"/>
+        <v>22433.625</v>
       </c>
     </row>
     <row r="10" spans="1:12">
@@ -813,7 +1186,7 @@
         <v>4</v>
       </c>
       <c r="B10">
-        <f t="shared" si="2"/>
+        <f t="shared" si="3"/>
         <v>289</v>
       </c>
       <c r="C10">
@@ -826,7 +1199,7 @@
         <v>23</v>
       </c>
       <c r="F10">
-        <v>3</v>
+        <v>1</v>
       </c>
       <c r="G10">
         <v>1</v>
@@ -835,19 +1208,19 @@
         <v>25</v>
       </c>
       <c r="I10" s="4">
-        <f t="shared" si="3"/>
-        <v>11964600</v>
+        <f t="shared" si="0"/>
+        <v>6460884</v>
       </c>
       <c r="J10">
-        <v>480</v>
+        <f t="shared" si="1"/>
+        <v>256</v>
       </c>
       <c r="K10">
-        <f t="shared" si="0"/>
-        <v>30</v>
+        <v>16</v>
       </c>
       <c r="L10" s="4">
-        <f t="shared" si="1"/>
-        <v>24926.25</v>
+        <f t="shared" si="2"/>
+        <v>25237.828125</v>
       </c>
     </row>
     <row r="11" spans="1:12">
@@ -855,7 +1228,7 @@
         <v>5</v>
       </c>
       <c r="B11">
-        <f t="shared" si="2"/>
+        <f t="shared" si="3"/>
         <v>289</v>
       </c>
       <c r="C11">
@@ -868,7 +1241,7 @@
         <v>23</v>
       </c>
       <c r="F11">
-        <v>3</v>
+        <v>1</v>
       </c>
       <c r="G11">
         <v>1</v>
@@ -877,19 +1250,19 @@
         <v>50</v>
       </c>
       <c r="I11" s="4">
-        <f t="shared" si="3"/>
-        <v>23929200</v>
+        <f t="shared" si="0"/>
+        <v>12443184</v>
       </c>
       <c r="J11">
-        <v>960</v>
+        <f t="shared" si="1"/>
+        <v>496</v>
       </c>
       <c r="K11">
-        <f t="shared" si="0"/>
-        <v>60</v>
+        <v>31</v>
       </c>
       <c r="L11" s="4">
-        <f t="shared" si="1"/>
-        <v>24926.25</v>
+        <f t="shared" si="2"/>
+        <v>25087.064516129034</v>
       </c>
     </row>
     <row r="12" spans="1:12">
@@ -897,7 +1270,7 @@
         <v>6</v>
       </c>
       <c r="B12">
-        <f t="shared" si="2"/>
+        <f t="shared" si="3"/>
         <v>289</v>
       </c>
       <c r="C12">
@@ -910,7 +1283,7 @@
         <v>23</v>
       </c>
       <c r="F12">
-        <v>3</v>
+        <v>1</v>
       </c>
       <c r="G12">
         <v>1</v>
@@ -919,19 +1292,19 @@
         <v>100</v>
       </c>
       <c r="I12" s="4">
-        <f t="shared" si="3"/>
-        <v>47858400</v>
+        <f t="shared" si="0"/>
+        <v>24407784</v>
       </c>
       <c r="J12">
-        <v>1920</v>
+        <f t="shared" si="1"/>
+        <v>976</v>
       </c>
       <c r="K12">
-        <f t="shared" si="0"/>
-        <v>120</v>
+        <v>61</v>
       </c>
       <c r="L12" s="4">
-        <f t="shared" si="1"/>
-        <v>24926.25</v>
+        <f t="shared" si="2"/>
+        <v>25007.975409836065</v>
       </c>
     </row>
     <row r="15" spans="1:12">
@@ -953,13 +1326,13 @@
         <v>15</v>
       </c>
       <c r="E16" s="1" t="s">
-        <v>18</v>
+        <v>19</v>
       </c>
       <c r="F16" s="1" t="s">
-        <v>19</v>
+        <v>20</v>
       </c>
       <c r="G16" s="1" t="s">
-        <v>20</v>
+        <v>66</v>
       </c>
     </row>
     <row r="17" spans="1:7">
@@ -1011,13 +1384,13 @@
         <v>15</v>
       </c>
       <c r="E25" s="1" t="s">
-        <v>18</v>
+        <v>19</v>
       </c>
       <c r="F25" s="1" t="s">
-        <v>19</v>
+        <v>20</v>
       </c>
       <c r="G25" s="1" t="s">
-        <v>20</v>
+        <v>66</v>
       </c>
     </row>
     <row r="26" spans="1:7">
@@ -1069,13 +1442,13 @@
         <v>15</v>
       </c>
       <c r="E34" s="1" t="s">
-        <v>18</v>
+        <v>19</v>
       </c>
       <c r="F34" s="1" t="s">
-        <v>19</v>
+        <v>20</v>
       </c>
       <c r="G34" s="1" t="s">
-        <v>20</v>
+        <v>66</v>
       </c>
     </row>
     <row r="35" spans="1:8">
@@ -1110,7 +1483,7 @@
     </row>
     <row r="42" spans="1:8">
       <c r="A42" s="3" t="s">
-        <v>23</v>
+        <v>26</v>
       </c>
     </row>
     <row r="43" spans="1:8">
@@ -1118,7 +1491,7 @@
         <v>11</v>
       </c>
       <c r="B43" s="1" t="s">
-        <v>17</v>
+        <v>68</v>
       </c>
       <c r="C43" s="1" t="s">
         <v>14</v>
@@ -1127,107 +1500,64 @@
         <v>15</v>
       </c>
       <c r="E43" s="1" t="s">
-        <v>18</v>
+        <v>19</v>
       </c>
       <c r="F43" s="1" t="s">
-        <v>19</v>
+        <v>20</v>
       </c>
       <c r="G43" s="1" t="s">
-        <v>20</v>
+        <v>66</v>
       </c>
       <c r="H43" s="1" t="s">
-        <v>24</v>
+        <v>23</v>
       </c>
     </row>
     <row r="44" spans="1:8">
       <c r="A44" s="6">
         <v>1</v>
       </c>
+      <c r="H44" s="4">
+        <v>75000</v>
+      </c>
     </row>
     <row r="45" spans="1:8">
       <c r="A45" s="6">
         <v>2</v>
       </c>
+      <c r="H45" s="4">
+        <v>168000</v>
+      </c>
     </row>
     <row r="46" spans="1:8">
       <c r="A46" s="6">
         <v>3</v>
       </c>
+      <c r="H46" s="4">
+        <v>288000</v>
+      </c>
     </row>
     <row r="47" spans="1:8">
       <c r="A47" s="6">
         <v>4</v>
       </c>
+      <c r="H47" s="4">
+        <v>646000</v>
+      </c>
     </row>
     <row r="48" spans="1:8">
       <c r="A48" s="6">
         <v>5</v>
       </c>
+      <c r="H48" s="4">
+        <v>1245000</v>
+      </c>
     </row>
     <row r="49" spans="1:8">
       <c r="A49" s="6">
         <v>6</v>
       </c>
-    </row>
-    <row r="51" spans="1:8">
-      <c r="A51" s="3" t="s">
-        <v>27</v>
-      </c>
-    </row>
-    <row r="52" spans="1:8">
-      <c r="A52" s="1" t="s">
-        <v>11</v>
-      </c>
-      <c r="B52" s="1" t="s">
-        <v>17</v>
-      </c>
-      <c r="C52" s="1" t="s">
-        <v>14</v>
-      </c>
-      <c r="D52" s="1" t="s">
-        <v>15</v>
-      </c>
-      <c r="E52" s="1" t="s">
-        <v>18</v>
-      </c>
-      <c r="F52" s="1" t="s">
-        <v>19</v>
-      </c>
-      <c r="G52" s="1" t="s">
-        <v>20</v>
-      </c>
-      <c r="H52" s="1" t="s">
-        <v>24</v>
-      </c>
-    </row>
-    <row r="53" spans="1:8">
-      <c r="A53" s="6">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="54" spans="1:8">
-      <c r="A54" s="6">
-        <v>2</v>
-      </c>
-    </row>
-    <row r="55" spans="1:8">
-      <c r="A55" s="6">
-        <v>3</v>
-      </c>
-    </row>
-    <row r="56" spans="1:8">
-      <c r="A56" s="6">
-        <v>4</v>
-      </c>
-    </row>
-    <row r="57" spans="1:8">
-      <c r="A57" s="6">
-        <v>5</v>
-      </c>
-    </row>
-    <row r="58" spans="1:8">
-      <c r="A58" s="6">
-        <v>6</v>
+      <c r="H49" s="4">
+        <v>2440000</v>
       </c>
     </row>
   </sheetData>
@@ -1246,7 +1576,7 @@
   <dimension ref="A1:G5"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="B5" sqref="B5"/>
+      <selection activeCell="F45" sqref="F45"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="12.33203125" defaultRowHeight="15" x14ac:dyDescent="0"/>
@@ -1261,23 +1591,23 @@
   <sheetData>
     <row r="1" spans="1:7">
       <c r="A1" s="1" t="s">
-        <v>28</v>
+        <v>27</v>
       </c>
     </row>
     <row r="3" spans="1:7">
       <c r="A3" s="3" t="s">
-        <v>29</v>
+        <v>28</v>
       </c>
     </row>
     <row r="4" spans="1:7">
       <c r="A4" s="1" t="s">
+        <v>29</v>
+      </c>
+      <c r="B4" s="1" t="s">
         <v>30</v>
       </c>
-      <c r="B4" s="1" t="s">
+      <c r="C4" s="1" t="s">
         <v>31</v>
-      </c>
-      <c r="C4" s="1" t="s">
-        <v>32</v>
       </c>
       <c r="D4" s="1" t="s">
         <v>13</v>
@@ -1299,6 +1629,7 @@
     </row>
   </sheetData>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
+  <pageSetup orientation="portrait" horizontalDpi="4294967292" verticalDpi="4294967292"/>
   <extLst>
     <ext xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" uri="{64002731-A6B0-56B0-2670-7721B7C09600}">
       <mx:PLV Mode="0" OnePage="0" WScale="0"/>
@@ -1309,13 +1640,2961 @@
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1"/>
+  <dimension ref="A1:AI55"/>
   <sheetViews>
-    <sheetView workbookViewId="0"/>
+    <sheetView topLeftCell="A2" workbookViewId="0">
+      <selection activeCell="A24" sqref="A24:AI24"/>
+    </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0"/>
-  <sheetData/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="13.33203125" defaultRowHeight="15" x14ac:dyDescent="0"/>
+  <cols>
+    <col min="1" max="1" width="13" customWidth="1"/>
+    <col min="2" max="2" width="14" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="9.5" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="13" bestFit="1" customWidth="1"/>
+    <col min="5" max="22" width="6.5" bestFit="1" customWidth="1"/>
+    <col min="23" max="30" width="7.5" bestFit="1" customWidth="1"/>
+    <col min="31" max="31" width="9.6640625" bestFit="1" customWidth="1"/>
+    <col min="32" max="32" width="10.33203125" bestFit="1" customWidth="1"/>
+    <col min="33" max="33" width="10" bestFit="1" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:35">
+      <c r="A1" s="1" t="s">
+        <v>32</v>
+      </c>
+    </row>
+    <row r="3" spans="1:35">
+      <c r="A3" s="3" t="s">
+        <v>28</v>
+      </c>
+      <c r="B3" t="s">
+        <v>35</v>
+      </c>
+    </row>
+    <row r="4" spans="1:35">
+      <c r="A4" s="1" t="s">
+        <v>29</v>
+      </c>
+      <c r="B4" s="1" t="s">
+        <v>34</v>
+      </c>
+      <c r="C4" s="1" t="s">
+        <v>33</v>
+      </c>
+      <c r="D4" s="1" t="s">
+        <v>30</v>
+      </c>
+      <c r="E4" s="1" t="s">
+        <v>36</v>
+      </c>
+      <c r="F4" s="1" t="s">
+        <v>37</v>
+      </c>
+      <c r="G4" s="1" t="s">
+        <v>38</v>
+      </c>
+      <c r="H4" s="1" t="s">
+        <v>39</v>
+      </c>
+      <c r="I4" s="1" t="s">
+        <v>40</v>
+      </c>
+      <c r="J4" s="1" t="s">
+        <v>41</v>
+      </c>
+      <c r="K4" s="1" t="s">
+        <v>42</v>
+      </c>
+      <c r="L4" s="1" t="s">
+        <v>43</v>
+      </c>
+      <c r="M4" s="1" t="s">
+        <v>44</v>
+      </c>
+      <c r="N4" s="1" t="s">
+        <v>45</v>
+      </c>
+      <c r="O4" s="1" t="s">
+        <v>46</v>
+      </c>
+      <c r="P4" s="1" t="s">
+        <v>47</v>
+      </c>
+      <c r="Q4" s="1" t="s">
+        <v>48</v>
+      </c>
+      <c r="R4" s="1" t="s">
+        <v>49</v>
+      </c>
+      <c r="S4" s="1" t="s">
+        <v>50</v>
+      </c>
+      <c r="T4" s="1" t="s">
+        <v>51</v>
+      </c>
+      <c r="U4" s="1" t="s">
+        <v>52</v>
+      </c>
+      <c r="V4" s="1" t="s">
+        <v>53</v>
+      </c>
+      <c r="W4" s="1" t="s">
+        <v>54</v>
+      </c>
+      <c r="X4" s="1" t="s">
+        <v>55</v>
+      </c>
+      <c r="Y4" s="1" t="s">
+        <v>56</v>
+      </c>
+      <c r="Z4" s="1" t="s">
+        <v>57</v>
+      </c>
+      <c r="AA4" s="1" t="s">
+        <v>58</v>
+      </c>
+      <c r="AB4" s="1" t="s">
+        <v>59</v>
+      </c>
+      <c r="AC4" s="1" t="s">
+        <v>60</v>
+      </c>
+      <c r="AD4" s="1" t="s">
+        <v>61</v>
+      </c>
+      <c r="AE4" s="1" t="s">
+        <v>62</v>
+      </c>
+      <c r="AF4" s="1" t="s">
+        <v>64</v>
+      </c>
+      <c r="AG4" s="1" t="s">
+        <v>65</v>
+      </c>
+      <c r="AH4" s="1" t="s">
+        <v>63</v>
+      </c>
+      <c r="AI4" s="1" t="s">
+        <v>66</v>
+      </c>
+    </row>
+    <row r="5" spans="1:35">
+      <c r="A5" s="7">
+        <v>5</v>
+      </c>
+      <c r="B5" s="7">
+        <v>1</v>
+      </c>
+      <c r="C5" s="7">
+        <v>1E-3</v>
+      </c>
+      <c r="D5" s="8">
+        <v>75000</v>
+      </c>
+      <c r="E5" s="7">
+        <v>19</v>
+      </c>
+      <c r="F5" s="7">
+        <v>1.784</v>
+      </c>
+      <c r="G5" s="7">
+        <v>20</v>
+      </c>
+      <c r="H5" s="7">
+        <v>2.0819000000000001</v>
+      </c>
+      <c r="I5" s="7">
+        <v>22</v>
+      </c>
+      <c r="J5" s="7">
+        <v>2.282</v>
+      </c>
+      <c r="K5" s="7">
+        <v>20</v>
+      </c>
+      <c r="L5" s="7">
+        <v>2.06</v>
+      </c>
+      <c r="M5" s="7">
+        <v>23</v>
+      </c>
+      <c r="N5" s="7">
+        <v>2.63</v>
+      </c>
+      <c r="O5" s="7">
+        <v>21</v>
+      </c>
+      <c r="P5" s="7">
+        <v>2.04</v>
+      </c>
+      <c r="Q5" s="7">
+        <v>21</v>
+      </c>
+      <c r="R5" s="7">
+        <v>2.42</v>
+      </c>
+      <c r="S5" s="7">
+        <v>23</v>
+      </c>
+      <c r="T5" s="7">
+        <v>2.4300000000000002</v>
+      </c>
+      <c r="U5" s="7">
+        <v>22</v>
+      </c>
+      <c r="V5" s="7">
+        <v>2.4300000000000002</v>
+      </c>
+      <c r="W5" s="7">
+        <v>21</v>
+      </c>
+      <c r="X5" s="7">
+        <v>2.27</v>
+      </c>
+      <c r="Y5" s="7">
+        <v>21</v>
+      </c>
+      <c r="Z5" s="7">
+        <v>2.2770000000000001</v>
+      </c>
+      <c r="AA5" s="7">
+        <v>21</v>
+      </c>
+      <c r="AB5" s="7">
+        <v>2.1589999999999998</v>
+      </c>
+      <c r="AC5" s="7">
+        <v>21</v>
+      </c>
+      <c r="AD5" s="7">
+        <v>2.1429999999999998</v>
+      </c>
+      <c r="AE5">
+        <f>E5+G5+I5+K5+M5+O5+Q5+S5+U5+W5+Y5+AA5+AC5</f>
+        <v>275</v>
+      </c>
+      <c r="AF5" s="9">
+        <f>F5+H5+J5+L5+N5+P5+R5+T5+V5+X5+Z5+AB5+AD5</f>
+        <v>29.006900000000002</v>
+      </c>
+      <c r="AG5">
+        <v>33.700000000000003</v>
+      </c>
+      <c r="AH5">
+        <v>68.7</v>
+      </c>
+      <c r="AI5">
+        <f>(A5+1)*AE5</f>
+        <v>1650</v>
+      </c>
+    </row>
+    <row r="6" spans="1:35">
+      <c r="A6" s="7">
+        <v>5</v>
+      </c>
+      <c r="B6" s="7">
+        <v>1</v>
+      </c>
+      <c r="C6" s="7">
+        <v>0.01</v>
+      </c>
+      <c r="D6" s="8">
+        <v>75000</v>
+      </c>
+      <c r="E6" s="7">
+        <v>22</v>
+      </c>
+      <c r="F6" s="7">
+        <v>1.7</v>
+      </c>
+      <c r="G6" s="7">
+        <v>22</v>
+      </c>
+      <c r="H6" s="7">
+        <v>1.84</v>
+      </c>
+      <c r="I6" s="7">
+        <v>22</v>
+      </c>
+      <c r="J6" s="7">
+        <v>1.84</v>
+      </c>
+      <c r="K6" s="7">
+        <v>22</v>
+      </c>
+      <c r="L6" s="7">
+        <v>1.81</v>
+      </c>
+      <c r="M6" s="7">
+        <v>24</v>
+      </c>
+      <c r="N6" s="7">
+        <v>2.33</v>
+      </c>
+      <c r="O6" s="7">
+        <v>24</v>
+      </c>
+      <c r="P6" s="7">
+        <v>2.2400000000000002</v>
+      </c>
+      <c r="Q6" s="7">
+        <v>25</v>
+      </c>
+      <c r="R6" s="7">
+        <v>2.34</v>
+      </c>
+      <c r="S6" s="7">
+        <v>22</v>
+      </c>
+      <c r="T6" s="7">
+        <v>1.66</v>
+      </c>
+      <c r="U6" s="7">
+        <v>21</v>
+      </c>
+      <c r="V6" s="7">
+        <v>1.736</v>
+      </c>
+      <c r="W6" s="7">
+        <v>22</v>
+      </c>
+      <c r="X6" s="7">
+        <v>1.7</v>
+      </c>
+      <c r="Y6" s="7">
+        <v>22</v>
+      </c>
+      <c r="Z6" s="7">
+        <v>1.89</v>
+      </c>
+      <c r="AA6" s="7">
+        <v>22</v>
+      </c>
+      <c r="AB6" s="7">
+        <v>1.72</v>
+      </c>
+      <c r="AC6" s="7">
+        <v>21</v>
+      </c>
+      <c r="AD6" s="7">
+        <v>1.66</v>
+      </c>
+      <c r="AE6">
+        <f t="shared" ref="AE6:AE15" si="0">E6+G6+I6+K6+M6+O6+Q6+S6+U6+W6+Y6+AA6+AC6</f>
+        <v>291</v>
+      </c>
+      <c r="AF6" s="9">
+        <f t="shared" ref="AF6:AF15" si="1">F6+H6+J6+L6+N6+P6+R6+T6+V6+X6+Z6+AB6+AD6</f>
+        <v>24.465999999999998</v>
+      </c>
+      <c r="AG6">
+        <v>10.9</v>
+      </c>
+      <c r="AH6">
+        <v>38.700000000000003</v>
+      </c>
+      <c r="AI6">
+        <f t="shared" ref="AI6:AI15" si="2">(A6+1)*AE6</f>
+        <v>1746</v>
+      </c>
+    </row>
+    <row r="7" spans="1:35">
+      <c r="A7" s="7">
+        <v>5</v>
+      </c>
+      <c r="B7" s="7">
+        <v>1</v>
+      </c>
+      <c r="C7" s="7">
+        <v>0.05</v>
+      </c>
+      <c r="D7" s="8">
+        <v>75000</v>
+      </c>
+      <c r="E7" s="7">
+        <v>27</v>
+      </c>
+      <c r="F7" s="7">
+        <v>1.94</v>
+      </c>
+      <c r="G7" s="7">
+        <v>30</v>
+      </c>
+      <c r="H7" s="7">
+        <v>2.4500000000000002</v>
+      </c>
+      <c r="I7" s="7">
+        <v>27</v>
+      </c>
+      <c r="J7" s="7">
+        <v>1.93</v>
+      </c>
+      <c r="K7" s="7">
+        <v>26</v>
+      </c>
+      <c r="L7" s="7">
+        <v>1.86</v>
+      </c>
+      <c r="M7" s="7">
+        <v>29</v>
+      </c>
+      <c r="N7" s="7">
+        <v>2.3199999999999998</v>
+      </c>
+      <c r="O7" s="7">
+        <v>30</v>
+      </c>
+      <c r="P7" s="7">
+        <v>2.59</v>
+      </c>
+      <c r="Q7" s="7">
+        <v>25</v>
+      </c>
+      <c r="R7" s="7">
+        <v>1.86</v>
+      </c>
+      <c r="S7" s="7">
+        <v>28</v>
+      </c>
+      <c r="T7" s="7">
+        <v>2.31</v>
+      </c>
+      <c r="U7" s="7">
+        <v>28</v>
+      </c>
+      <c r="V7" s="7">
+        <v>2.14</v>
+      </c>
+      <c r="W7" s="7">
+        <v>27</v>
+      </c>
+      <c r="X7" s="7">
+        <v>2</v>
+      </c>
+      <c r="Y7" s="7">
+        <v>28</v>
+      </c>
+      <c r="Z7" s="7">
+        <v>2.2000000000000002</v>
+      </c>
+      <c r="AA7" s="7">
+        <v>30</v>
+      </c>
+      <c r="AB7" s="7">
+        <v>2.69</v>
+      </c>
+      <c r="AC7" s="7">
+        <v>28</v>
+      </c>
+      <c r="AD7" s="7">
+        <v>4.45</v>
+      </c>
+      <c r="AE7">
+        <f t="shared" si="0"/>
+        <v>363</v>
+      </c>
+      <c r="AF7" s="9">
+        <f t="shared" si="1"/>
+        <v>30.74</v>
+      </c>
+      <c r="AG7">
+        <v>2.38</v>
+      </c>
+      <c r="AH7">
+        <v>33.9</v>
+      </c>
+      <c r="AI7">
+        <f t="shared" si="2"/>
+        <v>2178</v>
+      </c>
+    </row>
+    <row r="8" spans="1:35">
+      <c r="A8" s="7">
+        <v>5</v>
+      </c>
+      <c r="B8" s="7">
+        <v>1</v>
+      </c>
+      <c r="C8" s="7">
+        <v>0.1</v>
+      </c>
+      <c r="D8" s="8">
+        <v>75000</v>
+      </c>
+      <c r="E8" s="7">
+        <v>98</v>
+      </c>
+      <c r="F8" s="7">
+        <v>9.5</v>
+      </c>
+      <c r="G8" s="7">
+        <v>125</v>
+      </c>
+      <c r="H8" s="7">
+        <v>12.2</v>
+      </c>
+      <c r="I8" s="7">
+        <v>102</v>
+      </c>
+      <c r="J8">
+        <v>9.65</v>
+      </c>
+      <c r="K8" s="7">
+        <v>85</v>
+      </c>
+      <c r="L8" s="7">
+        <v>7.5</v>
+      </c>
+      <c r="M8" s="7">
+        <v>74</v>
+      </c>
+      <c r="N8" s="7">
+        <v>6.89</v>
+      </c>
+      <c r="O8" s="7">
+        <v>108</v>
+      </c>
+      <c r="P8" s="7">
+        <v>10.4</v>
+      </c>
+      <c r="Q8" s="7">
+        <v>63</v>
+      </c>
+      <c r="R8" s="7">
+        <v>5.48</v>
+      </c>
+      <c r="S8" s="7">
+        <v>67</v>
+      </c>
+      <c r="T8" s="7">
+        <v>6.28</v>
+      </c>
+      <c r="U8" s="7">
+        <v>72</v>
+      </c>
+      <c r="V8" s="7">
+        <v>5.98</v>
+      </c>
+      <c r="W8" s="7">
+        <v>74</v>
+      </c>
+      <c r="X8" s="7">
+        <v>6.78</v>
+      </c>
+      <c r="Y8" s="7">
+        <v>83</v>
+      </c>
+      <c r="Z8" s="7">
+        <v>7.68</v>
+      </c>
+      <c r="AA8" s="7">
+        <v>82</v>
+      </c>
+      <c r="AB8" s="7">
+        <v>7.5</v>
+      </c>
+      <c r="AC8" s="7">
+        <v>65</v>
+      </c>
+      <c r="AD8" s="7">
+        <v>5.84</v>
+      </c>
+      <c r="AE8">
+        <f t="shared" si="0"/>
+        <v>1098</v>
+      </c>
+      <c r="AF8" s="9">
+        <f t="shared" si="1"/>
+        <v>101.68</v>
+      </c>
+      <c r="AG8">
+        <v>1.22</v>
+      </c>
+      <c r="AH8">
+        <v>105.5</v>
+      </c>
+      <c r="AI8">
+        <f t="shared" si="2"/>
+        <v>6588</v>
+      </c>
+    </row>
+    <row r="9" spans="1:35">
+      <c r="A9" s="7">
+        <v>5</v>
+      </c>
+      <c r="B9" s="7">
+        <v>2</v>
+      </c>
+      <c r="C9" s="7">
+        <v>0.01</v>
+      </c>
+      <c r="D9" s="8">
+        <v>75000</v>
+      </c>
+      <c r="E9" s="7">
+        <v>13</v>
+      </c>
+      <c r="F9" s="7">
+        <v>1.1890000000000001</v>
+      </c>
+      <c r="G9" s="7">
+        <v>13</v>
+      </c>
+      <c r="H9" s="7">
+        <v>1.08</v>
+      </c>
+      <c r="I9" s="7">
+        <v>12</v>
+      </c>
+      <c r="J9" s="7">
+        <v>0.97499999999999998</v>
+      </c>
+      <c r="K9" s="7">
+        <v>12</v>
+      </c>
+      <c r="L9" s="7">
+        <v>1.02</v>
+      </c>
+      <c r="M9" s="7">
+        <v>14</v>
+      </c>
+      <c r="N9" s="7">
+        <v>1.26</v>
+      </c>
+      <c r="O9" s="7">
+        <v>12</v>
+      </c>
+      <c r="P9" s="7">
+        <v>0.99099999999999999</v>
+      </c>
+      <c r="Q9" s="7">
+        <v>12</v>
+      </c>
+      <c r="R9" s="7">
+        <v>0.99299999999999999</v>
+      </c>
+      <c r="S9" s="7">
+        <v>13</v>
+      </c>
+      <c r="T9" s="7">
+        <v>1.097</v>
+      </c>
+      <c r="U9" s="7">
+        <v>12</v>
+      </c>
+      <c r="V9" s="7">
+        <v>0.90400000000000003</v>
+      </c>
+      <c r="W9" s="7">
+        <v>13</v>
+      </c>
+      <c r="X9" s="7">
+        <v>1.07</v>
+      </c>
+      <c r="Y9" s="7">
+        <v>12</v>
+      </c>
+      <c r="Z9" s="7">
+        <v>0.94</v>
+      </c>
+      <c r="AA9" s="7">
+        <v>12</v>
+      </c>
+      <c r="AB9" s="7">
+        <v>0.91700000000000004</v>
+      </c>
+      <c r="AC9" s="7">
+        <v>12</v>
+      </c>
+      <c r="AD9" s="7">
+        <v>1.01</v>
+      </c>
+      <c r="AE9">
+        <f t="shared" ref="AE9:AF11" si="3">E9+G9+I9+K9+M9+O9+Q9+S9+U9+W9+Y9+AA9+AC9</f>
+        <v>162</v>
+      </c>
+      <c r="AF9" s="9">
+        <f t="shared" si="3"/>
+        <v>13.446</v>
+      </c>
+      <c r="AG9">
+        <v>74.010000000000005</v>
+      </c>
+      <c r="AH9">
+        <f>92.89</f>
+        <v>92.89</v>
+      </c>
+      <c r="AI9">
+        <f>(A9+1)*AE9</f>
+        <v>972</v>
+      </c>
+    </row>
+    <row r="10" spans="1:35">
+      <c r="A10" s="7">
+        <v>5</v>
+      </c>
+      <c r="B10" s="7">
+        <v>2</v>
+      </c>
+      <c r="C10" s="7">
+        <v>0.05</v>
+      </c>
+      <c r="D10" s="8">
+        <v>75000</v>
+      </c>
+      <c r="E10" s="7">
+        <v>13</v>
+      </c>
+      <c r="F10" s="7">
+        <v>0.91200000000000003</v>
+      </c>
+      <c r="G10" s="7">
+        <v>13</v>
+      </c>
+      <c r="H10" s="7">
+        <v>0.85499999999999998</v>
+      </c>
+      <c r="I10" s="7">
+        <v>12</v>
+      </c>
+      <c r="J10" s="7">
+        <v>0.79600000000000004</v>
+      </c>
+      <c r="K10" s="7">
+        <v>13</v>
+      </c>
+      <c r="L10" s="7">
+        <v>0.98</v>
+      </c>
+      <c r="M10" s="7">
+        <v>12</v>
+      </c>
+      <c r="N10" s="7">
+        <v>0.81299999999999994</v>
+      </c>
+      <c r="O10" s="7">
+        <v>13</v>
+      </c>
+      <c r="P10" s="7">
+        <v>0.97199999999999998</v>
+      </c>
+      <c r="Q10" s="7">
+        <v>14</v>
+      </c>
+      <c r="R10" s="7">
+        <v>1.08</v>
+      </c>
+      <c r="S10" s="7">
+        <v>13</v>
+      </c>
+      <c r="T10" s="7">
+        <v>0.89500000000000002</v>
+      </c>
+      <c r="U10" s="7">
+        <v>13</v>
+      </c>
+      <c r="V10" s="7">
+        <v>0.91800000000000004</v>
+      </c>
+      <c r="W10" s="7">
+        <v>13</v>
+      </c>
+      <c r="X10" s="7">
+        <v>0.97599999999999998</v>
+      </c>
+      <c r="Y10" s="7">
+        <v>14</v>
+      </c>
+      <c r="Z10" s="7">
+        <v>1.1599999999999999</v>
+      </c>
+      <c r="AA10" s="7">
+        <v>13</v>
+      </c>
+      <c r="AB10" s="7">
+        <v>0.90600000000000003</v>
+      </c>
+      <c r="AC10" s="7">
+        <v>13</v>
+      </c>
+      <c r="AD10" s="7">
+        <v>0.95</v>
+      </c>
+      <c r="AE10">
+        <f t="shared" si="3"/>
+        <v>169</v>
+      </c>
+      <c r="AF10" s="9">
+        <f t="shared" si="3"/>
+        <v>12.212999999999999</v>
+      </c>
+      <c r="AG10">
+        <v>11.63</v>
+      </c>
+      <c r="AH10">
+        <v>28.8</v>
+      </c>
+      <c r="AI10">
+        <f>(A10+1)*AE10</f>
+        <v>1014</v>
+      </c>
+    </row>
+    <row r="11" spans="1:35">
+      <c r="A11" s="7">
+        <v>5</v>
+      </c>
+      <c r="B11" s="7">
+        <v>2</v>
+      </c>
+      <c r="C11" s="7">
+        <v>0.1</v>
+      </c>
+      <c r="D11" s="8">
+        <v>75000</v>
+      </c>
+      <c r="E11" s="7">
+        <v>183</v>
+      </c>
+      <c r="F11" s="7">
+        <v>17.2</v>
+      </c>
+      <c r="G11" s="7">
+        <v>194</v>
+      </c>
+      <c r="H11" s="7">
+        <v>19.100000000000001</v>
+      </c>
+      <c r="I11" s="7">
+        <v>188</v>
+      </c>
+      <c r="J11" s="7">
+        <v>17.3</v>
+      </c>
+      <c r="K11" s="7">
+        <v>187</v>
+      </c>
+      <c r="L11" s="7">
+        <v>18.2</v>
+      </c>
+      <c r="M11" s="7">
+        <v>339</v>
+      </c>
+      <c r="N11" s="7">
+        <v>33.6</v>
+      </c>
+      <c r="O11" s="7">
+        <v>197</v>
+      </c>
+      <c r="P11" s="7">
+        <v>18.899999999999999</v>
+      </c>
+      <c r="Q11" s="7">
+        <v>283</v>
+      </c>
+      <c r="R11" s="7">
+        <v>27.8</v>
+      </c>
+      <c r="S11" s="7">
+        <v>150</v>
+      </c>
+      <c r="T11" s="7">
+        <v>15.2</v>
+      </c>
+      <c r="U11" s="7">
+        <v>196</v>
+      </c>
+      <c r="V11" s="7">
+        <v>20.3</v>
+      </c>
+      <c r="W11" s="7">
+        <v>191</v>
+      </c>
+      <c r="X11" s="7">
+        <v>19.399999999999999</v>
+      </c>
+      <c r="Y11" s="7">
+        <v>261</v>
+      </c>
+      <c r="Z11" s="7">
+        <v>26.2</v>
+      </c>
+      <c r="AA11" s="7">
+        <v>256</v>
+      </c>
+      <c r="AB11" s="7">
+        <v>27.3</v>
+      </c>
+      <c r="AC11" s="7">
+        <v>125</v>
+      </c>
+      <c r="AD11" s="7">
+        <v>12.9</v>
+      </c>
+      <c r="AE11">
+        <f t="shared" si="3"/>
+        <v>2750</v>
+      </c>
+      <c r="AF11" s="9">
+        <f t="shared" si="3"/>
+        <v>273.39999999999998</v>
+      </c>
+      <c r="AG11">
+        <v>4.32</v>
+      </c>
+      <c r="AH11">
+        <v>281.60000000000002</v>
+      </c>
+      <c r="AI11">
+        <f>(A11+1)*AE11</f>
+        <v>16500</v>
+      </c>
+    </row>
+    <row r="13" spans="1:35">
+      <c r="A13" s="7">
+        <v>4</v>
+      </c>
+      <c r="B13" s="7">
+        <v>1</v>
+      </c>
+      <c r="C13" s="7">
+        <v>1E-3</v>
+      </c>
+      <c r="D13" s="8">
+        <v>75000</v>
+      </c>
+      <c r="E13" s="7">
+        <v>25</v>
+      </c>
+      <c r="F13" s="7">
+        <v>2.29</v>
+      </c>
+      <c r="G13" s="7">
+        <v>27</v>
+      </c>
+      <c r="H13" s="7">
+        <v>2.88</v>
+      </c>
+      <c r="I13" s="7">
+        <v>26</v>
+      </c>
+      <c r="J13" s="7">
+        <v>2.35</v>
+      </c>
+      <c r="K13" s="7">
+        <v>27</v>
+      </c>
+      <c r="L13" s="7">
+        <v>2.63</v>
+      </c>
+      <c r="M13" s="7">
+        <v>26</v>
+      </c>
+      <c r="N13" s="7">
+        <v>2.67</v>
+      </c>
+      <c r="O13" s="7">
+        <v>27</v>
+      </c>
+      <c r="P13" s="7">
+        <v>2.66</v>
+      </c>
+      <c r="Q13" s="7">
+        <v>28</v>
+      </c>
+      <c r="R13" s="7">
+        <v>2.62</v>
+      </c>
+      <c r="S13" s="7">
+        <v>25</v>
+      </c>
+      <c r="T13" s="7">
+        <v>2.31</v>
+      </c>
+      <c r="U13" s="7">
+        <v>26</v>
+      </c>
+      <c r="V13" s="7">
+        <v>2.42</v>
+      </c>
+      <c r="W13" s="7">
+        <v>27</v>
+      </c>
+      <c r="X13" s="7">
+        <v>2.39</v>
+      </c>
+      <c r="Y13" s="7">
+        <v>25</v>
+      </c>
+      <c r="Z13" s="7">
+        <v>2.25</v>
+      </c>
+      <c r="AA13" s="7">
+        <v>27</v>
+      </c>
+      <c r="AB13" s="7">
+        <v>2.66</v>
+      </c>
+      <c r="AC13" s="7">
+        <v>27</v>
+      </c>
+      <c r="AD13" s="7">
+        <v>2.77</v>
+      </c>
+      <c r="AE13">
+        <f t="shared" si="0"/>
+        <v>343</v>
+      </c>
+      <c r="AF13" s="9">
+        <f t="shared" si="1"/>
+        <v>32.9</v>
+      </c>
+      <c r="AG13">
+        <v>33.700000000000003</v>
+      </c>
+      <c r="AH13">
+        <v>72.5</v>
+      </c>
+      <c r="AI13">
+        <f t="shared" si="2"/>
+        <v>1715</v>
+      </c>
+    </row>
+    <row r="14" spans="1:35">
+      <c r="A14" s="7">
+        <v>4</v>
+      </c>
+      <c r="B14" s="7">
+        <v>1</v>
+      </c>
+      <c r="C14" s="7">
+        <v>0.01</v>
+      </c>
+      <c r="D14" s="8">
+        <v>75000</v>
+      </c>
+      <c r="E14" s="7">
+        <v>27</v>
+      </c>
+      <c r="F14" s="7">
+        <v>2.0499999999999998</v>
+      </c>
+      <c r="G14" s="7">
+        <v>28</v>
+      </c>
+      <c r="H14" s="7">
+        <v>2.2400000000000002</v>
+      </c>
+      <c r="I14" s="7">
+        <v>27</v>
+      </c>
+      <c r="J14" s="7">
+        <v>1.9</v>
+      </c>
+      <c r="K14" s="7">
+        <v>27</v>
+      </c>
+      <c r="L14" s="7">
+        <v>1.9</v>
+      </c>
+      <c r="M14" s="7">
+        <v>28</v>
+      </c>
+      <c r="N14" s="7">
+        <v>2.06</v>
+      </c>
+      <c r="O14" s="7">
+        <v>28</v>
+      </c>
+      <c r="P14" s="7">
+        <v>2.15</v>
+      </c>
+      <c r="Q14" s="7">
+        <v>29</v>
+      </c>
+      <c r="R14" s="7">
+        <v>2.16</v>
+      </c>
+      <c r="S14" s="7">
+        <v>30</v>
+      </c>
+      <c r="T14" s="7">
+        <v>2.42</v>
+      </c>
+      <c r="U14" s="7">
+        <v>30</v>
+      </c>
+      <c r="V14" s="7">
+        <v>2.48</v>
+      </c>
+      <c r="W14" s="7">
+        <v>26</v>
+      </c>
+      <c r="X14" s="7">
+        <v>1.97</v>
+      </c>
+      <c r="Y14" s="7">
+        <v>27</v>
+      </c>
+      <c r="Z14" s="7">
+        <v>1.85</v>
+      </c>
+      <c r="AA14" s="7">
+        <v>28</v>
+      </c>
+      <c r="AB14" s="7">
+        <v>2.25</v>
+      </c>
+      <c r="AC14" s="7">
+        <v>27</v>
+      </c>
+      <c r="AD14" s="7">
+        <v>1.98</v>
+      </c>
+      <c r="AE14">
+        <f t="shared" si="0"/>
+        <v>362</v>
+      </c>
+      <c r="AF14" s="9">
+        <f t="shared" si="1"/>
+        <v>27.410000000000004</v>
+      </c>
+      <c r="AG14">
+        <v>10.96</v>
+      </c>
+      <c r="AH14">
+        <v>41.6</v>
+      </c>
+      <c r="AI14">
+        <f t="shared" si="2"/>
+        <v>1810</v>
+      </c>
+    </row>
+    <row r="15" spans="1:35">
+      <c r="A15" s="7">
+        <v>4</v>
+      </c>
+      <c r="B15" s="7">
+        <v>1</v>
+      </c>
+      <c r="C15" s="7">
+        <v>0.05</v>
+      </c>
+      <c r="D15" s="8">
+        <v>75000</v>
+      </c>
+      <c r="E15" s="7">
+        <v>37</v>
+      </c>
+      <c r="F15" s="7">
+        <v>2.54</v>
+      </c>
+      <c r="G15" s="7">
+        <v>45</v>
+      </c>
+      <c r="H15" s="7">
+        <v>3.47</v>
+      </c>
+      <c r="I15" s="7">
+        <v>39</v>
+      </c>
+      <c r="J15" s="7">
+        <v>2.93</v>
+      </c>
+      <c r="K15" s="7">
+        <v>37</v>
+      </c>
+      <c r="L15" s="7">
+        <v>2.77</v>
+      </c>
+      <c r="M15" s="7">
+        <v>38</v>
+      </c>
+      <c r="N15" s="7">
+        <v>2.64</v>
+      </c>
+      <c r="O15" s="7">
+        <v>38</v>
+      </c>
+      <c r="P15" s="7">
+        <v>2.5</v>
+      </c>
+      <c r="Q15" s="7">
+        <v>36</v>
+      </c>
+      <c r="R15" s="7">
+        <v>2.4700000000000002</v>
+      </c>
+      <c r="S15" s="7">
+        <v>48</v>
+      </c>
+      <c r="T15" s="7">
+        <v>3.98</v>
+      </c>
+      <c r="U15" s="7">
+        <v>37</v>
+      </c>
+      <c r="V15" s="7">
+        <v>2.58</v>
+      </c>
+      <c r="W15" s="7">
+        <v>39</v>
+      </c>
+      <c r="X15" s="7">
+        <v>3.22</v>
+      </c>
+      <c r="Y15" s="7">
+        <v>39</v>
+      </c>
+      <c r="Z15" s="7">
+        <v>2.84</v>
+      </c>
+      <c r="AA15" s="7">
+        <v>43</v>
+      </c>
+      <c r="AB15" s="7">
+        <v>3.57</v>
+      </c>
+      <c r="AC15" s="7">
+        <v>39</v>
+      </c>
+      <c r="AD15" s="7">
+        <v>3.06</v>
+      </c>
+      <c r="AE15">
+        <f t="shared" si="0"/>
+        <v>515</v>
+      </c>
+      <c r="AF15" s="9">
+        <f t="shared" si="1"/>
+        <v>38.57</v>
+      </c>
+      <c r="AG15">
+        <v>2.39</v>
+      </c>
+      <c r="AH15">
+        <v>44.1</v>
+      </c>
+      <c r="AI15">
+        <f t="shared" si="2"/>
+        <v>2575</v>
+      </c>
+    </row>
+    <row r="16" spans="1:35">
+      <c r="A16" s="7">
+        <v>4</v>
+      </c>
+      <c r="B16" s="7">
+        <v>2</v>
+      </c>
+      <c r="C16" s="7">
+        <v>0.01</v>
+      </c>
+      <c r="D16" s="8">
+        <v>75000</v>
+      </c>
+      <c r="E16" s="7">
+        <v>14</v>
+      </c>
+      <c r="F16" s="7">
+        <v>1.02</v>
+      </c>
+      <c r="G16" s="7">
+        <v>15</v>
+      </c>
+      <c r="H16" s="7">
+        <v>1.17</v>
+      </c>
+      <c r="I16" s="7">
+        <v>14</v>
+      </c>
+      <c r="J16" s="7">
+        <v>1.01</v>
+      </c>
+      <c r="K16" s="7">
+        <v>14</v>
+      </c>
+      <c r="L16" s="7">
+        <v>1.004</v>
+      </c>
+      <c r="M16" s="7">
+        <v>14</v>
+      </c>
+      <c r="N16" s="7">
+        <v>0.97899999999999998</v>
+      </c>
+      <c r="O16" s="7">
+        <v>14</v>
+      </c>
+      <c r="P16" s="7">
+        <v>1.1100000000000001</v>
+      </c>
+      <c r="Q16" s="7">
+        <v>13</v>
+      </c>
+      <c r="R16" s="7">
+        <v>8.82</v>
+      </c>
+      <c r="S16" s="7">
+        <v>14</v>
+      </c>
+      <c r="T16" s="7">
+        <v>1.08</v>
+      </c>
+      <c r="U16" s="7">
+        <v>13</v>
+      </c>
+      <c r="V16" s="7">
+        <v>0.91300000000000003</v>
+      </c>
+      <c r="W16" s="7">
+        <v>14</v>
+      </c>
+      <c r="X16" s="7">
+        <v>1.01</v>
+      </c>
+      <c r="Y16" s="7">
+        <v>14</v>
+      </c>
+      <c r="Z16" s="7">
+        <v>1.06</v>
+      </c>
+      <c r="AA16" s="7">
+        <v>14</v>
+      </c>
+      <c r="AB16" s="7">
+        <v>1.04</v>
+      </c>
+      <c r="AC16" s="7">
+        <v>14</v>
+      </c>
+      <c r="AD16" s="7">
+        <v>1.21</v>
+      </c>
+      <c r="AE16">
+        <f t="shared" ref="AE16:AF18" si="4">E16+G16+I16+K16+M16+O16+Q16+S16+U16+W16+Y16+AA16+AC16</f>
+        <v>181</v>
+      </c>
+      <c r="AF16" s="9">
+        <f t="shared" si="4"/>
+        <v>21.426000000000002</v>
+      </c>
+      <c r="AG16">
+        <v>73.400000000000006</v>
+      </c>
+      <c r="AH16">
+        <v>92.5</v>
+      </c>
+      <c r="AI16">
+        <f>(A16+1)*AE16</f>
+        <v>905</v>
+      </c>
+    </row>
+    <row r="17" spans="1:35">
+      <c r="A17" s="7">
+        <v>4</v>
+      </c>
+      <c r="B17" s="7">
+        <v>2</v>
+      </c>
+      <c r="C17" s="7">
+        <v>0.05</v>
+      </c>
+      <c r="D17" s="8">
+        <v>75000</v>
+      </c>
+      <c r="E17" s="7">
+        <v>16</v>
+      </c>
+      <c r="F17" s="7">
+        <v>1.0269999999999999</v>
+      </c>
+      <c r="G17" s="7">
+        <v>15</v>
+      </c>
+      <c r="H17" s="7">
+        <v>1.01</v>
+      </c>
+      <c r="I17" s="7">
+        <v>15</v>
+      </c>
+      <c r="J17" s="7">
+        <v>0.98699999999999999</v>
+      </c>
+      <c r="K17" s="7">
+        <v>16</v>
+      </c>
+      <c r="L17" s="7">
+        <v>1.1599999999999999</v>
+      </c>
+      <c r="M17" s="7">
+        <v>15</v>
+      </c>
+      <c r="N17" s="7">
+        <v>1.03</v>
+      </c>
+      <c r="O17" s="7">
+        <v>16</v>
+      </c>
+      <c r="P17" s="7">
+        <v>1.0900000000000001</v>
+      </c>
+      <c r="Q17" s="7">
+        <v>15</v>
+      </c>
+      <c r="R17" s="7">
+        <v>0.99299999999999999</v>
+      </c>
+      <c r="S17" s="7">
+        <v>14</v>
+      </c>
+      <c r="T17" s="7">
+        <v>0.86</v>
+      </c>
+      <c r="U17" s="7">
+        <v>15</v>
+      </c>
+      <c r="V17" s="7">
+        <v>0.91</v>
+      </c>
+      <c r="W17" s="7">
+        <v>15</v>
+      </c>
+      <c r="X17" s="7">
+        <v>0.93799999999999994</v>
+      </c>
+      <c r="Y17" s="7">
+        <v>15</v>
+      </c>
+      <c r="Z17" s="7">
+        <v>0.94399999999999995</v>
+      </c>
+      <c r="AA17" s="7">
+        <v>15</v>
+      </c>
+      <c r="AB17" s="7">
+        <v>0.95</v>
+      </c>
+      <c r="AC17" s="7">
+        <v>16</v>
+      </c>
+      <c r="AD17" s="7">
+        <v>1.05</v>
+      </c>
+      <c r="AE17">
+        <f t="shared" si="4"/>
+        <v>198</v>
+      </c>
+      <c r="AF17" s="9">
+        <f t="shared" si="4"/>
+        <v>12.949000000000002</v>
+      </c>
+      <c r="AG17">
+        <v>11.65</v>
+      </c>
+      <c r="AH17">
+        <v>29.5</v>
+      </c>
+      <c r="AI17">
+        <f>(A17+1)*AE17</f>
+        <v>990</v>
+      </c>
+    </row>
+    <row r="18" spans="1:35">
+      <c r="A18" s="7">
+        <v>4</v>
+      </c>
+      <c r="B18" s="7">
+        <v>3</v>
+      </c>
+      <c r="C18" s="7">
+        <v>0.05</v>
+      </c>
+      <c r="D18" s="8">
+        <v>75000</v>
+      </c>
+      <c r="E18" s="7">
+        <v>10</v>
+      </c>
+      <c r="F18" s="7">
+        <v>0.61</v>
+      </c>
+      <c r="G18" s="7">
+        <v>11</v>
+      </c>
+      <c r="H18" s="7">
+        <v>0.69799999999999995</v>
+      </c>
+      <c r="I18" s="7">
+        <v>10</v>
+      </c>
+      <c r="J18" s="7">
+        <v>0.71899999999999997</v>
+      </c>
+      <c r="K18" s="7">
+        <v>10</v>
+      </c>
+      <c r="L18" s="7">
+        <v>0.68799999999999994</v>
+      </c>
+      <c r="M18" s="7">
+        <v>10</v>
+      </c>
+      <c r="N18" s="7">
+        <v>0.65800000000000003</v>
+      </c>
+      <c r="O18" s="7">
+        <v>10</v>
+      </c>
+      <c r="P18" s="7">
+        <v>0.64900000000000002</v>
+      </c>
+      <c r="Q18" s="7">
+        <v>11</v>
+      </c>
+      <c r="R18" s="7">
+        <v>0.72399999999999998</v>
+      </c>
+      <c r="S18" s="7">
+        <v>10</v>
+      </c>
+      <c r="T18" s="7">
+        <v>0.63400000000000001</v>
+      </c>
+      <c r="U18" s="7">
+        <v>10</v>
+      </c>
+      <c r="V18" s="7">
+        <v>0.63300000000000001</v>
+      </c>
+      <c r="W18" s="7">
+        <v>10</v>
+      </c>
+      <c r="X18" s="7">
+        <v>0.66400000000000003</v>
+      </c>
+      <c r="Y18" s="7">
+        <v>10</v>
+      </c>
+      <c r="Z18" s="7">
+        <v>0.61499999999999999</v>
+      </c>
+      <c r="AA18" s="7">
+        <v>10</v>
+      </c>
+      <c r="AB18" s="7">
+        <v>0.622</v>
+      </c>
+      <c r="AC18" s="7">
+        <v>10</v>
+      </c>
+      <c r="AD18" s="7">
+        <v>0.63700000000000001</v>
+      </c>
+      <c r="AE18">
+        <f t="shared" si="4"/>
+        <v>132</v>
+      </c>
+      <c r="AF18" s="9">
+        <f t="shared" si="4"/>
+        <v>8.5510000000000002</v>
+      </c>
+      <c r="AG18">
+        <v>45.04</v>
+      </c>
+      <c r="AH18">
+        <v>61.3</v>
+      </c>
+      <c r="AI18">
+        <f>(A18+1)*AE18</f>
+        <v>660</v>
+      </c>
+    </row>
+    <row r="19" spans="1:35">
+      <c r="A19" s="7"/>
+      <c r="B19" s="7"/>
+      <c r="C19" s="7"/>
+      <c r="D19" s="8"/>
+      <c r="E19" s="7"/>
+      <c r="F19" s="7"/>
+      <c r="G19" s="7"/>
+      <c r="AF19" s="9"/>
+    </row>
+    <row r="21" spans="1:35">
+      <c r="A21" s="7">
+        <v>3</v>
+      </c>
+      <c r="B21" s="7">
+        <v>1</v>
+      </c>
+      <c r="C21" s="7">
+        <v>0.01</v>
+      </c>
+      <c r="D21" s="8">
+        <v>75000</v>
+      </c>
+      <c r="E21" s="7">
+        <v>38</v>
+      </c>
+      <c r="F21" s="7">
+        <v>2.4900000000000002</v>
+      </c>
+      <c r="G21" s="7">
+        <v>45</v>
+      </c>
+      <c r="H21" s="7">
+        <v>3.25</v>
+      </c>
+      <c r="I21" s="7">
+        <v>43</v>
+      </c>
+      <c r="J21" s="7">
+        <v>3.13</v>
+      </c>
+      <c r="K21" s="7">
+        <v>48</v>
+      </c>
+      <c r="L21" s="7">
+        <v>3.68</v>
+      </c>
+      <c r="M21" s="7">
+        <v>41</v>
+      </c>
+      <c r="N21" s="7">
+        <v>2.85</v>
+      </c>
+      <c r="O21" s="7">
+        <v>47</v>
+      </c>
+      <c r="P21" s="7">
+        <v>3.36</v>
+      </c>
+      <c r="Q21" s="7">
+        <v>44</v>
+      </c>
+      <c r="R21" s="7">
+        <v>3.07</v>
+      </c>
+      <c r="S21" s="7">
+        <v>50</v>
+      </c>
+      <c r="T21" s="7">
+        <v>3.97</v>
+      </c>
+      <c r="U21" s="7">
+        <v>46</v>
+      </c>
+      <c r="V21" s="7">
+        <v>3.2</v>
+      </c>
+      <c r="W21" s="7">
+        <v>48</v>
+      </c>
+      <c r="X21" s="7">
+        <v>3.6</v>
+      </c>
+      <c r="Y21" s="7">
+        <v>42</v>
+      </c>
+      <c r="Z21" s="7">
+        <v>2.9</v>
+      </c>
+      <c r="AA21" s="7">
+        <v>43</v>
+      </c>
+      <c r="AB21" s="7">
+        <v>3.02</v>
+      </c>
+      <c r="AC21" s="7">
+        <v>47</v>
+      </c>
+      <c r="AD21" s="7">
+        <v>3.4</v>
+      </c>
+      <c r="AE21">
+        <f t="shared" ref="AE21:AF24" si="5">E21+G21+I21+K21+M21+O21+Q21+S21+U21+W21+Y21+AA21+AC21</f>
+        <v>582</v>
+      </c>
+      <c r="AF21" s="9">
+        <f t="shared" si="5"/>
+        <v>41.92</v>
+      </c>
+      <c r="AG21">
+        <v>10.9</v>
+      </c>
+      <c r="AH21">
+        <v>56</v>
+      </c>
+      <c r="AI21">
+        <f>(A21+1)*AE21</f>
+        <v>2328</v>
+      </c>
+    </row>
+    <row r="22" spans="1:35">
+      <c r="A22" s="7">
+        <v>3</v>
+      </c>
+      <c r="B22" s="7">
+        <v>2</v>
+      </c>
+      <c r="C22" s="7">
+        <v>0.01</v>
+      </c>
+      <c r="D22" s="8">
+        <v>75000</v>
+      </c>
+      <c r="E22" s="7">
+        <v>18</v>
+      </c>
+      <c r="F22" s="7">
+        <v>1.35</v>
+      </c>
+      <c r="G22" s="7">
+        <v>17</v>
+      </c>
+      <c r="H22" s="7">
+        <v>1.19</v>
+      </c>
+      <c r="I22" s="7">
+        <v>16</v>
+      </c>
+      <c r="J22" s="7">
+        <v>0.98799999999999999</v>
+      </c>
+      <c r="K22" s="7">
+        <v>17</v>
+      </c>
+      <c r="L22" s="7">
+        <v>1.18</v>
+      </c>
+      <c r="M22" s="7">
+        <v>17</v>
+      </c>
+      <c r="N22" s="7">
+        <v>1.1499999999999999</v>
+      </c>
+      <c r="O22" s="7">
+        <v>16</v>
+      </c>
+      <c r="P22" s="7">
+        <v>1.002</v>
+      </c>
+      <c r="Q22" s="7">
+        <v>17</v>
+      </c>
+      <c r="R22" s="7">
+        <v>1.19</v>
+      </c>
+      <c r="S22" s="7">
+        <v>17</v>
+      </c>
+      <c r="T22" s="7">
+        <v>1.1599999999999999</v>
+      </c>
+      <c r="U22" s="7">
+        <v>17</v>
+      </c>
+      <c r="V22" s="7">
+        <v>1.1000000000000001</v>
+      </c>
+      <c r="W22" s="7">
+        <v>16</v>
+      </c>
+      <c r="X22" s="7">
+        <v>1.05</v>
+      </c>
+      <c r="Y22" s="7">
+        <v>16</v>
+      </c>
+      <c r="Z22" s="7">
+        <v>1.03</v>
+      </c>
+      <c r="AA22" s="7">
+        <v>16</v>
+      </c>
+      <c r="AB22" s="7">
+        <v>1.01</v>
+      </c>
+      <c r="AC22" s="7">
+        <v>16</v>
+      </c>
+      <c r="AD22" s="7">
+        <v>1.04</v>
+      </c>
+      <c r="AE22">
+        <f t="shared" si="5"/>
+        <v>216</v>
+      </c>
+      <c r="AF22" s="9">
+        <f t="shared" si="5"/>
+        <v>14.440000000000001</v>
+      </c>
+      <c r="AG22">
+        <v>73.22</v>
+      </c>
+      <c r="AH22">
+        <v>93.1</v>
+      </c>
+      <c r="AI22">
+        <f>(A22+1)*AE22</f>
+        <v>864</v>
+      </c>
+    </row>
+    <row r="23" spans="1:35" s="10" customFormat="1">
+      <c r="A23" s="10">
+        <v>3</v>
+      </c>
+      <c r="B23" s="10">
+        <v>2</v>
+      </c>
+      <c r="C23" s="10">
+        <v>0.05</v>
+      </c>
+      <c r="D23" s="11">
+        <v>75000</v>
+      </c>
+      <c r="E23" s="10">
+        <v>18</v>
+      </c>
+      <c r="F23" s="10">
+        <v>1.04</v>
+      </c>
+      <c r="G23" s="10">
+        <v>18</v>
+      </c>
+      <c r="H23" s="10">
+        <v>1.0900000000000001</v>
+      </c>
+      <c r="I23" s="10">
+        <v>19</v>
+      </c>
+      <c r="J23" s="10">
+        <v>1.1399999999999999</v>
+      </c>
+      <c r="K23" s="10">
+        <v>19</v>
+      </c>
+      <c r="L23" s="10">
+        <v>1.17</v>
+      </c>
+      <c r="M23" s="10">
+        <v>19</v>
+      </c>
+      <c r="N23" s="10">
+        <v>1.3</v>
+      </c>
+      <c r="O23" s="10">
+        <v>18</v>
+      </c>
+      <c r="P23" s="10">
+        <v>1.19</v>
+      </c>
+      <c r="Q23" s="10">
+        <v>19</v>
+      </c>
+      <c r="R23" s="10">
+        <v>1.21</v>
+      </c>
+      <c r="S23" s="10">
+        <v>19</v>
+      </c>
+      <c r="T23" s="10">
+        <v>1.1000000000000001</v>
+      </c>
+      <c r="U23" s="10">
+        <v>18</v>
+      </c>
+      <c r="V23" s="10">
+        <v>1.08</v>
+      </c>
+      <c r="W23" s="10">
+        <v>19</v>
+      </c>
+      <c r="X23" s="10">
+        <v>1.22</v>
+      </c>
+      <c r="Y23" s="10">
+        <v>18</v>
+      </c>
+      <c r="Z23" s="10">
+        <v>1.1000000000000001</v>
+      </c>
+      <c r="AA23" s="10">
+        <v>18</v>
+      </c>
+      <c r="AB23" s="10">
+        <v>1.05</v>
+      </c>
+      <c r="AC23" s="10">
+        <v>19</v>
+      </c>
+      <c r="AD23" s="10">
+        <v>1.1000000000000001</v>
+      </c>
+      <c r="AE23" s="10">
+        <f t="shared" si="5"/>
+        <v>241</v>
+      </c>
+      <c r="AF23" s="12">
+        <f t="shared" si="5"/>
+        <v>14.790000000000001</v>
+      </c>
+      <c r="AG23" s="10">
+        <v>11.6</v>
+      </c>
+      <c r="AH23" s="10">
+        <v>31.3</v>
+      </c>
+      <c r="AI23" s="10">
+        <f>(A23+1)*AE23</f>
+        <v>964</v>
+      </c>
+    </row>
+    <row r="24" spans="1:35">
+      <c r="A24" s="7">
+        <v>3</v>
+      </c>
+      <c r="B24" s="7">
+        <v>3</v>
+      </c>
+      <c r="C24" s="7">
+        <v>0.05</v>
+      </c>
+      <c r="D24" s="8">
+        <v>75000</v>
+      </c>
+      <c r="E24" s="7">
+        <v>12</v>
+      </c>
+      <c r="F24" s="7">
+        <v>0.82599999999999996</v>
+      </c>
+      <c r="G24" s="7">
+        <v>12</v>
+      </c>
+      <c r="H24" s="7">
+        <v>0.72</v>
+      </c>
+      <c r="I24" s="7">
+        <v>12</v>
+      </c>
+      <c r="J24" s="7">
+        <v>0.67</v>
+      </c>
+      <c r="K24" s="7">
+        <v>13</v>
+      </c>
+      <c r="L24" s="7">
+        <v>0.73</v>
+      </c>
+      <c r="M24" s="7">
+        <v>12</v>
+      </c>
+      <c r="N24" s="7">
+        <v>0.74</v>
+      </c>
+      <c r="O24" s="7">
+        <v>12</v>
+      </c>
+      <c r="P24" s="7">
+        <v>0.71</v>
+      </c>
+      <c r="Q24" s="7">
+        <v>12</v>
+      </c>
+      <c r="R24" s="7">
+        <v>0.70199999999999996</v>
+      </c>
+      <c r="S24" s="7">
+        <v>12</v>
+      </c>
+      <c r="T24" s="7">
+        <v>0.68600000000000005</v>
+      </c>
+      <c r="U24" s="7">
+        <v>12</v>
+      </c>
+      <c r="V24" s="7">
+        <v>0.69</v>
+      </c>
+      <c r="W24" s="7">
+        <v>12</v>
+      </c>
+      <c r="X24" s="7">
+        <v>0.66600000000000004</v>
+      </c>
+      <c r="Y24" s="7">
+        <v>12</v>
+      </c>
+      <c r="Z24" s="7">
+        <v>0.64900000000000002</v>
+      </c>
+      <c r="AA24" s="7">
+        <v>12</v>
+      </c>
+      <c r="AB24" s="7">
+        <v>0.71</v>
+      </c>
+      <c r="AC24" s="7">
+        <v>12</v>
+      </c>
+      <c r="AD24" s="7">
+        <v>0.59499999999999997</v>
+      </c>
+      <c r="AE24">
+        <f t="shared" si="5"/>
+        <v>157</v>
+      </c>
+      <c r="AF24" s="9">
+        <f t="shared" si="5"/>
+        <v>9.0940000000000012</v>
+      </c>
+      <c r="AG24">
+        <v>45.02</v>
+      </c>
+      <c r="AH24">
+        <v>61.6</v>
+      </c>
+      <c r="AI24">
+        <f>(A24+1)*AE24</f>
+        <v>628</v>
+      </c>
+    </row>
+    <row r="27" spans="1:35">
+      <c r="A27" s="7">
+        <v>2</v>
+      </c>
+      <c r="B27" s="7">
+        <v>1</v>
+      </c>
+      <c r="C27" s="7">
+        <v>0.01</v>
+      </c>
+      <c r="D27" s="8">
+        <v>75000</v>
+      </c>
+      <c r="E27" s="7">
+        <v>207</v>
+      </c>
+      <c r="F27" s="7">
+        <v>13.5</v>
+      </c>
+      <c r="G27" s="7">
+        <v>178</v>
+      </c>
+      <c r="H27" s="7">
+        <v>11.8</v>
+      </c>
+      <c r="I27" s="7">
+        <v>258</v>
+      </c>
+      <c r="J27" s="7">
+        <v>17.399999999999999</v>
+      </c>
+      <c r="K27" s="7">
+        <v>187</v>
+      </c>
+      <c r="L27" s="7">
+        <v>11.9</v>
+      </c>
+      <c r="M27" s="7">
+        <v>168</v>
+      </c>
+      <c r="N27" s="7">
+        <v>10.7</v>
+      </c>
+      <c r="O27" s="7">
+        <v>208</v>
+      </c>
+      <c r="P27" s="7">
+        <v>13.6</v>
+      </c>
+      <c r="Q27" s="7">
+        <v>204</v>
+      </c>
+      <c r="R27" s="7">
+        <v>13.2</v>
+      </c>
+      <c r="S27" s="7">
+        <v>215</v>
+      </c>
+      <c r="T27" s="7">
+        <v>14.4</v>
+      </c>
+      <c r="U27" s="7">
+        <v>185</v>
+      </c>
+      <c r="V27" s="7">
+        <v>12.1</v>
+      </c>
+      <c r="W27" s="7">
+        <v>194</v>
+      </c>
+      <c r="X27" s="7">
+        <v>12.8</v>
+      </c>
+      <c r="Y27" s="7">
+        <v>205</v>
+      </c>
+      <c r="Z27" s="7">
+        <v>13.6</v>
+      </c>
+      <c r="AA27" s="7">
+        <v>164</v>
+      </c>
+      <c r="AB27" s="7">
+        <v>10.7</v>
+      </c>
+      <c r="AC27" s="7">
+        <v>221</v>
+      </c>
+      <c r="AD27" s="7">
+        <v>14.4</v>
+      </c>
+      <c r="AE27">
+        <f t="shared" ref="AE27:AF29" si="6">E27+G27+I27+K27+M27+O27+Q27+S27+U27+W27+Y27+AA27+AC27</f>
+        <v>2594</v>
+      </c>
+      <c r="AF27" s="9">
+        <f t="shared" si="6"/>
+        <v>170.1</v>
+      </c>
+      <c r="AG27">
+        <v>10.9</v>
+      </c>
+      <c r="AH27">
+        <v>184.5</v>
+      </c>
+      <c r="AI27">
+        <f>(A27+1)*AE27</f>
+        <v>7782</v>
+      </c>
+    </row>
+    <row r="28" spans="1:35">
+      <c r="A28" s="7">
+        <v>2</v>
+      </c>
+      <c r="B28" s="7">
+        <v>2</v>
+      </c>
+      <c r="C28" s="7">
+        <v>0.01</v>
+      </c>
+      <c r="D28" s="8">
+        <v>75000</v>
+      </c>
+      <c r="E28" s="7">
+        <v>22</v>
+      </c>
+      <c r="F28" s="7">
+        <v>1.23</v>
+      </c>
+      <c r="G28" s="7">
+        <v>23</v>
+      </c>
+      <c r="H28" s="7">
+        <v>1.39</v>
+      </c>
+      <c r="I28" s="7">
+        <v>23</v>
+      </c>
+      <c r="J28" s="7">
+        <v>1.36</v>
+      </c>
+      <c r="K28" s="7">
+        <v>25</v>
+      </c>
+      <c r="L28" s="7">
+        <v>1.54</v>
+      </c>
+      <c r="M28" s="7">
+        <v>25</v>
+      </c>
+      <c r="N28" s="7">
+        <v>1.677</v>
+      </c>
+      <c r="O28" s="7">
+        <v>24</v>
+      </c>
+      <c r="P28" s="7">
+        <v>1.49</v>
+      </c>
+      <c r="Q28" s="7">
+        <v>24</v>
+      </c>
+      <c r="R28" s="7">
+        <v>1.42</v>
+      </c>
+      <c r="S28" s="7">
+        <v>23</v>
+      </c>
+      <c r="T28" s="7">
+        <v>1.43</v>
+      </c>
+      <c r="U28" s="7">
+        <v>23</v>
+      </c>
+      <c r="V28" s="7">
+        <v>1.41</v>
+      </c>
+      <c r="W28" s="7">
+        <v>25</v>
+      </c>
+      <c r="X28" s="7">
+        <v>1.52</v>
+      </c>
+      <c r="Y28" s="7">
+        <v>23</v>
+      </c>
+      <c r="Z28" s="7">
+        <v>1.35</v>
+      </c>
+      <c r="AA28" s="7">
+        <v>24</v>
+      </c>
+      <c r="AB28" s="7">
+        <v>1.53</v>
+      </c>
+      <c r="AC28" s="7">
+        <v>24</v>
+      </c>
+      <c r="AD28" s="7">
+        <v>1.51</v>
+      </c>
+      <c r="AE28">
+        <f t="shared" si="6"/>
+        <v>308</v>
+      </c>
+      <c r="AF28" s="9">
+        <f t="shared" si="6"/>
+        <v>18.857000000000003</v>
+      </c>
+      <c r="AG28">
+        <v>73.2</v>
+      </c>
+      <c r="AH28">
+        <v>97.6</v>
+      </c>
+      <c r="AI28">
+        <f>(A28+1)*AE28</f>
+        <v>924</v>
+      </c>
+    </row>
+    <row r="29" spans="1:35">
+      <c r="A29" s="7">
+        <v>2</v>
+      </c>
+      <c r="B29" s="7">
+        <v>2</v>
+      </c>
+      <c r="C29" s="7">
+        <v>0.05</v>
+      </c>
+      <c r="D29" s="8">
+        <v>75000</v>
+      </c>
+      <c r="E29" s="7">
+        <v>27</v>
+      </c>
+      <c r="F29" s="7">
+        <v>1.34</v>
+      </c>
+      <c r="G29" s="7">
+        <v>27</v>
+      </c>
+      <c r="H29" s="7">
+        <v>1.4</v>
+      </c>
+      <c r="I29" s="7">
+        <v>29</v>
+      </c>
+      <c r="J29" s="7">
+        <v>1.56</v>
+      </c>
+      <c r="K29" s="7">
+        <v>28</v>
+      </c>
+      <c r="L29" s="7">
+        <v>1.67</v>
+      </c>
+      <c r="M29" s="7">
+        <v>26</v>
+      </c>
+      <c r="N29" s="7">
+        <v>1.41</v>
+      </c>
+      <c r="O29" s="7">
+        <v>29</v>
+      </c>
+      <c r="P29" s="7">
+        <v>1.58</v>
+      </c>
+      <c r="Q29" s="7">
+        <v>28</v>
+      </c>
+      <c r="R29" s="7">
+        <v>1.51</v>
+      </c>
+      <c r="S29" s="7">
+        <v>29</v>
+      </c>
+      <c r="T29" s="7">
+        <v>1.71</v>
+      </c>
+      <c r="U29" s="7">
+        <v>26</v>
+      </c>
+      <c r="V29" s="7">
+        <v>1.37</v>
+      </c>
+      <c r="W29" s="7">
+        <v>26</v>
+      </c>
+      <c r="X29" s="7">
+        <v>1.35</v>
+      </c>
+      <c r="Y29" s="7">
+        <v>26</v>
+      </c>
+      <c r="Z29" s="7">
+        <v>1.4</v>
+      </c>
+      <c r="AA29" s="7">
+        <v>27</v>
+      </c>
+      <c r="AB29" s="7">
+        <v>1.43</v>
+      </c>
+      <c r="AC29" s="7">
+        <v>30</v>
+      </c>
+      <c r="AD29" s="7">
+        <v>1.82</v>
+      </c>
+      <c r="AE29">
+        <f t="shared" si="6"/>
+        <v>358</v>
+      </c>
+      <c r="AF29" s="9">
+        <f t="shared" si="6"/>
+        <v>19.55</v>
+      </c>
+      <c r="AG29">
+        <v>11.6</v>
+      </c>
+      <c r="AH29">
+        <v>36.1</v>
+      </c>
+      <c r="AI29">
+        <f>(A29+1)*AE29</f>
+        <v>1074</v>
+      </c>
+    </row>
+    <row r="30" spans="1:35">
+      <c r="A30" s="7"/>
+      <c r="B30" s="7"/>
+      <c r="C30" s="7"/>
+      <c r="D30" s="8"/>
+      <c r="AF30" s="9"/>
+    </row>
+    <row r="32" spans="1:35">
+      <c r="A32" s="7">
+        <v>1</v>
+      </c>
+      <c r="B32" s="7">
+        <v>2</v>
+      </c>
+      <c r="C32" s="7">
+        <v>0.01</v>
+      </c>
+      <c r="D32" s="8">
+        <v>75000</v>
+      </c>
+      <c r="E32" s="7">
+        <v>297</v>
+      </c>
+      <c r="F32" s="7">
+        <v>15.1</v>
+      </c>
+      <c r="G32" s="7">
+        <v>327</v>
+      </c>
+      <c r="H32" s="7">
+        <v>16.7</v>
+      </c>
+      <c r="I32" s="7">
+        <v>277</v>
+      </c>
+      <c r="J32" s="7">
+        <v>13.96</v>
+      </c>
+      <c r="K32" s="7">
+        <v>363</v>
+      </c>
+      <c r="L32" s="7">
+        <v>18.8</v>
+      </c>
+      <c r="M32" s="7">
+        <v>345</v>
+      </c>
+      <c r="N32" s="7">
+        <v>17.68</v>
+      </c>
+      <c r="O32" s="7">
+        <v>371</v>
+      </c>
+      <c r="P32" s="7">
+        <v>18.899999999999999</v>
+      </c>
+      <c r="Q32" s="7">
+        <v>323</v>
+      </c>
+      <c r="R32" s="7">
+        <v>16.5</v>
+      </c>
+      <c r="S32" s="7">
+        <v>394</v>
+      </c>
+      <c r="T32" s="7">
+        <v>20.8</v>
+      </c>
+      <c r="U32" s="7">
+        <v>325</v>
+      </c>
+      <c r="V32" s="7">
+        <v>16.7</v>
+      </c>
+      <c r="W32" s="7">
+        <v>342</v>
+      </c>
+      <c r="X32" s="7">
+        <v>17.8</v>
+      </c>
+      <c r="Y32" s="7">
+        <v>359</v>
+      </c>
+      <c r="Z32" s="7">
+        <v>18.7</v>
+      </c>
+      <c r="AA32" s="7">
+        <v>271</v>
+      </c>
+      <c r="AB32" s="7">
+        <v>13.8</v>
+      </c>
+      <c r="AC32" s="7">
+        <v>308</v>
+      </c>
+      <c r="AD32" s="7">
+        <v>15.6</v>
+      </c>
+      <c r="AE32">
+        <f>E32+G32+I32+K32+M32+O32+Q32+S32+U32+W32+Y32+AA32+AC32</f>
+        <v>4302</v>
+      </c>
+      <c r="AF32" s="9">
+        <f>F32+H32+J32+L32+N32+P32+R32+T32+V32+X32+Z32+AB32+AD32</f>
+        <v>221.04000000000002</v>
+      </c>
+      <c r="AG32">
+        <v>72.900000000000006</v>
+      </c>
+      <c r="AH32">
+        <v>299.3</v>
+      </c>
+      <c r="AI32">
+        <f>(A32+1)*AE32</f>
+        <v>8604</v>
+      </c>
+    </row>
+    <row r="34" spans="1:35">
+      <c r="A34" s="7"/>
+      <c r="B34" s="7"/>
+      <c r="C34" s="7"/>
+      <c r="D34" s="8"/>
+      <c r="AF34" s="9"/>
+    </row>
+    <row r="35" spans="1:35">
+      <c r="A35" s="7"/>
+      <c r="B35" s="7"/>
+      <c r="C35" s="7"/>
+      <c r="D35" s="8"/>
+      <c r="AF35" s="9"/>
+    </row>
+    <row r="36" spans="1:35">
+      <c r="A36" s="1" t="s">
+        <v>67</v>
+      </c>
+      <c r="B36" s="7">
+        <v>1</v>
+      </c>
+      <c r="C36" s="7">
+        <v>1E-3</v>
+      </c>
+      <c r="E36">
+        <v>343</v>
+      </c>
+      <c r="G36">
+        <v>304</v>
+      </c>
+      <c r="I36">
+        <v>306</v>
+      </c>
+      <c r="K36">
+        <v>292</v>
+      </c>
+      <c r="M36">
+        <v>301</v>
+      </c>
+      <c r="O36">
+        <v>315</v>
+      </c>
+      <c r="Q36">
+        <v>298</v>
+      </c>
+      <c r="S36">
+        <v>276</v>
+      </c>
+      <c r="U36">
+        <v>256</v>
+      </c>
+      <c r="W36">
+        <v>261</v>
+      </c>
+      <c r="Y36">
+        <v>247</v>
+      </c>
+      <c r="AA36">
+        <v>230</v>
+      </c>
+      <c r="AC36">
+        <v>226</v>
+      </c>
+      <c r="AE36">
+        <f t="shared" ref="AE36:AE42" si="7">E36+G36+I36+K36+M36+O36+Q36+S36+U36+W36+Y36+AA36+AC36</f>
+        <v>3655</v>
+      </c>
+      <c r="AF36" s="9">
+        <f t="shared" ref="AF36:AF42" si="8">AH36-AG36</f>
+        <v>25</v>
+      </c>
+      <c r="AG36">
+        <v>33.799999999999997</v>
+      </c>
+      <c r="AH36">
+        <v>58.8</v>
+      </c>
+      <c r="AI36">
+        <f t="shared" ref="AI36:AI42" si="9">AE36</f>
+        <v>3655</v>
+      </c>
+    </row>
+    <row r="37" spans="1:35">
+      <c r="B37" s="7">
+        <v>1</v>
+      </c>
+      <c r="C37" s="7">
+        <v>0.01</v>
+      </c>
+      <c r="E37">
+        <v>343</v>
+      </c>
+      <c r="G37">
+        <v>304</v>
+      </c>
+      <c r="I37">
+        <v>306</v>
+      </c>
+      <c r="K37">
+        <v>292</v>
+      </c>
+      <c r="M37">
+        <v>301</v>
+      </c>
+      <c r="O37">
+        <v>315</v>
+      </c>
+      <c r="Q37">
+        <v>298</v>
+      </c>
+      <c r="S37">
+        <v>276</v>
+      </c>
+      <c r="U37">
+        <v>256</v>
+      </c>
+      <c r="W37">
+        <v>261</v>
+      </c>
+      <c r="Y37">
+        <v>247</v>
+      </c>
+      <c r="AA37">
+        <v>230</v>
+      </c>
+      <c r="AC37">
+        <v>226</v>
+      </c>
+      <c r="AE37">
+        <f t="shared" si="7"/>
+        <v>3655</v>
+      </c>
+      <c r="AF37" s="9">
+        <f t="shared" si="8"/>
+        <v>17.170000000000002</v>
+      </c>
+      <c r="AG37">
+        <v>10.95</v>
+      </c>
+      <c r="AH37">
+        <v>28.12</v>
+      </c>
+      <c r="AI37">
+        <f t="shared" si="9"/>
+        <v>3655</v>
+      </c>
+    </row>
+    <row r="38" spans="1:35">
+      <c r="B38" s="7">
+        <v>1</v>
+      </c>
+      <c r="C38" s="7">
+        <v>0.05</v>
+      </c>
+      <c r="E38">
+        <v>342</v>
+      </c>
+      <c r="G38">
+        <v>303</v>
+      </c>
+      <c r="I38">
+        <v>305</v>
+      </c>
+      <c r="K38">
+        <v>292</v>
+      </c>
+      <c r="M38">
+        <v>300</v>
+      </c>
+      <c r="O38">
+        <v>315</v>
+      </c>
+      <c r="Q38">
+        <v>298</v>
+      </c>
+      <c r="S38">
+        <v>275</v>
+      </c>
+      <c r="U38">
+        <v>256</v>
+      </c>
+      <c r="W38">
+        <v>261</v>
+      </c>
+      <c r="Y38">
+        <v>247</v>
+      </c>
+      <c r="AA38">
+        <v>230</v>
+      </c>
+      <c r="AC38">
+        <v>225</v>
+      </c>
+      <c r="AE38">
+        <f t="shared" si="7"/>
+        <v>3649</v>
+      </c>
+      <c r="AF38" s="9">
+        <f t="shared" si="8"/>
+        <v>14.650000000000002</v>
+      </c>
+      <c r="AG38">
+        <v>2.38</v>
+      </c>
+      <c r="AH38">
+        <v>17.03</v>
+      </c>
+      <c r="AI38">
+        <f t="shared" si="9"/>
+        <v>3649</v>
+      </c>
+    </row>
+    <row r="39" spans="1:35">
+      <c r="B39" s="7">
+        <v>1</v>
+      </c>
+      <c r="C39" s="7">
+        <v>0.1</v>
+      </c>
+      <c r="E39">
+        <v>342</v>
+      </c>
+      <c r="G39">
+        <v>303</v>
+      </c>
+      <c r="I39">
+        <v>305</v>
+      </c>
+      <c r="K39">
+        <v>292</v>
+      </c>
+      <c r="M39">
+        <v>300</v>
+      </c>
+      <c r="O39">
+        <v>314</v>
+      </c>
+      <c r="Q39">
+        <v>298</v>
+      </c>
+      <c r="S39">
+        <v>275</v>
+      </c>
+      <c r="U39">
+        <v>256</v>
+      </c>
+      <c r="W39">
+        <v>261</v>
+      </c>
+      <c r="Y39">
+        <v>247</v>
+      </c>
+      <c r="AA39">
+        <v>230</v>
+      </c>
+      <c r="AC39">
+        <v>225</v>
+      </c>
+      <c r="AE39">
+        <f t="shared" si="7"/>
+        <v>3648</v>
+      </c>
+      <c r="AF39" s="9">
+        <f t="shared" si="8"/>
+        <v>13.868</v>
+      </c>
+      <c r="AG39">
+        <v>1.212</v>
+      </c>
+      <c r="AH39">
+        <v>15.08</v>
+      </c>
+      <c r="AI39">
+        <f t="shared" si="9"/>
+        <v>3648</v>
+      </c>
+    </row>
+    <row r="40" spans="1:35">
+      <c r="B40" s="7">
+        <v>2</v>
+      </c>
+      <c r="C40" s="7">
+        <v>0.01</v>
+      </c>
+      <c r="E40">
+        <v>208</v>
+      </c>
+      <c r="G40">
+        <v>185</v>
+      </c>
+      <c r="I40">
+        <v>186</v>
+      </c>
+      <c r="K40">
+        <v>178</v>
+      </c>
+      <c r="M40">
+        <v>180</v>
+      </c>
+      <c r="O40">
+        <v>193</v>
+      </c>
+      <c r="Q40">
+        <v>182</v>
+      </c>
+      <c r="S40">
+        <v>168</v>
+      </c>
+      <c r="U40">
+        <v>157</v>
+      </c>
+      <c r="W40">
+        <v>160</v>
+      </c>
+      <c r="Y40">
+        <v>152</v>
+      </c>
+      <c r="AA40">
+        <v>143</v>
+      </c>
+      <c r="AC40">
+        <v>138</v>
+      </c>
+      <c r="AE40">
+        <f t="shared" si="7"/>
+        <v>2230</v>
+      </c>
+      <c r="AF40" s="9">
+        <f t="shared" si="8"/>
+        <v>14.394999999999996</v>
+      </c>
+      <c r="AG40">
+        <v>74.03</v>
+      </c>
+      <c r="AH40">
+        <v>88.424999999999997</v>
+      </c>
+      <c r="AI40">
+        <f t="shared" si="9"/>
+        <v>2230</v>
+      </c>
+    </row>
+    <row r="41" spans="1:35">
+      <c r="B41" s="7">
+        <v>2</v>
+      </c>
+      <c r="C41" s="7">
+        <v>0.05</v>
+      </c>
+      <c r="E41">
+        <v>209</v>
+      </c>
+      <c r="G41">
+        <v>186</v>
+      </c>
+      <c r="I41">
+        <v>186</v>
+      </c>
+      <c r="K41">
+        <v>178</v>
+      </c>
+      <c r="M41">
+        <v>183</v>
+      </c>
+      <c r="O41">
+        <v>193</v>
+      </c>
+      <c r="Q41">
+        <v>182</v>
+      </c>
+      <c r="S41">
+        <v>168</v>
+      </c>
+      <c r="U41">
+        <v>157</v>
+      </c>
+      <c r="W41">
+        <v>160</v>
+      </c>
+      <c r="Y41">
+        <v>152</v>
+      </c>
+      <c r="AA41">
+        <v>143</v>
+      </c>
+      <c r="AC41">
+        <v>139</v>
+      </c>
+      <c r="AE41">
+        <f t="shared" si="7"/>
+        <v>2236</v>
+      </c>
+      <c r="AF41" s="9">
+        <f t="shared" si="8"/>
+        <v>10.329999999999998</v>
+      </c>
+      <c r="AG41">
+        <v>11.64</v>
+      </c>
+      <c r="AH41">
+        <v>21.97</v>
+      </c>
+      <c r="AI41">
+        <f t="shared" si="9"/>
+        <v>2236</v>
+      </c>
+    </row>
+    <row r="42" spans="1:35">
+      <c r="B42" s="7">
+        <v>2</v>
+      </c>
+      <c r="C42" s="7">
+        <v>0.1</v>
+      </c>
+      <c r="E42">
+        <v>210</v>
+      </c>
+      <c r="G42">
+        <v>190</v>
+      </c>
+      <c r="I42">
+        <v>190</v>
+      </c>
+      <c r="K42">
+        <v>182</v>
+      </c>
+      <c r="M42">
+        <v>187</v>
+      </c>
+      <c r="O42">
+        <v>197</v>
+      </c>
+      <c r="Q42">
+        <v>186</v>
+      </c>
+      <c r="S42">
+        <v>173</v>
+      </c>
+      <c r="U42">
+        <v>162</v>
+      </c>
+      <c r="W42">
+        <v>166</v>
+      </c>
+      <c r="Y42">
+        <v>157</v>
+      </c>
+      <c r="AA42">
+        <v>145</v>
+      </c>
+      <c r="AC42">
+        <v>138</v>
+      </c>
+      <c r="AE42">
+        <f t="shared" si="7"/>
+        <v>2283</v>
+      </c>
+      <c r="AF42" s="9">
+        <f t="shared" si="8"/>
+        <v>9.5800000000000018</v>
+      </c>
+      <c r="AG42">
+        <v>4.3</v>
+      </c>
+      <c r="AH42">
+        <v>13.88</v>
+      </c>
+      <c r="AI42">
+        <f t="shared" si="9"/>
+        <v>2283</v>
+      </c>
+    </row>
+    <row r="43" spans="1:35">
+      <c r="A43" s="7"/>
+      <c r="B43" s="7"/>
+      <c r="C43" s="7"/>
+      <c r="D43" s="8"/>
+      <c r="AF43" s="9"/>
+    </row>
+    <row r="45" spans="1:35">
+      <c r="A45" s="1"/>
+    </row>
+    <row r="55" spans="32:32">
+      <c r="AF55" s="9"/>
+    </row>
+  </sheetData>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
+  <pageSetup orientation="portrait" horizontalDpi="4294967292" verticalDpi="4294967292"/>
   <extLst>
     <ext xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" uri="{64002731-A6B0-56B0-2670-7721B7C09600}">
       <mx:PLV Mode="0" OnePage="0" WScale="0"/>

</xml_diff>

<commit_message>
adding problem eos run data
</commit_message>
<xml_diff>
--- a/doc/ttsp2013/data/problem_4/problem_4_preconditioning.xlsx
+++ b/doc/ttsp2013/data/problem_4/problem_4_preconditioning.xlsx
@@ -4,12 +4,11 @@
   <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="24816"/>
   <workbookPr showInkAnnotation="0" autoCompressPictures="0"/>
   <bookViews>
-    <workbookView xWindow="52860" yWindow="4740" windowWidth="51200" windowHeight="28280" tabRatio="500"/>
+    <workbookView xWindow="57240" yWindow="5720" windowWidth="25600" windowHeight="16060" tabRatio="500"/>
   </bookViews>
   <sheets>
     <sheet name="Results" sheetId="1" r:id="rId1"/>
-    <sheet name="Jacobi" sheetId="5" r:id="rId2"/>
-    <sheet name="Case 1 Pstudy" sheetId="6" r:id="rId3"/>
+    <sheet name="Case 1 Pstudy" sheetId="6" r:id="rId2"/>
   </sheets>
   <calcPr calcId="140000" concurrentCalc="0"/>
   <extLst>
@@ -21,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="96" uniqueCount="69">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="108" uniqueCount="74">
   <si>
     <t>MCSA Preconditioning Analysis</t>
   </si>
@@ -62,9 +61,6 @@
     <t>CASE DEFINITIONS</t>
   </si>
   <si>
-    <t>Eigenvalue Iterations</t>
-  </si>
-  <si>
     <t>Eigenvalue Iters</t>
   </si>
   <si>
@@ -77,9 +73,6 @@
     <t>Total GMRES Iters</t>
   </si>
   <si>
-    <t>Setup Time (s)</t>
-  </si>
-  <si>
     <t>Solve Time (s)</t>
   </si>
   <si>
@@ -104,9 +97,6 @@
     <t>ARNOLDI-MCLS-MCSA-AINV</t>
   </si>
   <si>
-    <t>Parameter Studies for Block Jacobi Preconditioning</t>
-  </si>
-  <si>
     <t>Case 1</t>
   </si>
   <si>
@@ -116,9 +106,6 @@
     <t>Num Histories</t>
   </si>
   <si>
-    <t>Total MCSA Iterations</t>
-  </si>
-  <si>
     <t>Parameter Studies for Sparse Approximate Inverse Preconditioning</t>
   </si>
   <si>
@@ -228,12 +215,45 @@
   </si>
   <si>
     <t>Total MCSA Iters</t>
+  </si>
+  <si>
+    <t>Solve Fraction</t>
+  </si>
+  <si>
+    <t>Smooth Steps</t>
+  </si>
+  <si>
+    <t>Linear/Eigen</t>
+  </si>
+  <si>
+    <t>Other Time</t>
+  </si>
+  <si>
+    <t>ILUT Ratio</t>
+  </si>
+  <si>
+    <t>AMG Ratio</t>
+  </si>
+  <si>
+    <t>MGE Ratio</t>
+  </si>
+  <si>
+    <t>SOLVE TIME RATIO</t>
+  </si>
+  <si>
+    <t>TOTAL TIME RATIO</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <numFmts count="4">
+    <numFmt numFmtId="165" formatCode="#,##0.0000000000"/>
+    <numFmt numFmtId="166" formatCode="0.0000000000"/>
+    <numFmt numFmtId="167" formatCode="0.0"/>
+    <numFmt numFmtId="168" formatCode="0.000"/>
+  </numFmts>
   <fonts count="8" x14ac:knownFonts="1">
     <font>
       <sz val="12"/>
@@ -314,7 +334,7 @@
       <diagonal/>
     </border>
   </borders>
-  <cellStyleXfs count="159">
+  <cellStyleXfs count="185">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="5" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
@@ -474,8 +494,34 @@
     <xf numFmtId="0" fontId="5" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="5" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="13">
+  <cellXfs count="20">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1"/>
@@ -493,8 +539,15 @@
     <xf numFmtId="0" fontId="7" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="3" fontId="7" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
     <xf numFmtId="2" fontId="7" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
+    <xf numFmtId="165" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="166" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="166" fontId="1" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
+    <xf numFmtId="167" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="2" fontId="1" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
+    <xf numFmtId="168" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="168" fontId="1" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
   </cellXfs>
-  <cellStyles count="159">
+  <cellStyles count="185">
     <cellStyle name="Followed Hyperlink" xfId="2" builtinId="9" hidden="1"/>
     <cellStyle name="Followed Hyperlink" xfId="4" builtinId="9" hidden="1"/>
     <cellStyle name="Followed Hyperlink" xfId="6" builtinId="9" hidden="1"/>
@@ -574,6 +627,19 @@
     <cellStyle name="Followed Hyperlink" xfId="154" builtinId="9" hidden="1"/>
     <cellStyle name="Followed Hyperlink" xfId="156" builtinId="9" hidden="1"/>
     <cellStyle name="Followed Hyperlink" xfId="158" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="160" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="162" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="164" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="166" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="168" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="170" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="172" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="174" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="176" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="178" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="180" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="182" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="184" builtinId="9" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="1" builtinId="8" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="3" builtinId="8" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="5" builtinId="8" hidden="1"/>
@@ -653,6 +719,19 @@
     <cellStyle name="Hyperlink" xfId="153" builtinId="8" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="155" builtinId="8" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="157" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="159" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="161" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="163" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="165" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="167" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="169" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="171" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="173" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="175" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="177" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="179" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="181" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="183" builtinId="8" hidden="1"/>
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="0"/>
@@ -982,10 +1061,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:L49"/>
+  <dimension ref="A1:M69"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="P13" sqref="P13"/>
+      <selection activeCell="N28" sqref="N28"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0"/>
@@ -993,13 +1072,15 @@
     <col min="1" max="1" width="10" customWidth="1"/>
     <col min="2" max="2" width="15.83203125" bestFit="1" customWidth="1"/>
     <col min="3" max="3" width="14.83203125" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="11.5" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="14.83203125" customWidth="1"/>
     <col min="5" max="5" width="13.33203125" bestFit="1" customWidth="1"/>
     <col min="6" max="6" width="12.83203125" bestFit="1" customWidth="1"/>
     <col min="7" max="7" width="9.6640625" bestFit="1" customWidth="1"/>
-    <col min="8" max="8" width="19.5" bestFit="1" customWidth="1"/>
-    <col min="9" max="9" width="10.33203125" bestFit="1" customWidth="1"/>
-    <col min="12" max="12" width="13.6640625" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="10.83203125" bestFit="1" customWidth="1"/>
+    <col min="9" max="9" width="11.6640625" bestFit="1" customWidth="1"/>
+    <col min="10" max="10" width="9.33203125" bestFit="1" customWidth="1"/>
+    <col min="11" max="11" width="19.5" bestFit="1" customWidth="1"/>
+    <col min="12" max="12" width="13.1640625" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:12">
@@ -1049,10 +1130,10 @@
         <v>10</v>
       </c>
       <c r="K6" s="1" t="s">
-        <v>24</v>
+        <v>22</v>
       </c>
       <c r="L6" s="1" t="s">
-        <v>25</v>
+        <v>23</v>
       </c>
     </row>
     <row r="7" spans="1:12">
@@ -1309,7 +1390,7 @@
     </row>
     <row r="15" spans="1:12">
       <c r="A15" s="3" t="s">
-        <v>16</v>
+        <v>15</v>
       </c>
     </row>
     <row r="16" spans="1:12">
@@ -1317,247 +1398,1240 @@
         <v>11</v>
       </c>
       <c r="B16" s="1" t="s">
+        <v>16</v>
+      </c>
+      <c r="C16" s="1" t="s">
+        <v>13</v>
+      </c>
+      <c r="D16" s="1" t="s">
+        <v>14</v>
+      </c>
+      <c r="E16" s="1" t="s">
+        <v>65</v>
+      </c>
+      <c r="F16" s="1" t="s">
         <v>17</v>
       </c>
-      <c r="C16" s="1" t="s">
-        <v>14</v>
-      </c>
-      <c r="D16" s="1" t="s">
-        <v>15</v>
-      </c>
-      <c r="E16" s="1" t="s">
-        <v>19</v>
-      </c>
-      <c r="F16" s="1" t="s">
-        <v>20</v>
-      </c>
       <c r="G16" s="1" t="s">
-        <v>66</v>
-      </c>
-    </row>
-    <row r="17" spans="1:7">
+        <v>18</v>
+      </c>
+      <c r="H16" s="1" t="s">
+        <v>62</v>
+      </c>
+      <c r="I16" s="1" t="s">
+        <v>67</v>
+      </c>
+    </row>
+    <row r="17" spans="1:9">
       <c r="A17" s="6">
         <v>1</v>
       </c>
-    </row>
-    <row r="18" spans="1:7">
+      <c r="B17">
+        <f>35*12 +34</f>
+        <v>454</v>
+      </c>
+      <c r="C17">
+        <v>13</v>
+      </c>
+      <c r="D17" s="13">
+        <v>1.1241137236000001</v>
+      </c>
+      <c r="E17">
+        <v>0.93286000000000002</v>
+      </c>
+      <c r="F17" s="18">
+        <f>E17*G17</f>
+        <v>4.2617709100000001</v>
+      </c>
+      <c r="G17" s="18">
+        <v>4.5685000000000002</v>
+      </c>
+      <c r="H17">
+        <f>B17</f>
+        <v>454</v>
+      </c>
+      <c r="I17" s="16">
+        <f>B17/C17</f>
+        <v>34.92307692307692</v>
+      </c>
+    </row>
+    <row r="18" spans="1:9">
       <c r="A18" s="6">
         <v>2</v>
       </c>
-    </row>
-    <row r="19" spans="1:7">
+      <c r="B18">
+        <f>37*20+2*36+39+40+40+40</f>
+        <v>971</v>
+      </c>
+      <c r="C18">
+        <v>26</v>
+      </c>
+      <c r="D18" s="13">
+        <v>1.1217344600000001</v>
+      </c>
+      <c r="E18">
+        <v>0.95123000000000002</v>
+      </c>
+      <c r="F18" s="18">
+        <f t="shared" ref="F18:F22" si="4">E18*G18</f>
+        <v>11.73437328</v>
+      </c>
+      <c r="G18" s="18">
+        <v>12.336</v>
+      </c>
+      <c r="H18">
+        <f t="shared" ref="H18:H22" si="5">B18</f>
+        <v>971</v>
+      </c>
+      <c r="I18" s="16">
+        <f t="shared" ref="I18:I22" si="6">B18/C18</f>
+        <v>37.346153846153847</v>
+      </c>
+    </row>
+    <row r="19" spans="1:9">
       <c r="A19" s="6">
         <v>3</v>
       </c>
-    </row>
-    <row r="20" spans="1:7">
+      <c r="B19">
+        <f>41*7+42*2+41*5+42*4+41+42*3+44+44+43+44</f>
+        <v>1086</v>
+      </c>
+      <c r="C19">
+        <v>26</v>
+      </c>
+      <c r="D19" s="13">
+        <v>1.1216287766999999</v>
+      </c>
+      <c r="E19">
+        <v>0.95077999999999996</v>
+      </c>
+      <c r="F19" s="18">
+        <f t="shared" si="4"/>
+        <v>12.45426722</v>
+      </c>
+      <c r="G19" s="18">
+        <v>13.099</v>
+      </c>
+      <c r="H19">
+        <f t="shared" si="5"/>
+        <v>1086</v>
+      </c>
+      <c r="I19" s="16">
+        <f t="shared" si="6"/>
+        <v>41.769230769230766</v>
+      </c>
+    </row>
+    <row r="20" spans="1:9">
       <c r="A20" s="6">
         <v>4</v>
       </c>
-    </row>
-    <row r="21" spans="1:7">
+      <c r="B20">
+        <f>46*16+47+46*5+49*4</f>
+        <v>1209</v>
+      </c>
+      <c r="C20">
+        <v>26</v>
+      </c>
+      <c r="D20" s="13">
+        <v>1.1215954205000001</v>
+      </c>
+      <c r="E20">
+        <v>0.95526999999999995</v>
+      </c>
+      <c r="F20" s="18">
+        <f t="shared" si="4"/>
+        <v>18.142487840000001</v>
+      </c>
+      <c r="G20" s="18">
+        <v>18.992000000000001</v>
+      </c>
+      <c r="H20">
+        <f t="shared" si="5"/>
+        <v>1209</v>
+      </c>
+      <c r="I20" s="16">
+        <f t="shared" si="6"/>
+        <v>46.5</v>
+      </c>
+    </row>
+    <row r="21" spans="1:9">
       <c r="A21" s="6">
         <v>5</v>
       </c>
-    </row>
-    <row r="22" spans="1:7">
+      <c r="B21">
+        <f>55+56*21+59*3+60</f>
+        <v>1468</v>
+      </c>
+      <c r="C21">
+        <v>26</v>
+      </c>
+      <c r="D21" s="13">
+        <v>1.1215878639000001</v>
+      </c>
+      <c r="E21">
+        <v>0.96220000000000006</v>
+      </c>
+      <c r="F21" s="18">
+        <f t="shared" si="4"/>
+        <v>27.160019400000003</v>
+      </c>
+      <c r="G21" s="18">
+        <v>28.227</v>
+      </c>
+      <c r="H21">
+        <f t="shared" si="5"/>
+        <v>1468</v>
+      </c>
+      <c r="I21" s="16">
+        <f t="shared" si="6"/>
+        <v>56.46153846153846</v>
+      </c>
+    </row>
+    <row r="22" spans="1:9">
       <c r="A22" s="6">
         <v>6</v>
       </c>
-    </row>
-    <row r="24" spans="1:7">
+      <c r="B22">
+        <f>78*4+79*3+78*3+79+78+78+79*3+78+79*5+82+84+84+83</f>
+        <v>2061</v>
+      </c>
+      <c r="C22">
+        <v>26</v>
+      </c>
+      <c r="D22" s="13">
+        <v>1.1215846503</v>
+      </c>
+      <c r="E22">
+        <v>0.97236999999999996</v>
+      </c>
+      <c r="F22" s="18">
+        <f t="shared" si="4"/>
+        <v>44.216581009999999</v>
+      </c>
+      <c r="G22" s="18">
+        <v>45.472999999999999</v>
+      </c>
+      <c r="H22">
+        <f t="shared" si="5"/>
+        <v>2061</v>
+      </c>
+      <c r="I22" s="16">
+        <f t="shared" si="6"/>
+        <v>79.269230769230774</v>
+      </c>
+    </row>
+    <row r="23" spans="1:9">
+      <c r="F23" s="18"/>
+      <c r="G23" s="18"/>
+    </row>
+    <row r="24" spans="1:9">
       <c r="A24" s="3" t="s">
-        <v>21</v>
-      </c>
-    </row>
-    <row r="25" spans="1:7">
+        <v>19</v>
+      </c>
+      <c r="F24" s="18"/>
+      <c r="G24" s="18"/>
+    </row>
+    <row r="25" spans="1:9">
       <c r="A25" s="1" t="s">
         <v>11</v>
       </c>
       <c r="B25" s="1" t="s">
+        <v>16</v>
+      </c>
+      <c r="C25" s="1" t="s">
+        <v>13</v>
+      </c>
+      <c r="D25" s="1" t="s">
+        <v>14</v>
+      </c>
+      <c r="E25" s="1" t="s">
+        <v>65</v>
+      </c>
+      <c r="F25" s="19" t="s">
         <v>17</v>
       </c>
-      <c r="C25" s="1" t="s">
-        <v>14</v>
-      </c>
-      <c r="D25" s="1" t="s">
-        <v>15</v>
-      </c>
-      <c r="E25" s="1" t="s">
-        <v>19</v>
-      </c>
-      <c r="F25" s="1" t="s">
-        <v>20</v>
-      </c>
-      <c r="G25" s="1" t="s">
-        <v>66</v>
-      </c>
-    </row>
-    <row r="26" spans="1:7">
+      <c r="G25" s="19" t="s">
+        <v>18</v>
+      </c>
+      <c r="H25" s="1" t="s">
+        <v>62</v>
+      </c>
+      <c r="I25" s="1" t="s">
+        <v>67</v>
+      </c>
+    </row>
+    <row r="26" spans="1:9">
       <c r="A26" s="6">
         <v>1</v>
       </c>
-    </row>
-    <row r="27" spans="1:7">
+      <c r="B26">
+        <f>13*16-5</f>
+        <v>203</v>
+      </c>
+      <c r="C26">
+        <v>13</v>
+      </c>
+      <c r="D26" s="14">
+        <v>1.1241137634</v>
+      </c>
+      <c r="E26">
+        <v>0.97023999999999999</v>
+      </c>
+      <c r="F26" s="18">
+        <f>E26*G26</f>
+        <v>9.9226444800000007</v>
+      </c>
+      <c r="G26" s="18">
+        <v>10.227</v>
+      </c>
+      <c r="H26">
+        <f>B26</f>
+        <v>203</v>
+      </c>
+      <c r="I26" s="16">
+        <f>B26/C26</f>
+        <v>15.615384615384615</v>
+      </c>
+    </row>
+    <row r="27" spans="1:9">
       <c r="A27" s="6">
         <v>2</v>
       </c>
-    </row>
-    <row r="28" spans="1:7">
+      <c r="B27">
+        <f>20+20+21+22*19+23*4</f>
+        <v>571</v>
+      </c>
+      <c r="C27">
+        <v>26</v>
+      </c>
+      <c r="D27" s="14">
+        <v>1.1217344214</v>
+      </c>
+      <c r="E27">
+        <v>0.98648999999999998</v>
+      </c>
+      <c r="F27" s="18">
+        <f t="shared" ref="F27:F31" si="7">E27*G27</f>
+        <v>44.027048700000002</v>
+      </c>
+      <c r="G27" s="18">
+        <v>44.63</v>
+      </c>
+      <c r="H27">
+        <f t="shared" ref="H27:H31" si="8">B27</f>
+        <v>571</v>
+      </c>
+      <c r="I27" s="16">
+        <f t="shared" ref="I27:I31" si="9">B27/C27</f>
+        <v>21.96153846153846</v>
+      </c>
+    </row>
+    <row r="28" spans="1:9">
       <c r="A28" s="6">
         <v>3</v>
       </c>
-    </row>
-    <row r="29" spans="1:7">
+      <c r="B28">
+        <f>22+22+23*5+24*2+23+24+23*4+24*2+23*5+24*4</f>
+        <v>605</v>
+      </c>
+      <c r="C28">
+        <v>26</v>
+      </c>
+      <c r="D28" s="14">
+        <v>1.1216288163999999</v>
+      </c>
+      <c r="E28">
+        <v>0.98626999999999998</v>
+      </c>
+      <c r="F28" s="18">
+        <f t="shared" si="7"/>
+        <v>46.137710599999998</v>
+      </c>
+      <c r="G28" s="18">
+        <v>46.78</v>
+      </c>
+      <c r="H28">
+        <f t="shared" si="8"/>
+        <v>605</v>
+      </c>
+      <c r="I28" s="16">
+        <f t="shared" si="9"/>
+        <v>23.26923076923077</v>
+      </c>
+    </row>
+    <row r="29" spans="1:9">
       <c r="A29" s="6">
         <v>4</v>
       </c>
-    </row>
-    <row r="30" spans="1:7">
+      <c r="B29">
+        <f>22*3+23*19+24*4</f>
+        <v>599</v>
+      </c>
+      <c r="C29">
+        <v>26</v>
+      </c>
+      <c r="D29" s="14">
+        <v>1.1215954267999999</v>
+      </c>
+      <c r="E29">
+        <v>0.98616999999999999</v>
+      </c>
+      <c r="F29" s="18">
+        <f t="shared" si="7"/>
+        <v>60.454193339999996</v>
+      </c>
+      <c r="G29" s="18">
+        <v>61.302</v>
+      </c>
+      <c r="H29">
+        <f t="shared" si="8"/>
+        <v>599</v>
+      </c>
+      <c r="I29" s="16">
+        <f t="shared" si="9"/>
+        <v>23.03846153846154</v>
+      </c>
+    </row>
+    <row r="30" spans="1:9">
       <c r="A30" s="6">
         <v>5</v>
       </c>
-    </row>
-    <row r="31" spans="1:7">
+      <c r="B30">
+        <f>21*2+22*20+23*4</f>
+        <v>574</v>
+      </c>
+      <c r="C30">
+        <v>26</v>
+      </c>
+      <c r="D30" s="14">
+        <v>1.1215878622</v>
+      </c>
+      <c r="E30">
+        <v>0.98448000000000002</v>
+      </c>
+      <c r="F30" s="18">
+        <f t="shared" si="7"/>
+        <v>70.287934079999999</v>
+      </c>
+      <c r="G30" s="18">
+        <v>71.396000000000001</v>
+      </c>
+      <c r="H30">
+        <f t="shared" si="8"/>
+        <v>574</v>
+      </c>
+      <c r="I30" s="16">
+        <f t="shared" si="9"/>
+        <v>22.076923076923077</v>
+      </c>
+    </row>
+    <row r="31" spans="1:9">
       <c r="A31" s="6">
         <v>6</v>
       </c>
-    </row>
-    <row r="33" spans="1:8">
+      <c r="B31">
+        <f>24*22+25*4</f>
+        <v>628</v>
+      </c>
+      <c r="C31">
+        <v>26</v>
+      </c>
+      <c r="D31" s="14">
+        <v>1.1215846811000001</v>
+      </c>
+      <c r="E31">
+        <v>0.98601000000000005</v>
+      </c>
+      <c r="F31" s="18">
+        <f t="shared" si="7"/>
+        <v>84.777139800000015</v>
+      </c>
+      <c r="G31" s="18">
+        <v>85.98</v>
+      </c>
+      <c r="H31">
+        <f t="shared" si="8"/>
+        <v>628</v>
+      </c>
+      <c r="I31" s="16">
+        <f t="shared" si="9"/>
+        <v>24.153846153846153</v>
+      </c>
+    </row>
+    <row r="32" spans="1:9">
+      <c r="D32" s="14"/>
+      <c r="F32" s="18"/>
+      <c r="G32" s="18"/>
+    </row>
+    <row r="33" spans="1:13">
       <c r="A33" s="3" t="s">
-        <v>22</v>
-      </c>
-    </row>
-    <row r="34" spans="1:8">
+        <v>20</v>
+      </c>
+      <c r="D33" s="14"/>
+      <c r="F33" s="18"/>
+      <c r="G33" s="18"/>
+    </row>
+    <row r="34" spans="1:13">
       <c r="A34" s="1" t="s">
         <v>11</v>
       </c>
       <c r="B34" s="1" t="s">
+        <v>16</v>
+      </c>
+      <c r="C34" s="1" t="s">
+        <v>13</v>
+      </c>
+      <c r="D34" s="15" t="s">
+        <v>14</v>
+      </c>
+      <c r="E34" s="1" t="s">
+        <v>65</v>
+      </c>
+      <c r="F34" s="19" t="s">
         <v>17</v>
       </c>
-      <c r="C34" s="1" t="s">
-        <v>14</v>
-      </c>
-      <c r="D34" s="1" t="s">
-        <v>15</v>
-      </c>
-      <c r="E34" s="1" t="s">
-        <v>19</v>
-      </c>
-      <c r="F34" s="1" t="s">
-        <v>20</v>
-      </c>
-      <c r="G34" s="1" t="s">
-        <v>66</v>
-      </c>
-    </row>
-    <row r="35" spans="1:8">
+      <c r="G34" s="19" t="s">
+        <v>18</v>
+      </c>
+      <c r="H34" s="1" t="s">
+        <v>62</v>
+      </c>
+      <c r="I34" s="1" t="s">
+        <v>67</v>
+      </c>
+    </row>
+    <row r="35" spans="1:13">
       <c r="A35" s="6">
         <v>1</v>
       </c>
-    </row>
-    <row r="36" spans="1:8">
+      <c r="B35">
+        <f>13*13-3</f>
+        <v>166</v>
+      </c>
+      <c r="C35">
+        <v>13</v>
+      </c>
+      <c r="D35" s="14">
+        <v>1.1241137896</v>
+      </c>
+      <c r="E35">
+        <v>0.90800999999999998</v>
+      </c>
+      <c r="F35" s="18">
+        <f>E35*G35</f>
+        <v>7.386933753000001</v>
+      </c>
+      <c r="G35" s="18">
+        <v>8.1353000000000009</v>
+      </c>
+      <c r="H35">
+        <f>B35</f>
+        <v>166</v>
+      </c>
+      <c r="I35" s="16">
+        <f>B35/C35</f>
+        <v>12.76923076923077</v>
+      </c>
+    </row>
+    <row r="36" spans="1:13">
       <c r="A36" s="6">
         <v>2</v>
       </c>
-    </row>
-    <row r="37" spans="1:8">
+      <c r="B36">
+        <f>22*13+4*14</f>
+        <v>342</v>
+      </c>
+      <c r="C36">
+        <v>26</v>
+      </c>
+      <c r="D36" s="14">
+        <v>1.1217344198999999</v>
+      </c>
+      <c r="E36">
+        <v>0.94874999999999998</v>
+      </c>
+      <c r="F36" s="18">
+        <f t="shared" ref="F36:F40" si="10">E36*G36</f>
+        <v>26.007134999999998</v>
+      </c>
+      <c r="G36" s="18">
+        <v>27.411999999999999</v>
+      </c>
+      <c r="H36">
+        <f t="shared" ref="H36:H40" si="11">B36</f>
+        <v>342</v>
+      </c>
+      <c r="I36" s="16">
+        <f t="shared" ref="I36:I40" si="12">B36/C36</f>
+        <v>13.153846153846153</v>
+      </c>
+    </row>
+    <row r="37" spans="1:13">
       <c r="A37" s="6">
         <v>3</v>
       </c>
-    </row>
-    <row r="38" spans="1:8">
+      <c r="B37">
+        <f>22*14+4*15</f>
+        <v>368</v>
+      </c>
+      <c r="C37">
+        <v>26</v>
+      </c>
+      <c r="D37" s="14">
+        <v>1.1216288096</v>
+      </c>
+      <c r="E37">
+        <v>0.94979000000000002</v>
+      </c>
+      <c r="F37" s="18">
+        <f t="shared" si="10"/>
+        <v>27.76141191</v>
+      </c>
+      <c r="G37" s="18">
+        <v>29.228999999999999</v>
+      </c>
+      <c r="H37">
+        <f t="shared" si="11"/>
+        <v>368</v>
+      </c>
+      <c r="I37" s="16">
+        <f t="shared" si="12"/>
+        <v>14.153846153846153</v>
+      </c>
+    </row>
+    <row r="38" spans="1:13">
       <c r="A38" s="6">
         <v>4</v>
       </c>
-    </row>
-    <row r="39" spans="1:8">
+      <c r="B38">
+        <f>22*15+4*16</f>
+        <v>394</v>
+      </c>
+      <c r="C38">
+        <v>26</v>
+      </c>
+      <c r="D38" s="14">
+        <v>1.1215954239999999</v>
+      </c>
+      <c r="E38">
+        <v>0.95282</v>
+      </c>
+      <c r="F38" s="18">
+        <f t="shared" si="10"/>
+        <v>39.051327700000002</v>
+      </c>
+      <c r="G38" s="18">
+        <v>40.984999999999999</v>
+      </c>
+      <c r="H38">
+        <f t="shared" si="11"/>
+        <v>394</v>
+      </c>
+      <c r="I38" s="16">
+        <f t="shared" si="12"/>
+        <v>15.153846153846153</v>
+      </c>
+    </row>
+    <row r="39" spans="1:13">
       <c r="A39" s="6">
         <v>5</v>
       </c>
-    </row>
-    <row r="40" spans="1:8">
+      <c r="B39">
+        <f>17*22+4*18</f>
+        <v>446</v>
+      </c>
+      <c r="C39">
+        <v>26</v>
+      </c>
+      <c r="D39" s="14">
+        <v>1.1215878505000001</v>
+      </c>
+      <c r="E39">
+        <v>0.95179999999999998</v>
+      </c>
+      <c r="F39" s="18">
+        <f t="shared" si="10"/>
+        <v>50.965082799999998</v>
+      </c>
+      <c r="G39" s="18">
+        <v>53.545999999999999</v>
+      </c>
+      <c r="H39">
+        <f t="shared" si="11"/>
+        <v>446</v>
+      </c>
+      <c r="I39" s="16">
+        <f t="shared" si="12"/>
+        <v>17.153846153846153</v>
+      </c>
+    </row>
+    <row r="40" spans="1:13">
       <c r="A40" s="6">
         <v>6</v>
       </c>
-    </row>
-    <row r="42" spans="1:8">
+      <c r="B40">
+        <f>4*25+5*26+8*25+2*26+3*25+4*27</f>
+        <v>665</v>
+      </c>
+      <c r="C40">
+        <v>26</v>
+      </c>
+      <c r="D40" s="14">
+        <v>1.1215846624000001</v>
+      </c>
+      <c r="E40">
+        <v>0.96862999999999999</v>
+      </c>
+      <c r="F40" s="18">
+        <f t="shared" si="10"/>
+        <v>78.081264300000001</v>
+      </c>
+      <c r="G40" s="18">
+        <v>80.61</v>
+      </c>
+      <c r="H40">
+        <f t="shared" si="11"/>
+        <v>665</v>
+      </c>
+      <c r="I40" s="16">
+        <f t="shared" si="12"/>
+        <v>25.576923076923077</v>
+      </c>
+    </row>
+    <row r="41" spans="1:13">
+      <c r="D41" s="14"/>
+      <c r="F41" s="18"/>
+      <c r="G41" s="18"/>
+    </row>
+    <row r="42" spans="1:13">
       <c r="A42" s="3" t="s">
-        <v>26</v>
-      </c>
-    </row>
-    <row r="43" spans="1:8">
+        <v>24</v>
+      </c>
+      <c r="D42" s="14"/>
+      <c r="F42" s="18"/>
+      <c r="G42" s="18"/>
+    </row>
+    <row r="43" spans="1:13">
       <c r="A43" s="1" t="s">
         <v>11</v>
       </c>
       <c r="B43" s="1" t="s">
+        <v>64</v>
+      </c>
+      <c r="C43" s="1" t="s">
+        <v>13</v>
+      </c>
+      <c r="D43" s="15" t="s">
+        <v>14</v>
+      </c>
+      <c r="E43" s="1" t="s">
+        <v>65</v>
+      </c>
+      <c r="F43" s="19" t="s">
+        <v>17</v>
+      </c>
+      <c r="G43" s="19" t="s">
+        <v>18</v>
+      </c>
+      <c r="H43" s="1" t="s">
+        <v>62</v>
+      </c>
+      <c r="I43" s="1" t="s">
+        <v>67</v>
+      </c>
+      <c r="J43" s="1" t="s">
+        <v>61</v>
+      </c>
+      <c r="K43" s="1" t="s">
+        <v>21</v>
+      </c>
+      <c r="L43" s="1" t="s">
+        <v>66</v>
+      </c>
+      <c r="M43" s="1" t="s">
         <v>68</v>
       </c>
-      <c r="C43" s="1" t="s">
-        <v>14</v>
-      </c>
-      <c r="D43" s="1" t="s">
-        <v>15</v>
-      </c>
-      <c r="E43" s="1" t="s">
-        <v>19</v>
-      </c>
-      <c r="F43" s="1" t="s">
-        <v>20</v>
-      </c>
-      <c r="G43" s="1" t="s">
-        <v>66</v>
-      </c>
-      <c r="H43" s="1" t="s">
-        <v>23</v>
-      </c>
-    </row>
-    <row r="44" spans="1:8">
+    </row>
+    <row r="44" spans="1:13">
       <c r="A44" s="6">
         <v>1</v>
       </c>
-      <c r="H44" s="4">
+      <c r="B44">
+        <f>19*2+18*2+19+18+19*2+18+17+18+19+18</f>
+        <v>239</v>
+      </c>
+      <c r="C44">
+        <v>13</v>
+      </c>
+      <c r="D44" s="14">
+        <v>1.1241137821</v>
+      </c>
+      <c r="E44">
+        <v>0.98675000000000002</v>
+      </c>
+      <c r="F44" s="18">
+        <v>14.26</v>
+      </c>
+      <c r="G44" s="18">
+        <v>30.875</v>
+      </c>
+      <c r="H44">
+        <f>B44*(L44+1)</f>
+        <v>956</v>
+      </c>
+      <c r="I44" s="16">
+        <f>B44/C44</f>
+        <v>18.384615384615383</v>
+      </c>
+      <c r="J44" s="9">
+        <v>11.65</v>
+      </c>
+      <c r="K44" s="4">
         <v>75000</v>
       </c>
-    </row>
-    <row r="45" spans="1:8">
+      <c r="L44">
+        <v>3</v>
+      </c>
+      <c r="M44" s="18">
+        <f>G44-F44-J44</f>
+        <v>4.9650000000000016</v>
+      </c>
+    </row>
+    <row r="45" spans="1:13">
       <c r="A45" s="6">
         <v>2</v>
       </c>
-      <c r="H45" s="4">
+      <c r="B45">
+        <f>26*2+28+27+28+26*3+25*2+27*2+26*2+29+26+27+26*2+25+27*2+30+28+27*2</f>
+        <v>694</v>
+      </c>
+      <c r="C45">
+        <f>26</f>
+        <v>26</v>
+      </c>
+      <c r="D45" s="14">
+        <v>1.1217344145999999</v>
+      </c>
+      <c r="E45">
+        <v>0.99351</v>
+      </c>
+      <c r="F45" s="18">
+        <v>68.021600000000007</v>
+      </c>
+      <c r="G45" s="18">
+        <v>111.9</v>
+      </c>
+      <c r="H45">
+        <f t="shared" ref="H45:H49" si="13">B45*(L45+1)</f>
+        <v>2776</v>
+      </c>
+      <c r="I45" s="16">
+        <f t="shared" ref="I45:I49" si="14">B45/C45</f>
+        <v>26.692307692307693</v>
+      </c>
+      <c r="J45" s="9">
+        <v>27.9</v>
+      </c>
+      <c r="K45" s="4">
         <v>168000</v>
       </c>
-    </row>
-    <row r="46" spans="1:8">
+      <c r="L45">
+        <v>3</v>
+      </c>
+      <c r="M45" s="18">
+        <f t="shared" ref="M45:M49" si="15">G45-F45-J45</f>
+        <v>15.978400000000001</v>
+      </c>
+    </row>
+    <row r="46" spans="1:13">
       <c r="A46" s="6">
         <v>3</v>
       </c>
-      <c r="H46" s="4">
+      <c r="B46">
+        <v>770</v>
+      </c>
+      <c r="C46">
+        <v>26</v>
+      </c>
+      <c r="D46" s="14">
+        <v>1.1216288072</v>
+      </c>
+      <c r="E46">
+        <v>0.99424000000000001</v>
+      </c>
+      <c r="F46" s="18">
+        <v>82.78</v>
+      </c>
+      <c r="G46" s="18">
+        <v>129.36000000000001</v>
+      </c>
+      <c r="H46">
+        <f t="shared" si="13"/>
+        <v>3080</v>
+      </c>
+      <c r="I46" s="16">
+        <f t="shared" si="14"/>
+        <v>29.615384615384617</v>
+      </c>
+      <c r="J46" s="9">
+        <v>28.1</v>
+      </c>
+      <c r="K46" s="4">
         <v>288000</v>
       </c>
-    </row>
-    <row r="47" spans="1:8">
+      <c r="L46">
+        <v>3</v>
+      </c>
+      <c r="M46" s="18">
+        <f t="shared" si="15"/>
+        <v>18.480000000000011</v>
+      </c>
+    </row>
+    <row r="47" spans="1:13">
       <c r="A47" s="6">
         <v>4</v>
       </c>
-      <c r="H47" s="4">
+      <c r="B47">
+        <f>27+29+27+29+25+26+24+26+26+26+26+25+26+29+27+26+25+26+25+28+24+24+27+26+29+29+27</f>
+        <v>714</v>
+      </c>
+      <c r="C47">
+        <v>26</v>
+      </c>
+      <c r="D47" s="14">
+        <v>1.1215954284</v>
+      </c>
+      <c r="E47">
+        <v>0.99399000000000004</v>
+      </c>
+      <c r="F47" s="18">
+        <v>100.6215</v>
+      </c>
+      <c r="G47" s="18">
+        <v>164.25</v>
+      </c>
+      <c r="H47">
+        <f t="shared" si="13"/>
+        <v>2856</v>
+      </c>
+      <c r="I47" s="16">
+        <f t="shared" si="14"/>
+        <v>27.46153846153846</v>
+      </c>
+      <c r="J47" s="9">
+        <v>35.880000000000003</v>
+      </c>
+      <c r="K47" s="4">
         <v>646000</v>
       </c>
-    </row>
-    <row r="48" spans="1:8">
+      <c r="L47">
+        <v>3</v>
+      </c>
+      <c r="M47" s="18">
+        <f t="shared" si="15"/>
+        <v>27.7485</v>
+      </c>
+    </row>
+    <row r="48" spans="1:13">
       <c r="A48" s="6">
         <v>5</v>
       </c>
-      <c r="H48" s="4">
+      <c r="D48" s="14"/>
+      <c r="G48" s="18"/>
+      <c r="H48">
+        <f t="shared" si="13"/>
+        <v>0</v>
+      </c>
+      <c r="I48" s="16" t="e">
+        <f t="shared" si="14"/>
+        <v>#DIV/0!</v>
+      </c>
+      <c r="J48" s="9"/>
+      <c r="K48" s="4">
         <v>1245000</v>
       </c>
-    </row>
-    <row r="49" spans="1:8">
+      <c r="L48">
+        <v>3</v>
+      </c>
+      <c r="M48" s="18">
+        <f t="shared" si="15"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="49" spans="1:13">
       <c r="A49" s="6">
         <v>6</v>
       </c>
-      <c r="H49" s="4">
+      <c r="D49" s="14"/>
+      <c r="G49" s="18"/>
+      <c r="H49">
+        <f t="shared" si="13"/>
+        <v>0</v>
+      </c>
+      <c r="I49" s="16" t="e">
+        <f t="shared" si="14"/>
+        <v>#DIV/0!</v>
+      </c>
+      <c r="J49" s="9"/>
+      <c r="K49" s="4">
         <v>2440000</v>
+      </c>
+      <c r="L49">
+        <v>3</v>
+      </c>
+      <c r="M49" s="18">
+        <f t="shared" si="15"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="53" spans="1:13">
+      <c r="A53" s="3" t="s">
+        <v>72</v>
+      </c>
+    </row>
+    <row r="54" spans="1:13">
+      <c r="A54" s="1" t="s">
+        <v>11</v>
+      </c>
+      <c r="B54" s="1" t="s">
+        <v>69</v>
+      </c>
+      <c r="C54" s="1" t="s">
+        <v>70</v>
+      </c>
+      <c r="D54" s="1" t="s">
+        <v>71</v>
+      </c>
+    </row>
+    <row r="55" spans="1:13">
+      <c r="A55" s="6">
+        <v>1</v>
+      </c>
+      <c r="B55" s="9">
+        <f>F44/F17</f>
+        <v>3.3460268750109798</v>
+      </c>
+      <c r="C55" s="9">
+        <f>F44/F26</f>
+        <v>1.437116892451638</v>
+      </c>
+      <c r="D55" s="9">
+        <f>F44/F35</f>
+        <v>1.9304356146701183</v>
+      </c>
+    </row>
+    <row r="56" spans="1:13">
+      <c r="A56" s="6">
+        <v>2</v>
+      </c>
+      <c r="B56" s="9">
+        <f t="shared" ref="B56:B60" si="16">F45/F18</f>
+        <v>5.7967816752459749</v>
+      </c>
+      <c r="C56" s="9">
+        <f t="shared" ref="C56:C60" si="17">F45/F27</f>
+        <v>1.5449956789858594</v>
+      </c>
+      <c r="D56" s="9">
+        <f t="shared" ref="D56:D60" si="18">F45/F36</f>
+        <v>2.6154976317076066</v>
+      </c>
+    </row>
+    <row r="57" spans="1:13">
+      <c r="A57" s="6">
+        <v>3</v>
+      </c>
+      <c r="B57" s="9">
+        <f t="shared" si="16"/>
+        <v>6.6467178307420323</v>
+      </c>
+      <c r="C57" s="9">
+        <f t="shared" si="17"/>
+        <v>1.7941939234410127</v>
+      </c>
+      <c r="D57" s="9">
+        <f t="shared" si="18"/>
+        <v>2.9818368124922938</v>
+      </c>
+    </row>
+    <row r="58" spans="1:13">
+      <c r="A58" s="6">
+        <v>4</v>
+      </c>
+      <c r="B58" s="9">
+        <f t="shared" si="16"/>
+        <v>5.5461798231526327</v>
+      </c>
+      <c r="C58" s="9">
+        <f t="shared" si="17"/>
+        <v>1.6644254838385708</v>
+      </c>
+      <c r="D58" s="9">
+        <f t="shared" si="18"/>
+        <v>2.5766473491757873</v>
+      </c>
+    </row>
+    <row r="59" spans="1:13">
+      <c r="A59" s="6">
+        <v>5</v>
+      </c>
+      <c r="B59" s="9">
+        <f t="shared" si="16"/>
+        <v>0</v>
+      </c>
+      <c r="C59" s="9">
+        <f t="shared" si="17"/>
+        <v>0</v>
+      </c>
+      <c r="D59" s="9">
+        <f t="shared" si="18"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="60" spans="1:13">
+      <c r="A60" s="6">
+        <v>6</v>
+      </c>
+      <c r="B60" s="9">
+        <f t="shared" si="16"/>
+        <v>0</v>
+      </c>
+      <c r="C60" s="9">
+        <f t="shared" si="17"/>
+        <v>0</v>
+      </c>
+      <c r="D60" s="9">
+        <f t="shared" si="18"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="61" spans="1:13">
+      <c r="B61" s="9"/>
+      <c r="C61" s="9"/>
+      <c r="D61" s="9"/>
+    </row>
+    <row r="62" spans="1:13">
+      <c r="A62" t="s">
+        <v>73</v>
+      </c>
+      <c r="B62" s="9"/>
+      <c r="C62" s="9"/>
+      <c r="D62" s="9"/>
+    </row>
+    <row r="63" spans="1:13">
+      <c r="A63" s="1" t="s">
+        <v>11</v>
+      </c>
+      <c r="B63" s="17" t="s">
+        <v>69</v>
+      </c>
+      <c r="C63" s="17" t="s">
+        <v>70</v>
+      </c>
+      <c r="D63" s="17" t="s">
+        <v>71</v>
+      </c>
+    </row>
+    <row r="64" spans="1:13">
+      <c r="A64" s="6">
+        <v>1</v>
+      </c>
+      <c r="B64" s="9">
+        <f>G44/G17</f>
+        <v>6.7582357447739954</v>
+      </c>
+      <c r="C64" s="9">
+        <f>G44/G26</f>
+        <v>3.0189693947394152</v>
+      </c>
+      <c r="D64" s="9">
+        <f>G44/G35</f>
+        <v>3.79518886826546</v>
+      </c>
+    </row>
+    <row r="65" spans="1:4">
+      <c r="A65" s="6">
+        <v>2</v>
+      </c>
+      <c r="B65" s="9">
+        <f>G45/G18</f>
+        <v>9.0710116731517516</v>
+      </c>
+      <c r="C65" s="9">
+        <f>G45/G27</f>
+        <v>2.5072820972440062</v>
+      </c>
+      <c r="D65" s="9">
+        <f>G45/G36</f>
+        <v>4.0821538012549254</v>
+      </c>
+    </row>
+    <row r="66" spans="1:4">
+      <c r="A66" s="6">
+        <v>3</v>
+      </c>
+      <c r="B66" s="9">
+        <f>G46/G19</f>
+        <v>9.8755630200778697</v>
+      </c>
+      <c r="C66" s="9">
+        <f>G46/G28</f>
+        <v>2.765284309533989</v>
+      </c>
+      <c r="D66" s="9">
+        <f>G46/G37</f>
+        <v>4.4257415580416719</v>
+      </c>
+    </row>
+    <row r="67" spans="1:4">
+      <c r="A67" s="6">
+        <v>4</v>
+      </c>
+      <c r="B67" s="9">
+        <f>G47/G20</f>
+        <v>8.6483782645324343</v>
+      </c>
+      <c r="C67" s="9">
+        <f>G47/G29</f>
+        <v>2.6793579328570032</v>
+      </c>
+      <c r="D67" s="9">
+        <f>G47/G38</f>
+        <v>4.007563742832744</v>
+      </c>
+    </row>
+    <row r="68" spans="1:4">
+      <c r="A68" s="6">
+        <v>5</v>
+      </c>
+      <c r="B68" s="9">
+        <f>G48/G21</f>
+        <v>0</v>
+      </c>
+      <c r="C68" s="9">
+        <f>G48/G30</f>
+        <v>0</v>
+      </c>
+      <c r="D68" s="9">
+        <f>G48/G39</f>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="69" spans="1:4">
+      <c r="A69" s="6">
+        <v>6</v>
+      </c>
+      <c r="B69" s="9">
+        <f>G49/G22</f>
+        <v>0</v>
+      </c>
+      <c r="C69" s="9">
+        <f>G49/G31</f>
+        <v>0</v>
+      </c>
+      <c r="D69" s="9">
+        <f>G49/G40</f>
+        <v>0</v>
       </c>
     </row>
   </sheetData>
@@ -1573,77 +2647,10 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:G5"/>
-  <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="F45" sqref="F45"/>
-    </sheetView>
-  </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="12.33203125" defaultRowHeight="15" x14ac:dyDescent="0"/>
-  <cols>
-    <col min="2" max="2" width="13" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="19.33203125" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="18.83203125" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="13.1640625" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="12.83203125" bestFit="1" customWidth="1"/>
-    <col min="7" max="7" width="12.5" bestFit="1" customWidth="1"/>
-  </cols>
-  <sheetData>
-    <row r="1" spans="1:7">
-      <c r="A1" s="1" t="s">
-        <v>27</v>
-      </c>
-    </row>
-    <row r="3" spans="1:7">
-      <c r="A3" s="3" t="s">
-        <v>28</v>
-      </c>
-    </row>
-    <row r="4" spans="1:7">
-      <c r="A4" s="1" t="s">
-        <v>29</v>
-      </c>
-      <c r="B4" s="1" t="s">
-        <v>30</v>
-      </c>
-      <c r="C4" s="1" t="s">
-        <v>31</v>
-      </c>
-      <c r="D4" s="1" t="s">
-        <v>13</v>
-      </c>
-      <c r="E4" s="1" t="s">
-        <v>18</v>
-      </c>
-      <c r="F4" s="1" t="s">
-        <v>19</v>
-      </c>
-      <c r="G4" s="1" t="s">
-        <v>20</v>
-      </c>
-    </row>
-    <row r="5" spans="1:7">
-      <c r="A5">
-        <v>1</v>
-      </c>
-    </row>
-  </sheetData>
-  <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
-  <pageSetup orientation="portrait" horizontalDpi="4294967292" verticalDpi="4294967292"/>
-  <extLst>
-    <ext xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" uri="{64002731-A6B0-56B0-2670-7721B7C09600}">
-      <mx:PLV Mode="0" OnePage="0" WScale="0"/>
-    </ext>
-  </extLst>
-</worksheet>
-</file>
-
-<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:AI55"/>
   <sheetViews>
     <sheetView topLeftCell="A2" workbookViewId="0">
-      <selection activeCell="A24" sqref="A24:AI24"/>
+      <selection activeCell="C52" sqref="C52"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="13.33203125" defaultRowHeight="15" x14ac:dyDescent="0"/>
@@ -1661,122 +2668,122 @@
   <sheetData>
     <row r="1" spans="1:35">
       <c r="A1" s="1" t="s">
-        <v>32</v>
+        <v>28</v>
       </c>
     </row>
     <row r="3" spans="1:35">
       <c r="A3" s="3" t="s">
-        <v>28</v>
+        <v>25</v>
       </c>
       <c r="B3" t="s">
-        <v>35</v>
+        <v>31</v>
       </c>
     </row>
     <row r="4" spans="1:35">
       <c r="A4" s="1" t="s">
+        <v>26</v>
+      </c>
+      <c r="B4" s="1" t="s">
+        <v>30</v>
+      </c>
+      <c r="C4" s="1" t="s">
         <v>29</v>
       </c>
-      <c r="B4" s="1" t="s">
+      <c r="D4" s="1" t="s">
+        <v>27</v>
+      </c>
+      <c r="E4" s="1" t="s">
+        <v>32</v>
+      </c>
+      <c r="F4" s="1" t="s">
+        <v>33</v>
+      </c>
+      <c r="G4" s="1" t="s">
         <v>34</v>
       </c>
-      <c r="C4" s="1" t="s">
-        <v>33</v>
-      </c>
-      <c r="D4" s="1" t="s">
-        <v>30</v>
-      </c>
-      <c r="E4" s="1" t="s">
+      <c r="H4" s="1" t="s">
+        <v>35</v>
+      </c>
+      <c r="I4" s="1" t="s">
         <v>36</v>
       </c>
-      <c r="F4" s="1" t="s">
+      <c r="J4" s="1" t="s">
         <v>37</v>
       </c>
-      <c r="G4" s="1" t="s">
+      <c r="K4" s="1" t="s">
         <v>38</v>
       </c>
-      <c r="H4" s="1" t="s">
+      <c r="L4" s="1" t="s">
         <v>39</v>
       </c>
-      <c r="I4" s="1" t="s">
+      <c r="M4" s="1" t="s">
         <v>40</v>
       </c>
-      <c r="J4" s="1" t="s">
+      <c r="N4" s="1" t="s">
         <v>41</v>
       </c>
-      <c r="K4" s="1" t="s">
+      <c r="O4" s="1" t="s">
         <v>42</v>
       </c>
-      <c r="L4" s="1" t="s">
+      <c r="P4" s="1" t="s">
         <v>43</v>
       </c>
-      <c r="M4" s="1" t="s">
+      <c r="Q4" s="1" t="s">
         <v>44</v>
       </c>
-      <c r="N4" s="1" t="s">
+      <c r="R4" s="1" t="s">
         <v>45</v>
       </c>
-      <c r="O4" s="1" t="s">
+      <c r="S4" s="1" t="s">
         <v>46</v>
       </c>
-      <c r="P4" s="1" t="s">
+      <c r="T4" s="1" t="s">
         <v>47</v>
       </c>
-      <c r="Q4" s="1" t="s">
+      <c r="U4" s="1" t="s">
         <v>48</v>
       </c>
-      <c r="R4" s="1" t="s">
+      <c r="V4" s="1" t="s">
         <v>49</v>
       </c>
-      <c r="S4" s="1" t="s">
+      <c r="W4" s="1" t="s">
         <v>50</v>
       </c>
-      <c r="T4" s="1" t="s">
+      <c r="X4" s="1" t="s">
         <v>51</v>
       </c>
-      <c r="U4" s="1" t="s">
+      <c r="Y4" s="1" t="s">
         <v>52</v>
       </c>
-      <c r="V4" s="1" t="s">
+      <c r="Z4" s="1" t="s">
         <v>53</v>
       </c>
-      <c r="W4" s="1" t="s">
+      <c r="AA4" s="1" t="s">
         <v>54</v>
       </c>
-      <c r="X4" s="1" t="s">
+      <c r="AB4" s="1" t="s">
         <v>55</v>
       </c>
-      <c r="Y4" s="1" t="s">
+      <c r="AC4" s="1" t="s">
         <v>56</v>
       </c>
-      <c r="Z4" s="1" t="s">
+      <c r="AD4" s="1" t="s">
         <v>57</v>
       </c>
-      <c r="AA4" s="1" t="s">
+      <c r="AE4" s="1" t="s">
         <v>58</v>
       </c>
-      <c r="AB4" s="1" t="s">
+      <c r="AF4" s="1" t="s">
+        <v>60</v>
+      </c>
+      <c r="AG4" s="1" t="s">
+        <v>61</v>
+      </c>
+      <c r="AH4" s="1" t="s">
         <v>59</v>
       </c>
-      <c r="AC4" s="1" t="s">
-        <v>60</v>
-      </c>
-      <c r="AD4" s="1" t="s">
-        <v>61</v>
-      </c>
-      <c r="AE4" s="1" t="s">
+      <c r="AI4" s="1" t="s">
         <v>62</v>
-      </c>
-      <c r="AF4" s="1" t="s">
-        <v>64</v>
-      </c>
-      <c r="AG4" s="1" t="s">
-        <v>65</v>
-      </c>
-      <c r="AH4" s="1" t="s">
-        <v>63</v>
-      </c>
-      <c r="AI4" s="1" t="s">
-        <v>66</v>
       </c>
     </row>
     <row r="5" spans="1:35">
@@ -4123,7 +5130,7 @@
     </row>
     <row r="36" spans="1:35">
       <c r="A36" s="1" t="s">
-        <v>67</v>
+        <v>63</v>
       </c>
       <c r="B36" s="7">
         <v>1</v>

</xml_diff>

<commit_message>
adding c5g7 data for ttsp paper
</commit_message>
<xml_diff>
--- a/doc/ttsp2013/data/problem_4/problem_4_preconditioning.xlsx
+++ b/doc/ttsp2013/data/problem_4/problem_4_preconditioning.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="24816"/>
   <workbookPr showInkAnnotation="0" autoCompressPictures="0"/>
   <bookViews>
-    <workbookView xWindow="56500" yWindow="5980" windowWidth="28800" windowHeight="17480" tabRatio="500" activeTab="1"/>
+    <workbookView xWindow="56500" yWindow="5980" windowWidth="30920" windowHeight="17440" tabRatio="500" activeTab="1"/>
   </bookViews>
   <sheets>
     <sheet name="25K Results" sheetId="1" r:id="rId1"/>
@@ -433,8 +433,22 @@
       <diagonal/>
     </border>
   </borders>
-  <cellStyleXfs count="347">
+  <cellStyleXfs count="361">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="5" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
@@ -833,7 +847,7 @@
     </xf>
     <xf numFmtId="2" fontId="3" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
   </cellXfs>
-  <cellStyles count="347">
+  <cellStyles count="361">
     <cellStyle name="Followed Hyperlink" xfId="2" builtinId="9" hidden="1"/>
     <cellStyle name="Followed Hyperlink" xfId="4" builtinId="9" hidden="1"/>
     <cellStyle name="Followed Hyperlink" xfId="6" builtinId="9" hidden="1"/>
@@ -1007,6 +1021,13 @@
     <cellStyle name="Followed Hyperlink" xfId="342" builtinId="9" hidden="1"/>
     <cellStyle name="Followed Hyperlink" xfId="344" builtinId="9" hidden="1"/>
     <cellStyle name="Followed Hyperlink" xfId="346" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="348" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="350" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="352" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="354" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="356" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="358" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="360" builtinId="9" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="1" builtinId="8" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="3" builtinId="8" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="5" builtinId="8" hidden="1"/>
@@ -1180,6 +1201,13 @@
     <cellStyle name="Hyperlink" xfId="341" builtinId="8" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="343" builtinId="8" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="345" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="347" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="349" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="351" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="353" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="355" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="357" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="359" builtinId="8" hidden="1"/>
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="0"/>
@@ -3801,8 +3829,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:R76"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A23" workbookViewId="0">
-      <selection activeCell="M77" sqref="M77"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="M29" sqref="M29"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0"/>
@@ -3825,22 +3853,22 @@
     <col min="18" max="18" width="15.5" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:15">
+    <row r="1" spans="1:12">
       <c r="A1" s="2" t="s">
         <v>0</v>
       </c>
     </row>
-    <row r="3" spans="1:15">
+    <row r="3" spans="1:12">
       <c r="A3" s="3" t="s">
         <v>1</v>
       </c>
     </row>
-    <row r="5" spans="1:15">
+    <row r="5" spans="1:12">
       <c r="A5" s="3" t="s">
         <v>12</v>
       </c>
     </row>
-    <row r="6" spans="1:15">
+    <row r="6" spans="1:12">
       <c r="A6" s="1" t="s">
         <v>11</v>
       </c>
@@ -3877,14 +3905,8 @@
       <c r="L6" s="1" t="s">
         <v>23</v>
       </c>
-      <c r="N6">
-        <v>1</v>
-      </c>
-      <c r="O6">
-        <v>257</v>
-      </c>
-    </row>
-    <row r="7" spans="1:15">
+    </row>
+    <row r="7" spans="1:12">
       <c r="A7" s="5">
         <v>2</v>
       </c>
@@ -3925,14 +3947,8 @@
         <f t="shared" ref="L7:L11" si="2">I7/J7</f>
         <v>13086.28125</v>
       </c>
-      <c r="N7">
-        <v>2</v>
-      </c>
-      <c r="O7">
-        <v>254</v>
-      </c>
-    </row>
-    <row r="8" spans="1:15">
+    </row>
+    <row r="8" spans="1:12">
       <c r="A8" s="5">
         <v>3</v>
       </c>
@@ -3973,14 +3989,8 @@
         <f t="shared" si="2"/>
         <v>11216.8125</v>
       </c>
-      <c r="N8">
-        <v>3</v>
-      </c>
-      <c r="O8">
-        <v>230</v>
-      </c>
-    </row>
-    <row r="9" spans="1:15">
+    </row>
+    <row r="9" spans="1:12">
       <c r="A9" s="5">
         <v>4</v>
       </c>
@@ -4021,14 +4031,8 @@
         <f t="shared" si="2"/>
         <v>12618.9140625</v>
       </c>
-      <c r="N9">
-        <v>4</v>
-      </c>
-      <c r="O9">
-        <v>237</v>
-      </c>
-    </row>
-    <row r="10" spans="1:15">
+    </row>
+    <row r="10" spans="1:12">
       <c r="A10" s="5">
         <v>5</v>
       </c>
@@ -4069,14 +4073,8 @@
         <f t="shared" si="2"/>
         <v>12543.532258064517</v>
       </c>
-      <c r="N10">
-        <v>5</v>
-      </c>
-      <c r="O10">
-        <v>228</v>
-      </c>
-    </row>
-    <row r="11" spans="1:15">
+    </row>
+    <row r="11" spans="1:12">
       <c r="A11" s="5">
         <v>6</v>
       </c>
@@ -4117,49 +4115,13 @@
         <f t="shared" si="2"/>
         <v>12503.987704918032</v>
       </c>
-      <c r="N11">
-        <v>6</v>
-      </c>
-      <c r="O11">
-        <v>232</v>
-      </c>
-    </row>
-    <row r="12" spans="1:15">
-      <c r="N12">
-        <v>7</v>
-      </c>
-      <c r="O12">
-        <v>222</v>
-      </c>
-    </row>
-    <row r="13" spans="1:15">
-      <c r="N13">
-        <v>8</v>
-      </c>
-      <c r="O13">
-        <v>222</v>
-      </c>
-    </row>
-    <row r="14" spans="1:15">
-      <c r="N14">
-        <v>9</v>
-      </c>
-      <c r="O14">
-        <v>242</v>
-      </c>
-    </row>
-    <row r="15" spans="1:15">
+    </row>
+    <row r="15" spans="1:12">
       <c r="A15" s="3" t="s">
         <v>15</v>
       </c>
-      <c r="N15">
-        <v>10</v>
-      </c>
-      <c r="O15">
-        <v>239</v>
-      </c>
-    </row>
-    <row r="16" spans="1:15">
+    </row>
+    <row r="16" spans="1:12">
       <c r="A16" s="1" t="s">
         <v>11</v>
       </c>
@@ -4187,14 +4149,8 @@
       <c r="I16" s="1" t="s">
         <v>67</v>
       </c>
-      <c r="N16">
-        <v>11</v>
-      </c>
-      <c r="O16">
-        <v>233</v>
-      </c>
-    </row>
-    <row r="17" spans="1:15">
+    </row>
+    <row r="17" spans="1:9">
       <c r="A17" s="6">
         <v>2</v>
       </c>
@@ -4225,14 +4181,8 @@
         <f>B17/C17</f>
         <v>41.807692307692307</v>
       </c>
-      <c r="N17">
-        <v>12</v>
-      </c>
-      <c r="O17">
-        <v>227</v>
-      </c>
-    </row>
-    <row r="18" spans="1:15">
+    </row>
+    <row r="18" spans="1:9">
       <c r="A18" s="6">
         <v>3</v>
       </c>
@@ -4262,14 +4212,8 @@
         <f>B18/C18</f>
         <v>46.346153846153847</v>
       </c>
-      <c r="N18">
-        <v>13</v>
-      </c>
-      <c r="O18">
-        <v>225</v>
-      </c>
-    </row>
-    <row r="19" spans="1:15">
+    </row>
+    <row r="19" spans="1:9">
       <c r="A19" s="6">
         <v>4</v>
       </c>
@@ -4299,14 +4243,8 @@
         <f>B19/C19</f>
         <v>55.884615384615387</v>
       </c>
-      <c r="N19">
-        <v>14</v>
-      </c>
-      <c r="O19">
-        <v>225</v>
-      </c>
-    </row>
-    <row r="20" spans="1:15">
+    </row>
+    <row r="20" spans="1:9">
       <c r="A20" s="6">
         <v>5</v>
       </c>
@@ -4336,14 +4274,8 @@
         <f>B20/C20</f>
         <v>64.42307692307692</v>
       </c>
-      <c r="N20">
-        <v>15</v>
-      </c>
-      <c r="O20">
-        <v>227</v>
-      </c>
-    </row>
-    <row r="21" spans="1:15">
+    </row>
+    <row r="21" spans="1:9">
       <c r="A21" s="6">
         <v>6</v>
       </c>
@@ -4373,52 +4305,28 @@
         <f>B21/C21</f>
         <v>85.34615384615384</v>
       </c>
-      <c r="N21">
-        <v>16</v>
-      </c>
-      <c r="O21">
-        <v>237</v>
-      </c>
-    </row>
-    <row r="22" spans="1:15">
+    </row>
+    <row r="22" spans="1:9">
       <c r="D22" s="13"/>
       <c r="E22" s="18"/>
       <c r="G22" s="18"/>
       <c r="H22" s="4"/>
       <c r="I22" s="16"/>
-      <c r="N22">
-        <v>17</v>
-      </c>
-      <c r="O22">
-        <v>232</v>
-      </c>
-    </row>
-    <row r="23" spans="1:15">
+    </row>
+    <row r="23" spans="1:9">
       <c r="E23" s="18"/>
       <c r="G23" s="18"/>
       <c r="H23" s="4"/>
-      <c r="N23">
-        <v>18</v>
-      </c>
-      <c r="O23">
-        <v>223</v>
-      </c>
-    </row>
-    <row r="24" spans="1:15">
+    </row>
+    <row r="24" spans="1:9">
       <c r="A24" s="3" t="s">
         <v>19</v>
       </c>
       <c r="E24" s="18"/>
       <c r="G24" s="18"/>
       <c r="H24" s="4"/>
-      <c r="N24">
-        <v>19</v>
-      </c>
-      <c r="O24">
-        <v>221</v>
-      </c>
-    </row>
-    <row r="25" spans="1:15">
+    </row>
+    <row r="25" spans="1:9">
       <c r="A25" s="1" t="s">
         <v>11</v>
       </c>
@@ -4446,14 +4354,8 @@
       <c r="I25" s="1" t="s">
         <v>67</v>
       </c>
-      <c r="N25">
-        <v>20</v>
-      </c>
-      <c r="O25">
-        <v>223</v>
-      </c>
-    </row>
-    <row r="26" spans="1:15">
+    </row>
+    <row r="26" spans="1:9">
       <c r="A26" s="6">
         <v>2</v>
       </c>
@@ -4483,14 +4385,8 @@
         <f>B26/C26</f>
         <v>22.96153846153846</v>
       </c>
-      <c r="N26">
-        <v>21</v>
-      </c>
-      <c r="O26">
-        <v>230</v>
-      </c>
-    </row>
-    <row r="27" spans="1:15">
+    </row>
+    <row r="27" spans="1:9">
       <c r="A27" s="6">
         <v>3</v>
       </c>
@@ -4520,14 +4416,8 @@
         <f>B27/C27</f>
         <v>24.5</v>
       </c>
-      <c r="N27">
-        <v>22</v>
-      </c>
-      <c r="O27">
-        <v>227</v>
-      </c>
-    </row>
-    <row r="28" spans="1:15">
+    </row>
+    <row r="28" spans="1:9">
       <c r="A28" s="6">
         <v>4</v>
       </c>
@@ -4557,14 +4447,8 @@
         <f>B28/C28</f>
         <v>25</v>
       </c>
-      <c r="N28">
-        <v>23</v>
-      </c>
-      <c r="O28">
-        <v>235</v>
-      </c>
-    </row>
-    <row r="29" spans="1:15">
+    </row>
+    <row r="29" spans="1:9">
       <c r="A29" s="6">
         <v>5</v>
       </c>
@@ -4594,14 +4478,8 @@
         <f>B29/C29</f>
         <v>24.076923076923077</v>
       </c>
-      <c r="N29">
-        <v>24</v>
-      </c>
-      <c r="O29">
-        <v>230</v>
-      </c>
-    </row>
-    <row r="30" spans="1:15">
+    </row>
+    <row r="30" spans="1:9">
       <c r="A30" s="6">
         <v>6</v>
       </c>
@@ -4631,35 +4509,19 @@
         <f>B30/C30</f>
         <v>25.96153846153846</v>
       </c>
-      <c r="N30">
-        <v>25</v>
-      </c>
-      <c r="O30">
-        <v>227</v>
-      </c>
-    </row>
-    <row r="31" spans="1:15">
+    </row>
+    <row r="31" spans="1:9">
       <c r="D31" s="14"/>
       <c r="E31" s="18"/>
       <c r="G31" s="18"/>
       <c r="H31" s="4"/>
       <c r="I31" s="16"/>
-      <c r="N31">
-        <v>26</v>
-      </c>
-      <c r="O31">
-        <v>231</v>
-      </c>
-    </row>
-    <row r="32" spans="1:15">
+    </row>
+    <row r="32" spans="1:9">
       <c r="D32" s="14"/>
       <c r="E32" s="18"/>
       <c r="G32" s="18"/>
       <c r="H32" s="4"/>
-      <c r="O32">
-        <f>SUM(O6:O31)</f>
-        <v>6016</v>
-      </c>
     </row>
     <row r="33" spans="1:16">
       <c r="A33" s="3" t="s">
@@ -5994,7 +5856,7 @@
   <dimension ref="A1:AI55"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="A17" sqref="A17:XFD17"/>
+      <selection activeCell="AE4" sqref="AE4:AI4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="13.33203125" defaultRowHeight="15" x14ac:dyDescent="0"/>

</xml_diff>

<commit_message>
updates to ttsp data
</commit_message>
<xml_diff>
--- a/doc/ttsp2013/data/problem_4/problem_4_preconditioning.xlsx
+++ b/doc/ttsp2013/data/problem_4/problem_4_preconditioning.xlsx
@@ -1,16 +1,17 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="24816"/>
+  <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="25317"/>
   <workbookPr showInkAnnotation="0" autoCompressPictures="0"/>
   <bookViews>
-    <workbookView xWindow="56500" yWindow="5980" windowWidth="30920" windowHeight="17440" tabRatio="500" activeTab="1"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="51200" windowHeight="28280" tabRatio="500" activeTab="4"/>
   </bookViews>
   <sheets>
     <sheet name="25K Results" sheetId="1" r:id="rId1"/>
     <sheet name="12.5K Results" sheetId="8" r:id="rId2"/>
     <sheet name="MCSA Case 1 Pstudy" sheetId="6" r:id="rId3"/>
     <sheet name="Threshold Study" sheetId="7" r:id="rId4"/>
+    <sheet name="Sufficient Condition" sheetId="9" r:id="rId5"/>
   </sheets>
   <calcPr calcId="140000" concurrentCalc="0"/>
   <extLst>
@@ -22,7 +23,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="316" uniqueCount="99">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="364" uniqueCount="109">
   <si>
     <t>MCSA Preconditioning Analysis</t>
   </si>
@@ -320,19 +321,50 @@
   <si>
     <t>Setup Time</t>
   </si>
+  <si>
+    <t>case id</t>
+  </si>
+  <si>
+    <t>rho(H)</t>
+  </si>
+  <si>
+    <t>rho(H*)</t>
+  </si>
+  <si>
+    <t>rho(H+)</t>
+  </si>
+  <si>
+    <t>Case 2</t>
+  </si>
+  <si>
+    <t>MCSA Iters</t>
+  </si>
+  <si>
+    <t>Filter</t>
+  </si>
+  <si>
+    <t>Case 3</t>
+  </si>
+  <si>
+    <t>SPAINV Parameter Study</t>
+  </si>
+  <si>
+    <t>0.0 Composite Operator Threshold</t>
+  </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <numFmts count="5">
+  <numFmts count="6">
     <numFmt numFmtId="164" formatCode="#,##0.0000000000"/>
     <numFmt numFmtId="165" formatCode="0.0000000000"/>
     <numFmt numFmtId="166" formatCode="0.0"/>
     <numFmt numFmtId="167" formatCode="0.000"/>
     <numFmt numFmtId="168" formatCode="0.0E+00"/>
+    <numFmt numFmtId="169" formatCode="0.0000000"/>
   </numFmts>
-  <fonts count="11" x14ac:knownFonts="1">
+  <fonts count="12" x14ac:knownFonts="1">
     <font>
       <sz val="12"/>
       <color theme="1"/>
@@ -415,6 +447,12 @@
       <name val="Calibri"/>
       <scheme val="minor"/>
     </font>
+    <font>
+      <sz val="8"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
   </fonts>
   <fills count="2">
     <fill>
@@ -433,7 +471,7 @@
       <diagonal/>
     </border>
   </borders>
-  <cellStyleXfs count="361">
+  <cellStyleXfs count="455">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="5" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
@@ -795,8 +833,102 @@
     <xf numFmtId="0" fontId="5" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="5" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="35">
+  <cellXfs count="39">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1"/>
@@ -846,8 +978,12 @@
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="2" fontId="3" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
+    <xf numFmtId="11" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="168" fontId="6" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
+    <xf numFmtId="1" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="169" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
   </cellXfs>
-  <cellStyles count="361">
+  <cellStyles count="455">
     <cellStyle name="Followed Hyperlink" xfId="2" builtinId="9" hidden="1"/>
     <cellStyle name="Followed Hyperlink" xfId="4" builtinId="9" hidden="1"/>
     <cellStyle name="Followed Hyperlink" xfId="6" builtinId="9" hidden="1"/>
@@ -1028,6 +1164,53 @@
     <cellStyle name="Followed Hyperlink" xfId="356" builtinId="9" hidden="1"/>
     <cellStyle name="Followed Hyperlink" xfId="358" builtinId="9" hidden="1"/>
     <cellStyle name="Followed Hyperlink" xfId="360" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="362" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="364" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="366" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="368" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="370" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="372" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="374" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="376" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="378" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="380" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="382" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="384" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="386" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="388" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="390" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="392" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="394" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="396" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="398" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="400" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="402" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="404" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="406" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="408" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="410" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="412" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="414" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="416" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="418" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="420" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="422" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="424" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="426" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="428" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="430" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="432" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="434" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="436" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="438" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="440" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="442" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="444" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="446" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="448" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="450" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="452" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="454" builtinId="9" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="1" builtinId="8" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="3" builtinId="8" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="5" builtinId="8" hidden="1"/>
@@ -1208,11 +1391,705 @@
     <cellStyle name="Hyperlink" xfId="355" builtinId="8" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="357" builtinId="8" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="359" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="361" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="363" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="365" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="367" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="369" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="371" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="373" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="375" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="377" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="379" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="381" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="383" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="385" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="387" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="389" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="391" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="393" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="395" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="397" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="399" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="401" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="403" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="405" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="407" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="409" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="411" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="413" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="415" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="417" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="419" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="421" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="423" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="425" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="427" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="429" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="431" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="433" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="435" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="437" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="439" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="441" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="443" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="445" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="447" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="449" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="451" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="453" builtinId="8" hidden="1"/>
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="0"/>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium9" defaultPivotStyle="PivotStyleMedium4"/>
 </styleSheet>
+</file>
+
+<file path=xl/charts/chart1.xml><?xml version="1.0" encoding="utf-8"?>
+<c:chartSpace xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+  <c:date1904 val="0"/>
+  <c:lang val="en-US"/>
+  <c:roundedCorners val="0"/>
+  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+    <mc:Choice xmlns:c14="http://schemas.microsoft.com/office/drawing/2007/8/2/chart" Requires="c14">
+      <c14:style val="118"/>
+    </mc:Choice>
+    <mc:Fallback>
+      <c:style val="18"/>
+    </mc:Fallback>
+  </mc:AlternateContent>
+  <c:chart>
+    <c:title>
+      <c:tx>
+        <c:rich>
+          <a:bodyPr/>
+          <a:lstStyle/>
+          <a:p>
+            <a:pPr>
+              <a:defRPr/>
+            </a:pPr>
+            <a:r>
+              <a:rPr lang="en-US"/>
+              <a:t>SPN SPAINV</a:t>
+            </a:r>
+            <a:r>
+              <a:rPr lang="en-US" baseline="0"/>
+              <a:t> Preconditioning - Problem 4</a:t>
+            </a:r>
+            <a:endParaRPr lang="en-US"/>
+          </a:p>
+        </c:rich>
+      </c:tx>
+      <c:layout/>
+      <c:overlay val="0"/>
+    </c:title>
+    <c:autoTitleDeleted val="0"/>
+    <c:plotArea>
+      <c:layout/>
+      <c:scatterChart>
+        <c:scatterStyle val="lineMarker"/>
+        <c:varyColors val="0"/>
+        <c:ser>
+          <c:idx val="0"/>
+          <c:order val="0"/>
+          <c:tx>
+            <c:v>H</c:v>
+          </c:tx>
+          <c:spPr>
+            <a:ln>
+              <a:solidFill>
+                <a:schemeClr val="tx1"/>
+              </a:solidFill>
+              <a:prstDash val="dash"/>
+            </a:ln>
+          </c:spPr>
+          <c:marker>
+            <c:spPr>
+              <a:noFill/>
+              <a:ln>
+                <a:solidFill>
+                  <a:schemeClr val="tx1"/>
+                </a:solidFill>
+              </a:ln>
+            </c:spPr>
+          </c:marker>
+          <c:xVal>
+            <c:numRef>
+              <c:f>'Sufficient Condition'!$A$32:$A$37</c:f>
+              <c:numCache>
+                <c:formatCode>0.0E+00</c:formatCode>
+                <c:ptCount val="6"/>
+                <c:pt idx="0">
+                  <c:v>1.0E-5</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>0.0001</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>0.001</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>0.01</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>0.1</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>0.5</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:xVal>
+          <c:yVal>
+            <c:numRef>
+              <c:f>'Sufficient Condition'!$B$32:$B$37</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="6"/>
+                <c:pt idx="0">
+                  <c:v>0.926873</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>0.925587</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>0.9235366</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>0.9071089</c:v>
+                </c:pt>
+                <c:pt idx="4" formatCode="0.00E+00">
+                  <c:v>0.059</c:v>
+                </c:pt>
+                <c:pt idx="5" formatCode="0.00E+00">
+                  <c:v>0.059</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:yVal>
+          <c:smooth val="0"/>
+        </c:ser>
+        <c:ser>
+          <c:idx val="1"/>
+          <c:order val="1"/>
+          <c:tx>
+            <c:v>H*</c:v>
+          </c:tx>
+          <c:spPr>
+            <a:ln>
+              <a:solidFill>
+                <a:schemeClr val="tx1"/>
+              </a:solidFill>
+            </a:ln>
+          </c:spPr>
+          <c:marker>
+            <c:spPr>
+              <a:solidFill>
+                <a:schemeClr val="tx1"/>
+              </a:solidFill>
+              <a:ln>
+                <a:solidFill>
+                  <a:schemeClr val="tx1"/>
+                </a:solidFill>
+              </a:ln>
+            </c:spPr>
+          </c:marker>
+          <c:xVal>
+            <c:numRef>
+              <c:f>'Sufficient Condition'!$A$32:$A$37</c:f>
+              <c:numCache>
+                <c:formatCode>0.0E+00</c:formatCode>
+                <c:ptCount val="6"/>
+                <c:pt idx="0">
+                  <c:v>1.0E-5</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>0.0001</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>0.001</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>0.01</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>0.1</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>0.5</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:xVal>
+          <c:yVal>
+            <c:numRef>
+              <c:f>'Sufficient Condition'!$D$32:$D$37</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="6"/>
+                <c:pt idx="0">
+                  <c:v>1.17702</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>1.173943</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>1.156509</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>0.8622272</c:v>
+                </c:pt>
+                <c:pt idx="4" formatCode="0.00E+00">
+                  <c:v>0.00369</c:v>
+                </c:pt>
+                <c:pt idx="5" formatCode="0.00E+00">
+                  <c:v>0.00348</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:yVal>
+          <c:smooth val="0"/>
+        </c:ser>
+        <c:ser>
+          <c:idx val="2"/>
+          <c:order val="2"/>
+          <c:tx>
+            <c:v>H+</c:v>
+          </c:tx>
+          <c:spPr>
+            <a:ln w="28575" cmpd="sng">
+              <a:solidFill>
+                <a:schemeClr val="tx1"/>
+              </a:solidFill>
+              <a:prstDash val="sysDot"/>
+            </a:ln>
+          </c:spPr>
+          <c:marker>
+            <c:symbol val="square"/>
+            <c:size val="11"/>
+            <c:spPr>
+              <a:noFill/>
+              <a:ln w="38100" cmpd="sng">
+                <a:solidFill>
+                  <a:schemeClr val="tx1"/>
+                </a:solidFill>
+                <a:prstDash val="solid"/>
+              </a:ln>
+            </c:spPr>
+          </c:marker>
+          <c:xVal>
+            <c:numRef>
+              <c:f>'Sufficient Condition'!$A$32:$A$37</c:f>
+              <c:numCache>
+                <c:formatCode>0.0E+00</c:formatCode>
+                <c:ptCount val="6"/>
+                <c:pt idx="0">
+                  <c:v>1.0E-5</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>0.0001</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>0.001</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>0.01</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>0.1</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>0.5</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:xVal>
+          <c:yVal>
+            <c:numRef>
+              <c:f>'Sufficient Condition'!$C$32:$C$37</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="6"/>
+                <c:pt idx="0">
+                  <c:v>0.926873</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>0.9255867</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>0.9235366</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>0.9071089</c:v>
+                </c:pt>
+                <c:pt idx="4" formatCode="0.00E+00">
+                  <c:v>0.059</c:v>
+                </c:pt>
+                <c:pt idx="5" formatCode="0.00E+00">
+                  <c:v>0.059</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:yVal>
+          <c:smooth val="0"/>
+        </c:ser>
+        <c:dLbls>
+          <c:showLegendKey val="0"/>
+          <c:showVal val="0"/>
+          <c:showCatName val="0"/>
+          <c:showSerName val="0"/>
+          <c:showPercent val="0"/>
+          <c:showBubbleSize val="0"/>
+        </c:dLbls>
+        <c:axId val="2132256520"/>
+        <c:axId val="2132262008"/>
+      </c:scatterChart>
+      <c:valAx>
+        <c:axId val="2132256520"/>
+        <c:scaling>
+          <c:logBase val="10.0"/>
+          <c:orientation val="minMax"/>
+          <c:min val="1.0E-5"/>
+        </c:scaling>
+        <c:delete val="0"/>
+        <c:axPos val="b"/>
+        <c:title>
+          <c:tx>
+            <c:rich>
+              <a:bodyPr/>
+              <a:lstStyle/>
+              <a:p>
+                <a:pPr>
+                  <a:defRPr sz="1600"/>
+                </a:pPr>
+                <a:r>
+                  <a:rPr lang="en-US" sz="1600"/>
+                  <a:t>Composit</a:t>
+                </a:r>
+                <a:r>
+                  <a:rPr lang="en-US" sz="1600" baseline="0"/>
+                  <a:t>e Operator Threshold</a:t>
+                </a:r>
+                <a:endParaRPr lang="en-US" sz="1600"/>
+              </a:p>
+            </c:rich>
+          </c:tx>
+          <c:layout/>
+          <c:overlay val="0"/>
+        </c:title>
+        <c:numFmt formatCode="0.0E+00" sourceLinked="1"/>
+        <c:majorTickMark val="out"/>
+        <c:minorTickMark val="none"/>
+        <c:tickLblPos val="nextTo"/>
+        <c:txPr>
+          <a:bodyPr/>
+          <a:lstStyle/>
+          <a:p>
+            <a:pPr>
+              <a:defRPr sz="1600"/>
+            </a:pPr>
+            <a:endParaRPr lang="en-US"/>
+          </a:p>
+        </c:txPr>
+        <c:crossAx val="2132262008"/>
+        <c:crosses val="autoZero"/>
+        <c:crossBetween val="midCat"/>
+      </c:valAx>
+      <c:valAx>
+        <c:axId val="2132262008"/>
+        <c:scaling>
+          <c:orientation val="minMax"/>
+          <c:max val="1.2"/>
+        </c:scaling>
+        <c:delete val="0"/>
+        <c:axPos val="l"/>
+        <c:majorGridlines/>
+        <c:title>
+          <c:tx>
+            <c:rich>
+              <a:bodyPr rot="-5400000" vert="horz"/>
+              <a:lstStyle/>
+              <a:p>
+                <a:pPr>
+                  <a:defRPr sz="1600"/>
+                </a:pPr>
+                <a:r>
+                  <a:rPr lang="en-US" sz="1600"/>
+                  <a:t>Spectral Radius</a:t>
+                </a:r>
+              </a:p>
+            </c:rich>
+          </c:tx>
+          <c:layout/>
+          <c:overlay val="0"/>
+        </c:title>
+        <c:numFmt formatCode="General" sourceLinked="1"/>
+        <c:majorTickMark val="out"/>
+        <c:minorTickMark val="none"/>
+        <c:tickLblPos val="nextTo"/>
+        <c:txPr>
+          <a:bodyPr/>
+          <a:lstStyle/>
+          <a:p>
+            <a:pPr>
+              <a:defRPr sz="1600"/>
+            </a:pPr>
+            <a:endParaRPr lang="en-US"/>
+          </a:p>
+        </c:txPr>
+        <c:crossAx val="2132256520"/>
+        <c:crossesAt val="1.0E-5"/>
+        <c:crossBetween val="midCat"/>
+        <c:majorUnit val="0.1"/>
+      </c:valAx>
+    </c:plotArea>
+    <c:legend>
+      <c:legendPos val="r"/>
+      <c:layout/>
+      <c:overlay val="0"/>
+      <c:txPr>
+        <a:bodyPr/>
+        <a:lstStyle/>
+        <a:p>
+          <a:pPr>
+            <a:defRPr sz="1600"/>
+          </a:pPr>
+          <a:endParaRPr lang="en-US"/>
+        </a:p>
+      </c:txPr>
+    </c:legend>
+    <c:plotVisOnly val="1"/>
+    <c:dispBlanksAs val="gap"/>
+    <c:showDLblsOverMax val="0"/>
+  </c:chart>
+  <c:printSettings>
+    <c:headerFooter/>
+    <c:pageMargins b="1.0" l="0.75" r="0.75" t="1.0" header="0.5" footer="0.5"/>
+    <c:pageSetup/>
+  </c:printSettings>
+</c:chartSpace>
+</file>
+
+<file path=xl/charts/chart2.xml><?xml version="1.0" encoding="utf-8"?>
+<c:chartSpace xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+  <c:date1904 val="0"/>
+  <c:lang val="en-US"/>
+  <c:roundedCorners val="0"/>
+  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+    <mc:Choice xmlns:c14="http://schemas.microsoft.com/office/drawing/2007/8/2/chart" Requires="c14">
+      <c14:style val="118"/>
+    </mc:Choice>
+    <mc:Fallback>
+      <c:style val="18"/>
+    </mc:Fallback>
+  </mc:AlternateContent>
+  <c:chart>
+    <c:title>
+      <c:layout/>
+      <c:overlay val="0"/>
+    </c:title>
+    <c:autoTitleDeleted val="0"/>
+    <c:plotArea>
+      <c:layout/>
+      <c:scatterChart>
+        <c:scatterStyle val="lineMarker"/>
+        <c:varyColors val="0"/>
+        <c:ser>
+          <c:idx val="0"/>
+          <c:order val="0"/>
+          <c:tx>
+            <c:strRef>
+              <c:f>'Sufficient Condition'!$E$31</c:f>
+              <c:strCache>
+                <c:ptCount val="1"/>
+                <c:pt idx="0">
+                  <c:v>MCSA Iters</c:v>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
+          </c:tx>
+          <c:xVal>
+            <c:numRef>
+              <c:f>'Sufficient Condition'!$A$32:$A$37</c:f>
+              <c:numCache>
+                <c:formatCode>0.0E+00</c:formatCode>
+                <c:ptCount val="6"/>
+                <c:pt idx="0">
+                  <c:v>1.0E-5</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>0.0001</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>0.001</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>0.01</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>0.1</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>0.5</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:xVal>
+          <c:yVal>
+            <c:numRef>
+              <c:f>'Sufficient Condition'!$E$32:$E$37</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="6"/>
+                <c:pt idx="0">
+                  <c:v>124.0</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>91.0</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>55.0</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>21.0</c:v>
+                </c:pt>
+                <c:pt idx="4" formatCode="0">
+                  <c:v>111.0</c:v>
+                </c:pt>
+                <c:pt idx="5" formatCode="0">
+                  <c:v>111.0</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:yVal>
+          <c:smooth val="0"/>
+        </c:ser>
+        <c:dLbls>
+          <c:showLegendKey val="0"/>
+          <c:showVal val="0"/>
+          <c:showCatName val="0"/>
+          <c:showSerName val="0"/>
+          <c:showPercent val="0"/>
+          <c:showBubbleSize val="0"/>
+        </c:dLbls>
+        <c:axId val="2132318312"/>
+        <c:axId val="2132321368"/>
+      </c:scatterChart>
+      <c:valAx>
+        <c:axId val="2132318312"/>
+        <c:scaling>
+          <c:logBase val="10.0"/>
+          <c:orientation val="minMax"/>
+        </c:scaling>
+        <c:delete val="0"/>
+        <c:axPos val="b"/>
+        <c:numFmt formatCode="0.0E+00" sourceLinked="1"/>
+        <c:majorTickMark val="out"/>
+        <c:minorTickMark val="none"/>
+        <c:tickLblPos val="nextTo"/>
+        <c:crossAx val="2132321368"/>
+        <c:crosses val="autoZero"/>
+        <c:crossBetween val="midCat"/>
+      </c:valAx>
+      <c:valAx>
+        <c:axId val="2132321368"/>
+        <c:scaling>
+          <c:orientation val="minMax"/>
+        </c:scaling>
+        <c:delete val="0"/>
+        <c:axPos val="l"/>
+        <c:majorGridlines/>
+        <c:numFmt formatCode="General" sourceLinked="1"/>
+        <c:majorTickMark val="out"/>
+        <c:minorTickMark val="none"/>
+        <c:tickLblPos val="nextTo"/>
+        <c:crossAx val="2132318312"/>
+        <c:crossesAt val="1.0E-5"/>
+        <c:crossBetween val="midCat"/>
+      </c:valAx>
+    </c:plotArea>
+    <c:legend>
+      <c:legendPos val="r"/>
+      <c:layout/>
+      <c:overlay val="0"/>
+    </c:legend>
+    <c:plotVisOnly val="1"/>
+    <c:dispBlanksAs val="gap"/>
+    <c:showDLblsOverMax val="0"/>
+  </c:chart>
+  <c:printSettings>
+    <c:headerFooter/>
+    <c:pageMargins b="1.0" l="0.75" r="0.75" t="1.0" header="0.5" footer="0.5"/>
+    <c:pageSetup/>
+  </c:printSettings>
+</c:chartSpace>
+</file>
+
+<file path=xl/drawings/drawing1.xml><?xml version="1.0" encoding="utf-8"?>
+<xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>5</xdr:col>
+      <xdr:colOff>203200</xdr:colOff>
+      <xdr:row>30</xdr:row>
+      <xdr:rowOff>0</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>16</xdr:col>
+      <xdr:colOff>228600</xdr:colOff>
+      <xdr:row>59</xdr:row>
+      <xdr:rowOff>146050</xdr:rowOff>
+    </xdr:to>
+    <xdr:graphicFrame macro="">
+      <xdr:nvGraphicFramePr>
+        <xdr:cNvPr id="2" name="Chart 1"/>
+        <xdr:cNvGraphicFramePr>
+          <a:graphicFrameLocks/>
+        </xdr:cNvGraphicFramePr>
+      </xdr:nvGraphicFramePr>
+      <xdr:xfrm>
+        <a:off x="0" y="0"/>
+        <a:ext cx="0" cy="0"/>
+      </xdr:xfrm>
+      <a:graphic>
+        <a:graphicData uri="http://schemas.openxmlformats.org/drawingml/2006/chart">
+          <c:chart xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="rId1"/>
+        </a:graphicData>
+      </a:graphic>
+    </xdr:graphicFrame>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>16</xdr:col>
+      <xdr:colOff>368300</xdr:colOff>
+      <xdr:row>29</xdr:row>
+      <xdr:rowOff>184150</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>24</xdr:col>
+      <xdr:colOff>812800</xdr:colOff>
+      <xdr:row>59</xdr:row>
+      <xdr:rowOff>152400</xdr:rowOff>
+    </xdr:to>
+    <xdr:graphicFrame macro="">
+      <xdr:nvGraphicFramePr>
+        <xdr:cNvPr id="3" name="Chart 2"/>
+        <xdr:cNvGraphicFramePr/>
+      </xdr:nvGraphicFramePr>
+      <xdr:xfrm>
+        <a:off x="0" y="0"/>
+        <a:ext cx="0" cy="0"/>
+      </xdr:xfrm>
+      <a:graphic>
+        <a:graphicData uri="http://schemas.openxmlformats.org/drawingml/2006/chart">
+          <c:chart xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="rId2"/>
+        </a:graphicData>
+      </a:graphic>
+    </xdr:graphicFrame>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+</xdr:wsDr>
 </file>
 
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
@@ -1537,10 +2414,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:R84"/>
+  <dimension ref="A1:S84"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="M25" sqref="M25"/>
+      <selection activeCell="Q61" sqref="Q61:S61"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0"/>
@@ -2859,15 +3736,15 @@
         <v>0</v>
       </c>
     </row>
-    <row r="49" spans="1:18">
+    <row r="49" spans="1:19">
       <c r="D49" s="14"/>
       <c r="E49" s="9"/>
     </row>
-    <row r="50" spans="1:18">
+    <row r="50" spans="1:19">
       <c r="D50" s="14"/>
       <c r="E50" s="9"/>
     </row>
-    <row r="51" spans="1:18">
+    <row r="51" spans="1:19">
       <c r="A51" s="3" t="s">
         <v>75</v>
       </c>
@@ -2876,7 +3753,7 @@
       <c r="F51" s="18"/>
       <c r="G51" s="18"/>
     </row>
-    <row r="52" spans="1:18">
+    <row r="52" spans="1:19">
       <c r="A52" s="1" t="s">
         <v>11</v>
       </c>
@@ -2932,7 +3809,7 @@
         <v>80</v>
       </c>
     </row>
-    <row r="53" spans="1:18">
+    <row r="53" spans="1:19">
       <c r="A53" s="6">
         <v>2</v>
       </c>
@@ -2993,7 +3870,7 @@
         <v>9.0965999999999987</v>
       </c>
     </row>
-    <row r="54" spans="1:18">
+    <row r="54" spans="1:19">
       <c r="A54" s="6">
         <v>3</v>
       </c>
@@ -3054,7 +3931,7 @@
         <v>9.5971999999999991</v>
       </c>
     </row>
-    <row r="55" spans="1:18">
+    <row r="55" spans="1:19">
       <c r="A55" s="6">
         <v>4</v>
       </c>
@@ -3115,7 +3992,7 @@
         <v>12.779799999999998</v>
       </c>
     </row>
-    <row r="56" spans="1:18">
+    <row r="56" spans="1:19">
       <c r="A56" s="6">
         <v>5</v>
       </c>
@@ -3176,7 +4053,7 @@
         <v>16.804200000000009</v>
       </c>
     </row>
-    <row r="57" spans="1:18">
+    <row r="57" spans="1:19">
       <c r="A57" s="6">
         <v>6</v>
       </c>
@@ -3237,17 +4114,17 @@
         <v>25.305500000000006</v>
       </c>
     </row>
-    <row r="58" spans="1:18">
+    <row r="58" spans="1:19">
       <c r="M58" s="9"/>
     </row>
-    <row r="59" spans="1:18">
+    <row r="59" spans="1:19">
       <c r="A59" s="3"/>
       <c r="D59" s="14"/>
       <c r="E59" s="9"/>
       <c r="F59" s="18"/>
       <c r="G59" s="18"/>
     </row>
-    <row r="60" spans="1:18">
+    <row r="60" spans="1:19">
       <c r="A60" s="3" t="s">
         <v>82</v>
       </c>
@@ -3257,7 +4134,7 @@
       <c r="Q60" s="1"/>
       <c r="R60" s="1"/>
     </row>
-    <row r="61" spans="1:18">
+    <row r="61" spans="1:19">
       <c r="A61" s="1" t="s">
         <v>11</v>
       </c>
@@ -3306,10 +4183,17 @@
       <c r="P61" s="20" t="s">
         <v>80</v>
       </c>
-      <c r="Q61" s="18"/>
-      <c r="R61" s="18"/>
-    </row>
-    <row r="62" spans="1:18">
+      <c r="Q61" s="1" t="s">
+        <v>100</v>
+      </c>
+      <c r="R61" s="1" t="s">
+        <v>102</v>
+      </c>
+      <c r="S61" s="1" t="s">
+        <v>101</v>
+      </c>
+    </row>
+    <row r="62" spans="1:19">
       <c r="A62" s="6">
         <v>2</v>
       </c>
@@ -3365,7 +4249,7 @@
       <c r="Q62" s="18"/>
       <c r="R62" s="18"/>
     </row>
-    <row r="63" spans="1:18">
+    <row r="63" spans="1:19">
       <c r="A63" s="6">
         <v>3</v>
       </c>
@@ -3421,7 +4305,7 @@
       <c r="Q63" s="18"/>
       <c r="R63" s="18"/>
     </row>
-    <row r="64" spans="1:18">
+    <row r="64" spans="1:19">
       <c r="A64" s="6">
         <v>4</v>
       </c>
@@ -3829,8 +4713,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:R76"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="M29" sqref="M29"/>
+    <sheetView topLeftCell="A18" workbookViewId="0">
+      <selection activeCell="M39" sqref="M39"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0"/>
@@ -3845,9 +4729,7 @@
     <col min="8" max="8" width="11" bestFit="1" customWidth="1"/>
     <col min="9" max="11" width="12.1640625" bestFit="1" customWidth="1"/>
     <col min="12" max="12" width="13.1640625" bestFit="1" customWidth="1"/>
-    <col min="13" max="13" width="19.5" bestFit="1" customWidth="1"/>
-    <col min="14" max="14" width="17.83203125" bestFit="1" customWidth="1"/>
-    <col min="15" max="15" width="19.5" bestFit="1" customWidth="1"/>
+    <col min="13" max="15" width="19.5" bestFit="1" customWidth="1"/>
     <col min="16" max="16" width="18" bestFit="1" customWidth="1"/>
     <col min="17" max="17" width="15.33203125" bestFit="1" customWidth="1"/>
     <col min="18" max="18" width="15.5" bestFit="1" customWidth="1"/>
@@ -4523,7 +5405,7 @@
       <c r="G32" s="18"/>
       <c r="H32" s="4"/>
     </row>
-    <row r="33" spans="1:16">
+    <row r="33" spans="1:18">
       <c r="A33" s="3" t="s">
         <v>20</v>
       </c>
@@ -4532,7 +5414,7 @@
       <c r="G33" s="18"/>
       <c r="H33" s="4"/>
     </row>
-    <row r="34" spans="1:16">
+    <row r="34" spans="1:18">
       <c r="A34" s="1" t="s">
         <v>11</v>
       </c>
@@ -4561,7 +5443,7 @@
         <v>67</v>
       </c>
     </row>
-    <row r="35" spans="1:16">
+    <row r="35" spans="1:18">
       <c r="A35" s="6">
         <v>2</v>
       </c>
@@ -4592,7 +5474,7 @@
         <v>14.153846153846153</v>
       </c>
     </row>
-    <row r="36" spans="1:16">
+    <row r="36" spans="1:18">
       <c r="A36" s="6">
         <v>3</v>
       </c>
@@ -4623,7 +5505,7 @@
         <v>15.153846153846153</v>
       </c>
     </row>
-    <row r="37" spans="1:16">
+    <row r="37" spans="1:18">
       <c r="A37" s="6">
         <v>4</v>
       </c>
@@ -4654,7 +5536,7 @@
         <v>17.153846153846153</v>
       </c>
     </row>
-    <row r="38" spans="1:16">
+    <row r="38" spans="1:18">
       <c r="A38" s="6">
         <v>5</v>
       </c>
@@ -4685,7 +5567,7 @@
         <v>19.153846153846153</v>
       </c>
     </row>
-    <row r="39" spans="1:16">
+    <row r="39" spans="1:18">
       <c r="A39" s="6">
         <v>6</v>
       </c>
@@ -4716,24 +5598,24 @@
         <v>27.923076923076923</v>
       </c>
     </row>
-    <row r="40" spans="1:16">
+    <row r="40" spans="1:18">
       <c r="D40" s="14"/>
       <c r="F40" s="18"/>
       <c r="G40" s="18"/>
       <c r="I40" s="16"/>
     </row>
-    <row r="41" spans="1:16">
+    <row r="41" spans="1:18">
       <c r="D41" s="14"/>
       <c r="F41" s="18"/>
       <c r="G41" s="18"/>
     </row>
-    <row r="42" spans="1:16">
+    <row r="42" spans="1:18">
       <c r="A42" s="3"/>
       <c r="D42" s="14"/>
       <c r="F42" s="18"/>
       <c r="G42" s="18"/>
     </row>
-    <row r="43" spans="1:16">
+    <row r="43" spans="1:18">
       <c r="A43" s="3" t="s">
         <v>82</v>
       </c>
@@ -4741,7 +5623,7 @@
       <c r="F43" s="18"/>
       <c r="G43" s="18"/>
     </row>
-    <row r="44" spans="1:16">
+    <row r="44" spans="1:18">
       <c r="A44" s="1" t="s">
         <v>11</v>
       </c>
@@ -4787,9 +5669,17 @@
       <c r="O44" s="20" t="s">
         <v>66</v>
       </c>
-      <c r="P44" s="20"/>
-    </row>
-    <row r="45" spans="1:16">
+      <c r="P44" s="1" t="s">
+        <v>100</v>
+      </c>
+      <c r="Q44" s="1" t="s">
+        <v>102</v>
+      </c>
+      <c r="R44" s="1" t="s">
+        <v>101</v>
+      </c>
+    </row>
+    <row r="45" spans="1:18">
       <c r="A45" s="6">
         <v>2</v>
       </c>
@@ -4840,7 +5730,7 @@
       </c>
       <c r="P45" s="18"/>
     </row>
-    <row r="46" spans="1:16">
+    <row r="46" spans="1:18">
       <c r="A46" s="6">
         <v>3</v>
       </c>
@@ -4891,7 +5781,7 @@
       </c>
       <c r="P46" s="18"/>
     </row>
-    <row r="47" spans="1:16">
+    <row r="47" spans="1:18">
       <c r="A47" s="6">
         <v>4</v>
       </c>
@@ -4942,7 +5832,7 @@
       </c>
       <c r="P47" s="18"/>
     </row>
-    <row r="48" spans="1:16">
+    <row r="48" spans="1:18">
       <c r="A48" s="6">
         <v>5</v>
       </c>
@@ -5853,10 +6743,10 @@
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:AI55"/>
+  <dimension ref="A1:AL55"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="AE4" sqref="AE4:AI4"/>
+    <sheetView topLeftCell="A4" workbookViewId="0">
+      <selection activeCell="A49" sqref="A49:F49"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="13.33203125" defaultRowHeight="15" x14ac:dyDescent="0"/>
@@ -5872,12 +6762,12 @@
     <col min="33" max="33" width="10" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:35">
+    <row r="1" spans="1:38">
       <c r="A1" s="1" t="s">
         <v>28</v>
       </c>
     </row>
-    <row r="3" spans="1:35">
+    <row r="3" spans="1:38">
       <c r="A3" s="3" t="s">
         <v>25</v>
       </c>
@@ -5885,7 +6775,7 @@
         <v>31</v>
       </c>
     </row>
-    <row r="4" spans="1:35">
+    <row r="4" spans="1:38">
       <c r="A4" s="1" t="s">
         <v>26</v>
       </c>
@@ -5991,8 +6881,17 @@
       <c r="AI4" s="1" t="s">
         <v>62</v>
       </c>
-    </row>
-    <row r="5" spans="1:35">
+      <c r="AJ4" s="1" t="s">
+        <v>100</v>
+      </c>
+      <c r="AK4" s="1" t="s">
+        <v>102</v>
+      </c>
+      <c r="AL4" s="1" t="s">
+        <v>101</v>
+      </c>
+    </row>
+    <row r="5" spans="1:38">
       <c r="A5" s="7">
         <v>5</v>
       </c>
@@ -6102,7 +7001,7 @@
         <v>1650</v>
       </c>
     </row>
-    <row r="6" spans="1:35">
+    <row r="6" spans="1:38">
       <c r="A6" s="7">
         <v>5</v>
       </c>
@@ -6212,7 +7111,7 @@
         <v>1746</v>
       </c>
     </row>
-    <row r="7" spans="1:35">
+    <row r="7" spans="1:38">
       <c r="A7" s="7">
         <v>5</v>
       </c>
@@ -6322,7 +7221,7 @@
         <v>2178</v>
       </c>
     </row>
-    <row r="8" spans="1:35">
+    <row r="8" spans="1:38">
       <c r="A8" s="7">
         <v>5</v>
       </c>
@@ -6432,7 +7331,7 @@
         <v>6588</v>
       </c>
     </row>
-    <row r="9" spans="1:35">
+    <row r="9" spans="1:38">
       <c r="A9" s="7">
         <v>5</v>
       </c>
@@ -6543,7 +7442,7 @@
         <v>972</v>
       </c>
     </row>
-    <row r="10" spans="1:35">
+    <row r="10" spans="1:38">
       <c r="A10" s="7">
         <v>5</v>
       </c>
@@ -6653,7 +7552,7 @@
         <v>1014</v>
       </c>
     </row>
-    <row r="11" spans="1:35">
+    <row r="11" spans="1:38">
       <c r="A11" s="7">
         <v>5</v>
       </c>
@@ -6763,7 +7662,7 @@
         <v>16500</v>
       </c>
     </row>
-    <row r="13" spans="1:35">
+    <row r="13" spans="1:38">
       <c r="A13" s="7">
         <v>4</v>
       </c>
@@ -6873,7 +7772,7 @@
         <v>1715</v>
       </c>
     </row>
-    <row r="14" spans="1:35">
+    <row r="14" spans="1:38">
       <c r="A14" s="7">
         <v>4</v>
       </c>
@@ -6983,7 +7882,7 @@
         <v>1810</v>
       </c>
     </row>
-    <row r="15" spans="1:35">
+    <row r="15" spans="1:38">
       <c r="A15" s="7">
         <v>4</v>
       </c>
@@ -7093,7 +7992,7 @@
         <v>2575</v>
       </c>
     </row>
-    <row r="16" spans="1:35">
+    <row r="16" spans="1:38">
       <c r="A16" s="7">
         <v>4</v>
       </c>
@@ -8818,10 +9717,10 @@
 
 <file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:R35"/>
+  <dimension ref="A1:S43"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="P61" sqref="P61"/>
+    <sheetView topLeftCell="A2" workbookViewId="0">
+      <selection activeCell="Q2" sqref="Q2:R8"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0"/>
@@ -8843,18 +9742,15 @@
     <col min="16" max="16" width="15.5" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:18">
+    <row r="1" spans="1:19">
       <c r="A1" s="23" t="s">
         <v>82</v>
       </c>
       <c r="D1" s="14"/>
       <c r="F1" s="18"/>
       <c r="G1" s="18"/>
-      <c r="R1" s="29" t="s">
-        <v>90</v>
-      </c>
-    </row>
-    <row r="2" spans="1:18">
+    </row>
+    <row r="2" spans="1:19">
       <c r="A2" s="24" t="s">
         <v>29</v>
       </c>
@@ -8903,11 +9799,9 @@
       <c r="P2" s="20" t="s">
         <v>80</v>
       </c>
-      <c r="R2" t="s">
-        <v>83</v>
-      </c>
-    </row>
-    <row r="3" spans="1:18">
+      <c r="S2" s="20"/>
+    </row>
+    <row r="3" spans="1:19">
       <c r="A3" s="30">
         <v>0</v>
       </c>
@@ -8958,11 +9852,8 @@
         <f>F3-G3-H3-I3</f>
         <v>1.2090000000000103</v>
       </c>
-      <c r="R3" t="s">
-        <v>84</v>
-      </c>
-    </row>
-    <row r="4" spans="1:18">
+    </row>
+    <row r="4" spans="1:19">
       <c r="A4" s="30">
         <v>1E-4</v>
       </c>
@@ -9012,11 +9903,8 @@
         <f t="shared" ref="P4:P8" si="2">F4-G4-H4-I4</f>
         <v>4.1197000000000017</v>
       </c>
-      <c r="R4" t="s">
-        <v>85</v>
-      </c>
-    </row>
-    <row r="5" spans="1:18">
+    </row>
+    <row r="5" spans="1:19">
       <c r="A5" s="30">
         <v>1E-3</v>
       </c>
@@ -9067,11 +9955,8 @@
         <f t="shared" si="2"/>
         <v>3.1602000000000032</v>
       </c>
-      <c r="R5" t="s">
-        <v>86</v>
-      </c>
-    </row>
-    <row r="6" spans="1:18">
+    </row>
+    <row r="6" spans="1:19">
       <c r="A6" s="30">
         <v>0.01</v>
       </c>
@@ -9122,11 +10007,8 @@
         <f t="shared" si="2"/>
         <v>3.3287999999999958</v>
       </c>
-      <c r="R6" t="s">
-        <v>87</v>
-      </c>
-    </row>
-    <row r="7" spans="1:18">
+    </row>
+    <row r="7" spans="1:19">
       <c r="A7" s="30">
         <v>0.1</v>
       </c>
@@ -9177,11 +10059,8 @@
         <f t="shared" si="2"/>
         <v>14.121300000000009</v>
       </c>
-      <c r="R7" t="s">
-        <v>88</v>
-      </c>
-    </row>
-    <row r="8" spans="1:18">
+    </row>
+    <row r="8" spans="1:19">
       <c r="A8" s="30">
         <v>0.5</v>
       </c>
@@ -9232,11 +10111,8 @@
         <f t="shared" si="2"/>
         <v>13.846900000000016</v>
       </c>
-      <c r="R8" t="s">
-        <v>89</v>
-      </c>
-    </row>
-    <row r="11" spans="1:18">
+    </row>
+    <row r="11" spans="1:19">
       <c r="A11" s="24" t="s">
         <v>29</v>
       </c>
@@ -9285,8 +10161,11 @@
       <c r="P11" s="20" t="s">
         <v>80</v>
       </c>
-    </row>
-    <row r="12" spans="1:18">
+      <c r="Q11" s="20"/>
+      <c r="R11" s="20"/>
+      <c r="S11" s="20"/>
+    </row>
+    <row r="12" spans="1:19">
       <c r="A12" s="28">
         <v>0.01</v>
       </c>
@@ -9338,7 +10217,7 @@
         <v>4.2551000000000023</v>
       </c>
     </row>
-    <row r="13" spans="1:18">
+    <row r="13" spans="1:19">
       <c r="A13" s="28">
         <v>0.01</v>
       </c>
@@ -9390,7 +10269,7 @@
         <v>3.9298999999999982</v>
       </c>
     </row>
-    <row r="14" spans="1:18">
+    <row r="14" spans="1:19">
       <c r="A14" s="28">
         <v>0.01</v>
       </c>
@@ -9442,7 +10321,7 @@
         <v>2.8032000000000026</v>
       </c>
     </row>
-    <row r="15" spans="1:18">
+    <row r="15" spans="1:19">
       <c r="A15" s="28">
         <v>0.01</v>
       </c>
@@ -9494,7 +10373,7 @@
         <v>3.3287999999999958</v>
       </c>
     </row>
-    <row r="16" spans="1:18">
+    <row r="16" spans="1:19">
       <c r="A16" s="28">
         <v>0.01</v>
       </c>
@@ -9546,7 +10425,7 @@
         <v>3.2663000000000011</v>
       </c>
     </row>
-    <row r="17" spans="1:16">
+    <row r="17" spans="1:19">
       <c r="A17" s="28">
         <v>0.01</v>
       </c>
@@ -9599,10 +10478,10 @@
         <v>2.5661000000000023</v>
       </c>
     </row>
-    <row r="18" spans="1:16">
+    <row r="18" spans="1:19">
       <c r="A18" s="26"/>
     </row>
-    <row r="20" spans="1:16">
+    <row r="20" spans="1:19">
       <c r="A20" s="24" t="s">
         <v>29</v>
       </c>
@@ -9651,8 +10530,11 @@
       <c r="P20" s="20" t="s">
         <v>80</v>
       </c>
-    </row>
-    <row r="21" spans="1:16">
+      <c r="Q20" s="20"/>
+      <c r="R20" s="20"/>
+      <c r="S20" s="20"/>
+    </row>
+    <row r="21" spans="1:19">
       <c r="A21" s="28">
         <v>0.01</v>
       </c>
@@ -9704,7 +10586,7 @@
         <v>6.4233999999999991</v>
       </c>
     </row>
-    <row r="22" spans="1:16">
+    <row r="22" spans="1:19">
       <c r="A22" s="28">
         <v>0.01</v>
       </c>
@@ -9756,7 +10638,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="23" spans="1:16">
+    <row r="23" spans="1:19">
       <c r="A23" s="28">
         <v>0.01</v>
       </c>
@@ -9808,7 +10690,7 @@
         <v>4.3287000000000013</v>
       </c>
     </row>
-    <row r="24" spans="1:16">
+    <row r="24" spans="1:19">
       <c r="A24" s="28">
         <v>0.01</v>
       </c>
@@ -9860,7 +10742,7 @@
         <v>4.1564999999999985</v>
       </c>
     </row>
-    <row r="25" spans="1:16">
+    <row r="25" spans="1:19">
       <c r="A25" s="28">
         <v>0.01</v>
       </c>
@@ -9912,7 +10794,7 @@
         <v>4.101200000000004</v>
       </c>
     </row>
-    <row r="26" spans="1:16">
+    <row r="26" spans="1:19">
       <c r="A26" s="28"/>
       <c r="D26" s="14"/>
       <c r="E26" s="9"/>
@@ -9924,7 +10806,7 @@
       <c r="O26" s="18"/>
       <c r="P26" s="18"/>
     </row>
-    <row r="29" spans="1:16">
+    <row r="29" spans="1:19">
       <c r="A29" s="24" t="s">
         <v>29</v>
       </c>
@@ -9973,8 +10855,11 @@
       <c r="P29" s="20" t="s">
         <v>80</v>
       </c>
-    </row>
-    <row r="30" spans="1:16">
+      <c r="Q29" s="20"/>
+      <c r="R29" s="20"/>
+      <c r="S29" s="20"/>
+    </row>
+    <row r="30" spans="1:19">
       <c r="A30" s="28">
         <v>0.01</v>
       </c>
@@ -10026,7 +10911,7 @@
         <v>13.1332</v>
       </c>
     </row>
-    <row r="31" spans="1:16">
+    <row r="31" spans="1:19">
       <c r="A31" s="28">
         <v>0.01</v>
       </c>
@@ -10078,7 +10963,7 @@
         <v>7.1314999999999991</v>
       </c>
     </row>
-    <row r="32" spans="1:16">
+    <row r="32" spans="1:19">
       <c r="A32" s="28">
         <v>0.01</v>
       </c>
@@ -10187,6 +11072,46 @@
       <c r="M35" s="31"/>
       <c r="O35" s="18"/>
       <c r="P35" s="18"/>
+    </row>
+    <row r="36" spans="1:16">
+      <c r="A36" s="29" t="s">
+        <v>90</v>
+      </c>
+    </row>
+    <row r="37" spans="1:16">
+      <c r="A37" t="s">
+        <v>83</v>
+      </c>
+    </row>
+    <row r="38" spans="1:16">
+      <c r="A38" t="s">
+        <v>84</v>
+      </c>
+    </row>
+    <row r="39" spans="1:16">
+      <c r="A39" t="s">
+        <v>85</v>
+      </c>
+    </row>
+    <row r="40" spans="1:16">
+      <c r="A40" t="s">
+        <v>86</v>
+      </c>
+    </row>
+    <row r="41" spans="1:16">
+      <c r="A41" t="s">
+        <v>87</v>
+      </c>
+    </row>
+    <row r="42" spans="1:16">
+      <c r="A42" t="s">
+        <v>88</v>
+      </c>
+    </row>
+    <row r="43" spans="1:16">
+      <c r="A43" t="s">
+        <v>89</v>
+      </c>
     </row>
   </sheetData>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
@@ -10197,4 +11122,834 @@
     </ext>
   </extLst>
 </worksheet>
+</file>
+
+<file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A1:L84"/>
+  <sheetViews>
+    <sheetView tabSelected="1" topLeftCell="A22" workbookViewId="0">
+      <selection activeCell="Q70" sqref="Q70"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0"/>
+  <cols>
+    <col min="2" max="2" width="13.5" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="12" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="11.6640625" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="13.5" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="10.83203125" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="9" bestFit="1" customWidth="1"/>
+    <col min="9" max="9" width="10.33203125" bestFit="1" customWidth="1"/>
+    <col min="10" max="10" width="7.33203125" bestFit="1" customWidth="1"/>
+    <col min="11" max="11" width="8" bestFit="1" customWidth="1"/>
+    <col min="12" max="12" width="13.1640625" bestFit="1" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:12">
+      <c r="A1" s="2" t="s">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="3" spans="1:12">
+      <c r="A3" s="3" t="s">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="5" spans="1:12">
+      <c r="A5" s="3" t="s">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="6" spans="1:12">
+      <c r="A6" s="1" t="s">
+        <v>11</v>
+      </c>
+      <c r="B6" s="1" t="s">
+        <v>2</v>
+      </c>
+      <c r="C6" s="1" t="s">
+        <v>3</v>
+      </c>
+      <c r="D6" s="1" t="s">
+        <v>4</v>
+      </c>
+      <c r="E6" s="1" t="s">
+        <v>5</v>
+      </c>
+      <c r="F6" s="1" t="s">
+        <v>8</v>
+      </c>
+      <c r="G6" s="1" t="s">
+        <v>7</v>
+      </c>
+      <c r="H6" s="1" t="s">
+        <v>9</v>
+      </c>
+      <c r="I6" s="1" t="s">
+        <v>6</v>
+      </c>
+      <c r="J6" s="1" t="s">
+        <v>10</v>
+      </c>
+      <c r="K6" s="1" t="s">
+        <v>22</v>
+      </c>
+      <c r="L6" s="1" t="s">
+        <v>23</v>
+      </c>
+    </row>
+    <row r="7" spans="1:12">
+      <c r="A7" s="5">
+        <v>2</v>
+      </c>
+      <c r="B7">
+        <f>17*17</f>
+        <v>289</v>
+      </c>
+      <c r="C7">
+        <v>9</v>
+      </c>
+      <c r="D7">
+        <v>2</v>
+      </c>
+      <c r="E7">
+        <v>23</v>
+      </c>
+      <c r="F7">
+        <v>1</v>
+      </c>
+      <c r="G7">
+        <v>1</v>
+      </c>
+      <c r="H7">
+        <v>5</v>
+      </c>
+      <c r="I7" s="4">
+        <f t="shared" ref="I7:I11" si="0">B7*C7*D7*D7*E7*(H7+2)*(F7+1)/2</f>
+        <v>1675044</v>
+      </c>
+      <c r="J7">
+        <f t="shared" ref="J7:J11" si="1">K7*16</f>
+        <v>128</v>
+      </c>
+      <c r="K7">
+        <v>8</v>
+      </c>
+      <c r="L7" s="4">
+        <f t="shared" ref="L7:L11" si="2">I7/J7</f>
+        <v>13086.28125</v>
+      </c>
+    </row>
+    <row r="8" spans="1:12">
+      <c r="A8" s="5">
+        <v>3</v>
+      </c>
+      <c r="B8">
+        <f t="shared" ref="B8:B11" si="3">17*17</f>
+        <v>289</v>
+      </c>
+      <c r="C8">
+        <v>9</v>
+      </c>
+      <c r="D8">
+        <v>2</v>
+      </c>
+      <c r="E8">
+        <v>23</v>
+      </c>
+      <c r="F8">
+        <v>1</v>
+      </c>
+      <c r="G8">
+        <v>1</v>
+      </c>
+      <c r="H8">
+        <v>10</v>
+      </c>
+      <c r="I8" s="4">
+        <f t="shared" si="0"/>
+        <v>2871504</v>
+      </c>
+      <c r="J8">
+        <f t="shared" si="1"/>
+        <v>256</v>
+      </c>
+      <c r="K8">
+        <v>16</v>
+      </c>
+      <c r="L8" s="4">
+        <f t="shared" si="2"/>
+        <v>11216.8125</v>
+      </c>
+    </row>
+    <row r="9" spans="1:12">
+      <c r="A9" s="5">
+        <v>4</v>
+      </c>
+      <c r="B9">
+        <f t="shared" si="3"/>
+        <v>289</v>
+      </c>
+      <c r="C9">
+        <v>9</v>
+      </c>
+      <c r="D9">
+        <v>2</v>
+      </c>
+      <c r="E9">
+        <v>23</v>
+      </c>
+      <c r="F9">
+        <v>1</v>
+      </c>
+      <c r="G9">
+        <v>1</v>
+      </c>
+      <c r="H9">
+        <v>25</v>
+      </c>
+      <c r="I9" s="4">
+        <f t="shared" si="0"/>
+        <v>6460884</v>
+      </c>
+      <c r="J9">
+        <f t="shared" si="1"/>
+        <v>512</v>
+      </c>
+      <c r="K9">
+        <v>32</v>
+      </c>
+      <c r="L9" s="4">
+        <f t="shared" si="2"/>
+        <v>12618.9140625</v>
+      </c>
+    </row>
+    <row r="10" spans="1:12">
+      <c r="A10" s="5">
+        <v>5</v>
+      </c>
+      <c r="B10">
+        <f t="shared" si="3"/>
+        <v>289</v>
+      </c>
+      <c r="C10">
+        <v>9</v>
+      </c>
+      <c r="D10">
+        <v>2</v>
+      </c>
+      <c r="E10">
+        <v>23</v>
+      </c>
+      <c r="F10">
+        <v>1</v>
+      </c>
+      <c r="G10">
+        <v>1</v>
+      </c>
+      <c r="H10">
+        <v>50</v>
+      </c>
+      <c r="I10" s="4">
+        <f t="shared" si="0"/>
+        <v>12443184</v>
+      </c>
+      <c r="J10">
+        <f t="shared" si="1"/>
+        <v>992</v>
+      </c>
+      <c r="K10">
+        <v>62</v>
+      </c>
+      <c r="L10" s="4">
+        <f t="shared" si="2"/>
+        <v>12543.532258064517</v>
+      </c>
+    </row>
+    <row r="11" spans="1:12">
+      <c r="A11" s="5">
+        <v>6</v>
+      </c>
+      <c r="B11">
+        <f t="shared" si="3"/>
+        <v>289</v>
+      </c>
+      <c r="C11">
+        <v>9</v>
+      </c>
+      <c r="D11">
+        <v>2</v>
+      </c>
+      <c r="E11">
+        <v>23</v>
+      </c>
+      <c r="F11">
+        <v>1</v>
+      </c>
+      <c r="G11">
+        <v>1</v>
+      </c>
+      <c r="H11">
+        <v>100</v>
+      </c>
+      <c r="I11" s="4">
+        <f t="shared" si="0"/>
+        <v>24407784</v>
+      </c>
+      <c r="J11">
+        <f t="shared" si="1"/>
+        <v>1952</v>
+      </c>
+      <c r="K11">
+        <v>122</v>
+      </c>
+      <c r="L11" s="4">
+        <f t="shared" si="2"/>
+        <v>12503.987704918032</v>
+      </c>
+    </row>
+    <row r="13" spans="1:12">
+      <c r="A13" s="1"/>
+    </row>
+    <row r="14" spans="1:12">
+      <c r="A14" s="1"/>
+      <c r="B14" s="1"/>
+      <c r="C14" s="1"/>
+    </row>
+    <row r="15" spans="1:12">
+      <c r="A15" s="5"/>
+    </row>
+    <row r="16" spans="1:12">
+      <c r="A16" s="5"/>
+    </row>
+    <row r="17" spans="1:5">
+      <c r="A17" s="5"/>
+    </row>
+    <row r="18" spans="1:5">
+      <c r="A18" s="5"/>
+    </row>
+    <row r="19" spans="1:5">
+      <c r="A19" s="5"/>
+    </row>
+    <row r="21" spans="1:5">
+      <c r="A21" s="1"/>
+    </row>
+    <row r="22" spans="1:5">
+      <c r="A22" s="1" t="s">
+        <v>99</v>
+      </c>
+      <c r="B22" s="1" t="s">
+        <v>100</v>
+      </c>
+      <c r="C22" s="1" t="s">
+        <v>101</v>
+      </c>
+    </row>
+    <row r="23" spans="1:5">
+      <c r="A23" s="5">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="24" spans="1:5">
+      <c r="A24" s="5">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="25" spans="1:5">
+      <c r="A25" s="5">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="26" spans="1:5">
+      <c r="A26" s="5">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="27" spans="1:5">
+      <c r="A27" s="5">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="30" spans="1:5">
+      <c r="A30" t="s">
+        <v>103</v>
+      </c>
+    </row>
+    <row r="31" spans="1:5">
+      <c r="A31" s="36" t="s">
+        <v>29</v>
+      </c>
+      <c r="B31" s="20" t="s">
+        <v>100</v>
+      </c>
+      <c r="C31" s="1" t="s">
+        <v>102</v>
+      </c>
+      <c r="D31" s="20" t="s">
+        <v>101</v>
+      </c>
+      <c r="E31" s="1" t="s">
+        <v>104</v>
+      </c>
+    </row>
+    <row r="32" spans="1:5">
+      <c r="A32" s="30">
+        <v>1.0000000000000001E-5</v>
+      </c>
+      <c r="B32">
+        <v>0.92687299999999995</v>
+      </c>
+      <c r="C32">
+        <v>0.92687299999999995</v>
+      </c>
+      <c r="D32">
+        <v>1.17702</v>
+      </c>
+      <c r="E32">
+        <v>124</v>
+      </c>
+    </row>
+    <row r="33" spans="1:5">
+      <c r="A33" s="30">
+        <v>1E-4</v>
+      </c>
+      <c r="B33">
+        <v>0.92558700000000005</v>
+      </c>
+      <c r="C33">
+        <v>0.92558669999999998</v>
+      </c>
+      <c r="D33">
+        <v>1.173943</v>
+      </c>
+      <c r="E33">
+        <v>91</v>
+      </c>
+    </row>
+    <row r="34" spans="1:5">
+      <c r="A34" s="30">
+        <v>1E-3</v>
+      </c>
+      <c r="B34">
+        <v>0.92353660000000004</v>
+      </c>
+      <c r="C34">
+        <v>0.92353660000000004</v>
+      </c>
+      <c r="D34">
+        <v>1.156509</v>
+      </c>
+      <c r="E34">
+        <v>55</v>
+      </c>
+    </row>
+    <row r="35" spans="1:5">
+      <c r="A35" s="30">
+        <v>0.01</v>
+      </c>
+      <c r="B35">
+        <v>0.9071089</v>
+      </c>
+      <c r="C35">
+        <v>0.9071089</v>
+      </c>
+      <c r="D35">
+        <v>0.86222719999999997</v>
+      </c>
+      <c r="E35">
+        <v>21</v>
+      </c>
+    </row>
+    <row r="36" spans="1:5">
+      <c r="A36" s="30">
+        <v>0.1</v>
+      </c>
+      <c r="B36" s="35">
+        <v>5.8999999999999997E-2</v>
+      </c>
+      <c r="C36" s="35">
+        <v>5.8999999999999997E-2</v>
+      </c>
+      <c r="D36" s="35">
+        <v>3.6900000000000001E-3</v>
+      </c>
+      <c r="E36" s="37">
+        <v>111</v>
+      </c>
+    </row>
+    <row r="37" spans="1:5">
+      <c r="A37" s="30">
+        <v>0.5</v>
+      </c>
+      <c r="B37" s="35">
+        <v>5.8999999999999997E-2</v>
+      </c>
+      <c r="C37" s="35">
+        <v>5.8999999999999997E-2</v>
+      </c>
+      <c r="D37" s="35">
+        <v>3.48E-3</v>
+      </c>
+      <c r="E37" s="37">
+        <v>111</v>
+      </c>
+    </row>
+    <row r="63" spans="1:6">
+      <c r="A63" t="s">
+        <v>106</v>
+      </c>
+      <c r="B63" t="s">
+        <v>107</v>
+      </c>
+      <c r="D63" t="s">
+        <v>108</v>
+      </c>
+    </row>
+    <row r="64" spans="1:6">
+      <c r="A64" s="1" t="s">
+        <v>29</v>
+      </c>
+      <c r="B64" s="1" t="s">
+        <v>30</v>
+      </c>
+      <c r="C64" s="1" t="s">
+        <v>105</v>
+      </c>
+      <c r="D64" s="1" t="s">
+        <v>100</v>
+      </c>
+      <c r="E64" s="1" t="s">
+        <v>102</v>
+      </c>
+      <c r="F64" s="1" t="s">
+        <v>101</v>
+      </c>
+    </row>
+    <row r="65" spans="1:6">
+      <c r="A65">
+        <v>0</v>
+      </c>
+      <c r="B65">
+        <v>0</v>
+      </c>
+      <c r="C65">
+        <v>0</v>
+      </c>
+      <c r="D65" s="38">
+        <v>0.97585409999999995</v>
+      </c>
+      <c r="E65" s="38">
+        <v>1.0095769999999999</v>
+      </c>
+      <c r="F65" s="38">
+        <v>1.1986460000000001</v>
+      </c>
+    </row>
+    <row r="66" spans="1:6">
+      <c r="A66" s="35">
+        <v>1E-4</v>
+      </c>
+      <c r="B66">
+        <v>0</v>
+      </c>
+      <c r="C66">
+        <v>0</v>
+      </c>
+      <c r="D66" s="38">
+        <v>0.975854</v>
+      </c>
+      <c r="E66" s="38">
+        <v>0.97585409999999995</v>
+      </c>
+      <c r="F66" s="38">
+        <v>1.193789</v>
+      </c>
+    </row>
+    <row r="67" spans="1:6">
+      <c r="A67" s="35">
+        <v>1E-3</v>
+      </c>
+      <c r="B67">
+        <v>0</v>
+      </c>
+      <c r="C67">
+        <v>0</v>
+      </c>
+      <c r="D67" s="38">
+        <v>0.97585909999999998</v>
+      </c>
+      <c r="E67" s="38">
+        <v>0.97585909999999998</v>
+      </c>
+      <c r="F67" s="38">
+        <v>1.1964520000000001</v>
+      </c>
+    </row>
+    <row r="68" spans="1:6">
+      <c r="A68" s="35">
+        <v>0.01</v>
+      </c>
+      <c r="B68">
+        <v>0</v>
+      </c>
+      <c r="C68">
+        <v>0</v>
+      </c>
+      <c r="D68" s="38">
+        <v>0.97585730000000004</v>
+      </c>
+      <c r="E68" s="38">
+        <v>0.97585730000000004</v>
+      </c>
+      <c r="F68" s="38">
+        <v>1.2212810000000001</v>
+      </c>
+    </row>
+    <row r="69" spans="1:6">
+      <c r="A69" s="35">
+        <v>0.1</v>
+      </c>
+      <c r="B69">
+        <v>0</v>
+      </c>
+      <c r="C69">
+        <v>0</v>
+      </c>
+      <c r="D69" s="38">
+        <v>0.97585730000000004</v>
+      </c>
+      <c r="E69" s="38">
+        <v>0.97585730000000004</v>
+      </c>
+      <c r="F69" s="38">
+        <v>1.398595</v>
+      </c>
+    </row>
+    <row r="70" spans="1:6">
+      <c r="A70" s="35">
+        <v>0</v>
+      </c>
+      <c r="B70">
+        <v>0</v>
+      </c>
+      <c r="C70" s="35">
+        <v>1E-4</v>
+      </c>
+      <c r="D70" s="38">
+        <v>0.97585409999999995</v>
+      </c>
+      <c r="E70" s="38">
+        <v>1.009514</v>
+      </c>
+      <c r="F70" s="38">
+        <v>1.1986220000000001</v>
+      </c>
+    </row>
+    <row r="71" spans="1:6">
+      <c r="A71">
+        <v>0</v>
+      </c>
+      <c r="B71">
+        <v>0</v>
+      </c>
+      <c r="C71" s="35">
+        <v>1E-3</v>
+      </c>
+      <c r="D71" s="38">
+        <v>0.97585909999999998</v>
+      </c>
+      <c r="E71" s="38">
+        <v>1.009584</v>
+      </c>
+      <c r="F71" s="38">
+        <v>1.19757</v>
+      </c>
+    </row>
+    <row r="72" spans="1:6">
+      <c r="C72" s="35"/>
+      <c r="D72" s="38"/>
+      <c r="E72" s="38"/>
+      <c r="F72" s="38"/>
+    </row>
+    <row r="73" spans="1:6">
+      <c r="C73" s="35"/>
+      <c r="D73" s="38"/>
+      <c r="E73" s="38"/>
+      <c r="F73" s="38"/>
+    </row>
+    <row r="74" spans="1:6">
+      <c r="D74" s="38"/>
+      <c r="E74" s="38"/>
+      <c r="F74" s="38"/>
+    </row>
+    <row r="75" spans="1:6">
+      <c r="A75" s="1" t="s">
+        <v>29</v>
+      </c>
+      <c r="B75" s="1" t="s">
+        <v>30</v>
+      </c>
+      <c r="C75" s="1" t="s">
+        <v>105</v>
+      </c>
+      <c r="D75" s="1" t="s">
+        <v>100</v>
+      </c>
+      <c r="E75" s="1" t="s">
+        <v>102</v>
+      </c>
+      <c r="F75" s="1" t="s">
+        <v>101</v>
+      </c>
+    </row>
+    <row r="76" spans="1:6">
+      <c r="A76">
+        <v>0</v>
+      </c>
+      <c r="B76">
+        <v>1</v>
+      </c>
+      <c r="C76">
+        <v>0</v>
+      </c>
+      <c r="D76" s="38">
+        <v>0.95464740000000003</v>
+      </c>
+      <c r="E76" s="38">
+        <v>0.95464720000000003</v>
+      </c>
+      <c r="F76" s="38">
+        <v>1.1746749999999999</v>
+      </c>
+    </row>
+    <row r="77" spans="1:6">
+      <c r="A77" s="35">
+        <v>1E-4</v>
+      </c>
+      <c r="B77">
+        <v>1</v>
+      </c>
+      <c r="C77">
+        <v>0</v>
+      </c>
+      <c r="D77" s="38">
+        <v>0.95464729999999998</v>
+      </c>
+      <c r="E77" s="38">
+        <v>0.95464760000000004</v>
+      </c>
+      <c r="F77" s="38">
+        <v>1.1746920000000001</v>
+      </c>
+    </row>
+    <row r="78" spans="1:6">
+      <c r="A78" s="35">
+        <v>1E-3</v>
+      </c>
+      <c r="B78">
+        <v>1</v>
+      </c>
+      <c r="C78">
+        <v>0</v>
+      </c>
+      <c r="D78" s="38"/>
+      <c r="E78" s="38"/>
+      <c r="F78" s="38"/>
+    </row>
+    <row r="79" spans="1:6">
+      <c r="A79" s="35">
+        <v>0.01</v>
+      </c>
+      <c r="B79">
+        <v>1</v>
+      </c>
+      <c r="C79">
+        <v>0</v>
+      </c>
+      <c r="D79" s="38"/>
+      <c r="E79" s="38"/>
+      <c r="F79" s="38"/>
+    </row>
+    <row r="80" spans="1:6">
+      <c r="A80" s="35">
+        <v>0.1</v>
+      </c>
+      <c r="B80">
+        <v>1</v>
+      </c>
+      <c r="C80">
+        <v>0</v>
+      </c>
+      <c r="D80" s="38"/>
+      <c r="E80" s="38"/>
+      <c r="F80" s="38"/>
+    </row>
+    <row r="81" spans="1:6">
+      <c r="A81" s="35">
+        <v>0</v>
+      </c>
+      <c r="B81">
+        <v>1</v>
+      </c>
+      <c r="C81" s="35">
+        <v>1E-4</v>
+      </c>
+      <c r="D81" s="38"/>
+      <c r="E81" s="38"/>
+      <c r="F81" s="38"/>
+    </row>
+    <row r="82" spans="1:6">
+      <c r="A82">
+        <v>0</v>
+      </c>
+      <c r="B82">
+        <v>1</v>
+      </c>
+      <c r="C82" s="35">
+        <v>1E-3</v>
+      </c>
+      <c r="D82" s="38"/>
+      <c r="E82" s="38"/>
+      <c r="F82" s="38"/>
+    </row>
+    <row r="83" spans="1:6">
+      <c r="A83">
+        <v>0</v>
+      </c>
+      <c r="B83">
+        <v>1</v>
+      </c>
+      <c r="C83" s="35">
+        <v>0.01</v>
+      </c>
+      <c r="D83" s="38"/>
+      <c r="E83" s="38"/>
+      <c r="F83" s="38"/>
+    </row>
+    <row r="84" spans="1:6">
+      <c r="A84">
+        <v>0</v>
+      </c>
+      <c r="B84">
+        <v>1</v>
+      </c>
+      <c r="C84" s="35">
+        <v>0.1</v>
+      </c>
+      <c r="D84" s="38"/>
+      <c r="E84" s="38"/>
+      <c r="F84" s="38"/>
+    </row>
+  </sheetData>
+  <phoneticPr fontId="11" type="noConversion"/>
+  <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
+  <pageSetup orientation="portrait" horizontalDpi="4294967292" verticalDpi="4294967292"/>
+  <drawing r:id="rId1"/>
+  <extLst>
+    <ext xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" uri="{64002731-A6B0-56B0-2670-7721B7C09600}">
+      <mx:PLV Mode="0" OnePage="0" WScale="0"/>
+    </ext>
+  </extLst>
+</worksheet>
 </file>
</xml_diff>